<commit_message>
Updated Pending Backlog file
</commit_message>
<xml_diff>
--- a/_files/requirements/Pending_Backlog_Stories_25Jun19_Updated.xlsx
+++ b/_files/requirements/Pending_Backlog_Stories_25Jun19_Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP wiki Open Source\Requirements\_files\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C04E1E8D-A561-4B54-B0FD-7F612C26EFD7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{48265009-98F6-4E15-9729-062A8C45CB11}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId13"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -113,7 +113,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>MINDTREE:</t>
         </r>
@@ -122,7 +122,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 design current sprint, next sprit dev</t>
@@ -6626,17 +6626,17 @@
     <t>P2 - To be decided in the next sprint based on the location hierarchy decision from other modules</t>
   </si>
   <si>
-    <t>Discussion Needed</t>
-  </si>
-  <si>
     <t>Prioritisation on &lt;07 15&gt;</t>
+  </si>
+  <si>
+    <t>Discussion Needed on the use case</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6751,19 +6751,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -7790,6 +7777,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7814,6 +7819,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7825,15 +7839,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -7869,24 +7874,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -15037,7 +15024,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:D32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -15955,18 +15942,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="195" t="s">
         <v>1343</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="192"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="198"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -16416,7 +16403,7 @@
       <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="193" t="s">
+      <c r="B17" s="199" t="s">
         <v>503</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -16448,7 +16435,7 @@
       <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="195"/>
+      <c r="B18" s="201"/>
       <c r="C18" s="4" t="s">
         <v>1362</v>
       </c>
@@ -16788,19 +16775,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="195" t="s">
         <v>1367</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="190"/>
-      <c r="K1" s="192"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="196"/>
+      <c r="K1" s="198"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="153" t="s">
@@ -22115,18 +22102,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="195" t="s">
         <v>1732</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="192"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="198"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
@@ -22164,7 +22151,7 @@
       <c r="A3" s="39">
         <v>1</v>
       </c>
-      <c r="B3" s="212" t="s">
+      <c r="B3" s="218" t="s">
         <v>527</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -22190,7 +22177,7 @@
       <c r="A4" s="39">
         <v>2</v>
       </c>
-      <c r="B4" s="213"/>
+      <c r="B4" s="219"/>
       <c r="C4" s="4" t="s">
         <v>1736</v>
       </c>
@@ -22212,7 +22199,7 @@
       <c r="A5" s="39">
         <v>3</v>
       </c>
-      <c r="B5" s="212" t="s">
+      <c r="B5" s="218" t="s">
         <v>530</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -22238,7 +22225,7 @@
       <c r="A6" s="39">
         <v>4</v>
       </c>
-      <c r="B6" s="214"/>
+      <c r="B6" s="220"/>
       <c r="C6" s="19" t="s">
         <v>1741</v>
       </c>
@@ -22262,7 +22249,7 @@
       <c r="A7" s="39">
         <v>5</v>
       </c>
-      <c r="B7" s="214"/>
+      <c r="B7" s="220"/>
       <c r="C7" s="19" t="s">
         <v>1744</v>
       </c>
@@ -22284,7 +22271,7 @@
       <c r="A8" s="39">
         <v>6</v>
       </c>
-      <c r="B8" s="214"/>
+      <c r="B8" s="220"/>
       <c r="C8" s="19" t="s">
         <v>1746</v>
       </c>
@@ -22306,7 +22293,7 @@
       <c r="A9" s="39">
         <v>7</v>
       </c>
-      <c r="B9" s="214"/>
+      <c r="B9" s="220"/>
       <c r="C9" s="19" t="s">
         <v>1748</v>
       </c>
@@ -22328,7 +22315,7 @@
       <c r="A10" s="39">
         <v>8</v>
       </c>
-      <c r="B10" s="214"/>
+      <c r="B10" s="220"/>
       <c r="C10" s="19" t="s">
         <v>1750</v>
       </c>
@@ -22350,7 +22337,7 @@
       <c r="A11" s="39">
         <v>9</v>
       </c>
-      <c r="B11" s="214"/>
+      <c r="B11" s="220"/>
       <c r="C11" s="19" t="s">
         <v>1752</v>
       </c>
@@ -22372,7 +22359,7 @@
       <c r="A12" s="39">
         <v>10</v>
       </c>
-      <c r="B12" s="214"/>
+      <c r="B12" s="220"/>
       <c r="C12" s="19" t="s">
         <v>1754</v>
       </c>
@@ -22394,7 +22381,7 @@
       <c r="A13" s="39">
         <v>11</v>
       </c>
-      <c r="B13" s="214"/>
+      <c r="B13" s="220"/>
       <c r="C13" s="19" t="s">
         <v>1756</v>
       </c>
@@ -22416,7 +22403,7 @@
       <c r="A14" s="39">
         <v>12</v>
       </c>
-      <c r="B14" s="214"/>
+      <c r="B14" s="220"/>
       <c r="C14" s="19" t="s">
         <v>1758</v>
       </c>
@@ -22440,7 +22427,7 @@
       <c r="A15" s="39">
         <v>13</v>
       </c>
-      <c r="B15" s="214"/>
+      <c r="B15" s="220"/>
       <c r="C15" s="19" t="s">
         <v>1761</v>
       </c>
@@ -22464,7 +22451,7 @@
       <c r="A16" s="39">
         <v>14</v>
       </c>
-      <c r="B16" s="213"/>
+      <c r="B16" s="219"/>
       <c r="C16" s="19" t="s">
         <v>1763</v>
       </c>
@@ -22586,7 +22573,7 @@
       <c r="A21" s="39">
         <v>19</v>
       </c>
-      <c r="B21" s="212" t="s">
+      <c r="B21" s="218" t="s">
         <v>545</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -22610,7 +22597,7 @@
       <c r="A22" s="39">
         <v>20</v>
       </c>
-      <c r="B22" s="214"/>
+      <c r="B22" s="220"/>
       <c r="C22" s="4" t="s">
         <v>1771</v>
       </c>
@@ -22632,7 +22619,7 @@
       <c r="A23" s="39">
         <v>21</v>
       </c>
-      <c r="B23" s="214"/>
+      <c r="B23" s="220"/>
       <c r="C23" s="4" t="s">
         <v>1773</v>
       </c>
@@ -22654,7 +22641,7 @@
       <c r="A24" s="39">
         <v>22</v>
       </c>
-      <c r="B24" s="214"/>
+      <c r="B24" s="220"/>
       <c r="C24" s="4" t="s">
         <v>1775</v>
       </c>
@@ -22676,7 +22663,7 @@
       <c r="A25" s="39">
         <v>23</v>
       </c>
-      <c r="B25" s="214"/>
+      <c r="B25" s="220"/>
       <c r="C25" s="4" t="s">
         <v>1777</v>
       </c>
@@ -22698,7 +22685,7 @@
       <c r="A26" s="39">
         <v>24</v>
       </c>
-      <c r="B26" s="213"/>
+      <c r="B26" s="219"/>
       <c r="C26" s="4" t="s">
         <v>1779</v>
       </c>
@@ -22720,7 +22707,7 @@
       <c r="A27" s="39">
         <v>25</v>
       </c>
-      <c r="B27" s="212" t="s">
+      <c r="B27" s="218" t="s">
         <v>548</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -22744,7 +22731,7 @@
       <c r="A28" s="39">
         <v>26</v>
       </c>
-      <c r="B28" s="213"/>
+      <c r="B28" s="219"/>
       <c r="C28" s="4" t="s">
         <v>1783</v>
       </c>
@@ -22766,7 +22753,7 @@
       <c r="A29" s="39">
         <v>27</v>
       </c>
-      <c r="B29" s="212" t="s">
+      <c r="B29" s="218" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -22790,7 +22777,7 @@
       <c r="A30" s="39">
         <v>28</v>
       </c>
-      <c r="B30" s="213"/>
+      <c r="B30" s="219"/>
       <c r="C30" s="4" t="s">
         <v>1787</v>
       </c>
@@ -22812,7 +22799,7 @@
       <c r="A31" s="39">
         <v>29</v>
       </c>
-      <c r="B31" s="212" t="s">
+      <c r="B31" s="218" t="s">
         <v>553</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -22836,7 +22823,7 @@
       <c r="A32" s="39">
         <v>30</v>
       </c>
-      <c r="B32" s="214"/>
+      <c r="B32" s="220"/>
       <c r="C32" s="4" t="s">
         <v>1791</v>
       </c>
@@ -22858,7 +22845,7 @@
       <c r="A33" s="39">
         <v>31</v>
       </c>
-      <c r="B33" s="214"/>
+      <c r="B33" s="220"/>
       <c r="C33" s="4" t="s">
         <v>1793</v>
       </c>
@@ -22880,7 +22867,7 @@
       <c r="A34" s="39">
         <v>32</v>
       </c>
-      <c r="B34" s="214"/>
+      <c r="B34" s="220"/>
       <c r="C34" s="4" t="s">
         <v>1795</v>
       </c>
@@ -22902,7 +22889,7 @@
       <c r="A35" s="39">
         <v>33</v>
       </c>
-      <c r="B35" s="213"/>
+      <c r="B35" s="219"/>
       <c r="C35" s="4" t="s">
         <v>1797</v>
       </c>
@@ -22924,7 +22911,7 @@
       <c r="A36" s="39">
         <v>34</v>
       </c>
-      <c r="B36" s="212" t="s">
+      <c r="B36" s="218" t="s">
         <v>556</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -22948,7 +22935,7 @@
       <c r="A37" s="39">
         <v>35</v>
       </c>
-      <c r="B37" s="214"/>
+      <c r="B37" s="220"/>
       <c r="C37" s="4" t="s">
         <v>1801</v>
       </c>
@@ -22970,7 +22957,7 @@
       <c r="A38" s="39">
         <v>36</v>
       </c>
-      <c r="B38" s="214"/>
+      <c r="B38" s="220"/>
       <c r="C38" s="4" t="s">
         <v>1803</v>
       </c>
@@ -22992,7 +22979,7 @@
       <c r="A39" s="39">
         <v>37</v>
       </c>
-      <c r="B39" s="213"/>
+      <c r="B39" s="219"/>
       <c r="C39" s="4" t="s">
         <v>1805</v>
       </c>
@@ -23014,7 +23001,7 @@
       <c r="A40" s="39">
         <v>38</v>
       </c>
-      <c r="B40" s="212" t="s">
+      <c r="B40" s="218" t="s">
         <v>559</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -23038,7 +23025,7 @@
       <c r="A41" s="39">
         <v>39</v>
       </c>
-      <c r="B41" s="213"/>
+      <c r="B41" s="219"/>
       <c r="C41" s="4" t="s">
         <v>1809</v>
       </c>
@@ -23084,7 +23071,7 @@
       <c r="A43" s="39">
         <v>41</v>
       </c>
-      <c r="B43" s="212" t="s">
+      <c r="B43" s="218" t="s">
         <v>565</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -23108,7 +23095,7 @@
       <c r="A44" s="39">
         <v>42</v>
       </c>
-      <c r="B44" s="214"/>
+      <c r="B44" s="220"/>
       <c r="C44" s="4" t="s">
         <v>1814</v>
       </c>
@@ -23130,7 +23117,7 @@
       <c r="A45" s="39">
         <v>43</v>
       </c>
-      <c r="B45" s="214"/>
+      <c r="B45" s="220"/>
       <c r="C45" s="4" t="s">
         <v>1816</v>
       </c>
@@ -23152,7 +23139,7 @@
       <c r="A46" s="39">
         <v>44</v>
       </c>
-      <c r="B46" s="214"/>
+      <c r="B46" s="220"/>
       <c r="C46" s="4" t="s">
         <v>1818</v>
       </c>
@@ -23176,7 +23163,7 @@
       <c r="A47" s="39">
         <v>45</v>
       </c>
-      <c r="B47" s="214"/>
+      <c r="B47" s="220"/>
       <c r="C47" s="4" t="s">
         <v>1821</v>
       </c>
@@ -23198,7 +23185,7 @@
       <c r="A48" s="39">
         <v>46</v>
       </c>
-      <c r="B48" s="214"/>
+      <c r="B48" s="220"/>
       <c r="C48" s="4" t="s">
         <v>1823</v>
       </c>
@@ -23220,7 +23207,7 @@
       <c r="A49" s="39">
         <v>47</v>
       </c>
-      <c r="B49" s="214"/>
+      <c r="B49" s="220"/>
       <c r="C49" s="4" t="s">
         <v>1825</v>
       </c>
@@ -23242,7 +23229,7 @@
       <c r="A50" s="39">
         <v>48</v>
       </c>
-      <c r="B50" s="214"/>
+      <c r="B50" s="220"/>
       <c r="C50" s="4" t="s">
         <v>1827</v>
       </c>
@@ -23266,7 +23253,7 @@
       <c r="A51" s="39">
         <v>49</v>
       </c>
-      <c r="B51" s="214"/>
+      <c r="B51" s="220"/>
       <c r="C51" s="4" t="s">
         <v>1829</v>
       </c>
@@ -23288,7 +23275,7 @@
       <c r="A52" s="39">
         <v>50</v>
       </c>
-      <c r="B52" s="214"/>
+      <c r="B52" s="220"/>
       <c r="C52" s="4" t="s">
         <v>1831</v>
       </c>
@@ -23310,7 +23297,7 @@
       <c r="A53" s="39">
         <v>51</v>
       </c>
-      <c r="B53" s="214"/>
+      <c r="B53" s="220"/>
       <c r="C53" s="4" t="s">
         <v>1833</v>
       </c>
@@ -23332,7 +23319,7 @@
       <c r="A54" s="39">
         <v>52</v>
       </c>
-      <c r="B54" s="213"/>
+      <c r="B54" s="219"/>
       <c r="C54" s="4" t="s">
         <v>1835</v>
       </c>
@@ -23365,16 +23352,16 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="10">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="B36:B39"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="B43:B54"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B35"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B36:B39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -23415,26 +23402,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="189" t="s">
+      <c r="B2" s="195" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="190"/>
-      <c r="F2" s="190"/>
-      <c r="G2" s="190"/>
-      <c r="H2" s="190"/>
-      <c r="I2" s="191"/>
-      <c r="J2" s="190"/>
-      <c r="K2" s="190"/>
-      <c r="L2" s="190"/>
-      <c r="M2" s="190"/>
-      <c r="N2" s="190"/>
-      <c r="O2" s="190"/>
-      <c r="P2" s="190"/>
-      <c r="Q2" s="190"/>
-      <c r="R2" s="190"/>
-      <c r="S2" s="192"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="196"/>
+      <c r="G2" s="196"/>
+      <c r="H2" s="196"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="196"/>
+      <c r="K2" s="196"/>
+      <c r="L2" s="196"/>
+      <c r="M2" s="196"/>
+      <c r="N2" s="196"/>
+      <c r="O2" s="196"/>
+      <c r="P2" s="196"/>
+      <c r="Q2" s="196"/>
+      <c r="R2" s="196"/>
+      <c r="S2" s="198"/>
     </row>
     <row r="3" spans="2:19" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -25619,7 +25606,7 @@
       <c r="C68" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="D68" s="188" t="s">
+      <c r="D68" s="194" t="s">
         <v>222</v>
       </c>
       <c r="E68" s="124"/>
@@ -25653,7 +25640,7 @@
       <c r="C69" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="D69" s="188"/>
+      <c r="D69" s="194"/>
       <c r="E69" s="124"/>
       <c r="F69" s="47" t="s">
         <v>225</v>
@@ -35398,12 +35385,12 @@
       <c r="F1" s="41"/>
     </row>
     <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="189" t="s">
+      <c r="B2" s="195" t="s">
         <v>885</v>
       </c>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="192"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="198"/>
       <c r="F2" s="41"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -36968,18 +36955,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="195" t="s">
         <v>907</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="192"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="198"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -37020,7 +37007,7 @@
       <c r="A3" s="36">
         <v>1</v>
       </c>
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="199" t="s">
         <v>116</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -37055,7 +37042,7 @@
       <c r="A4" s="36">
         <v>2</v>
       </c>
-      <c r="B4" s="194"/>
+      <c r="B4" s="200"/>
       <c r="C4" s="22" t="s">
         <v>920</v>
       </c>
@@ -37088,7 +37075,7 @@
       <c r="A5" s="36">
         <v>3</v>
       </c>
-      <c r="B5" s="194"/>
+      <c r="B5" s="200"/>
       <c r="C5" s="4" t="s">
         <v>924</v>
       </c>
@@ -37121,7 +37108,7 @@
       <c r="A6" s="36">
         <v>4</v>
       </c>
-      <c r="B6" s="194"/>
+      <c r="B6" s="200"/>
       <c r="C6" s="4" t="s">
         <v>927</v>
       </c>
@@ -37154,7 +37141,7 @@
       <c r="A7" s="36">
         <v>5</v>
       </c>
-      <c r="B7" s="194"/>
+      <c r="B7" s="200"/>
       <c r="C7" s="4" t="s">
         <v>930</v>
       </c>
@@ -37185,7 +37172,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
-      <c r="B8" s="194"/>
+      <c r="B8" s="200"/>
       <c r="C8" s="4" t="s">
         <v>934</v>
       </c>
@@ -37210,7 +37197,7 @@
       <c r="A9" s="36">
         <v>6</v>
       </c>
-      <c r="B9" s="195"/>
+      <c r="B9" s="201"/>
       <c r="C9" s="4" t="s">
         <v>936</v>
       </c>
@@ -37464,7 +37451,7 @@
       <c r="A17" s="36">
         <v>14</v>
       </c>
-      <c r="B17" s="193" t="s">
+      <c r="B17" s="199" t="s">
         <v>143</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -37497,7 +37484,7 @@
       <c r="A18" s="36">
         <v>15</v>
       </c>
-      <c r="B18" s="195"/>
+      <c r="B18" s="201"/>
       <c r="C18" s="4" t="s">
         <v>954</v>
       </c>
@@ -37528,7 +37515,7 @@
       <c r="A19" s="36">
         <v>16</v>
       </c>
-      <c r="B19" s="193" t="s">
+      <c r="B19" s="199" t="s">
         <v>146</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -37561,7 +37548,7 @@
       <c r="A20" s="36">
         <v>17</v>
       </c>
-      <c r="B20" s="195"/>
+      <c r="B20" s="201"/>
       <c r="C20" s="4" t="s">
         <v>960</v>
       </c>
@@ -37818,18 +37805,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="195" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="192"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="198"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -37903,7 +37890,7 @@
       <c r="A4" s="36">
         <v>2</v>
       </c>
-      <c r="B4" s="200" t="s">
+      <c r="B4" s="202" t="s">
         <v>158</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -37934,7 +37921,7 @@
       <c r="A5" s="36">
         <v>3</v>
       </c>
-      <c r="B5" s="201"/>
+      <c r="B5" s="203"/>
       <c r="C5" s="4" t="s">
         <v>974</v>
       </c>
@@ -38033,7 +38020,7 @@
       <c r="A8" s="36">
         <v>6</v>
       </c>
-      <c r="B8" s="200" t="s">
+      <c r="B8" s="202" t="s">
         <v>169</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -38066,7 +38053,7 @@
       <c r="A9" s="36">
         <v>11</v>
       </c>
-      <c r="B9" s="201"/>
+      <c r="B9" s="203"/>
       <c r="C9" s="4" t="s">
         <v>984</v>
       </c>
@@ -38225,7 +38212,7 @@
       <c r="A14" s="36">
         <v>12</v>
       </c>
-      <c r="B14" s="200" t="s">
+      <c r="B14" s="202" t="s">
         <v>182</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -38258,7 +38245,7 @@
       <c r="A15" s="36">
         <v>13</v>
       </c>
-      <c r="B15" s="201"/>
+      <c r="B15" s="203"/>
       <c r="C15" s="4" t="s">
         <v>1000</v>
       </c>
@@ -38493,7 +38480,7 @@
       <c r="A22" s="36">
         <v>20</v>
       </c>
-      <c r="B22" s="200" t="s">
+      <c r="B22" s="202" t="s">
         <v>1009</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -38526,7 +38513,7 @@
       <c r="A23" s="36">
         <v>21</v>
       </c>
-      <c r="B23" s="202"/>
+      <c r="B23" s="204"/>
       <c r="C23" s="4" t="s">
         <v>1013</v>
       </c>
@@ -38556,7 +38543,7 @@
       <c r="A24" s="36">
         <v>22</v>
       </c>
-      <c r="B24" s="201"/>
+      <c r="B24" s="203"/>
       <c r="C24" s="4" t="s">
         <v>1016</v>
       </c>
@@ -38748,7 +38735,7 @@
       <c r="A30" s="36">
         <v>28</v>
       </c>
-      <c r="B30" s="200" t="s">
+      <c r="B30" s="202" t="s">
         <v>222</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -38781,7 +38768,7 @@
       <c r="A31" s="36">
         <v>29</v>
       </c>
-      <c r="B31" s="201"/>
+      <c r="B31" s="203"/>
       <c r="C31" s="4" t="s">
         <v>1029</v>
       </c>
@@ -38812,7 +38799,7 @@
       <c r="A32" s="36">
         <v>30</v>
       </c>
-      <c r="B32" s="200" t="s">
+      <c r="B32" s="202" t="s">
         <v>226</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -38845,7 +38832,7 @@
       <c r="A33" s="36">
         <v>31</v>
       </c>
-      <c r="B33" s="201"/>
+      <c r="B33" s="203"/>
       <c r="C33" s="4" t="s">
         <v>1033</v>
       </c>
@@ -39107,7 +39094,7 @@
       <c r="A41" s="36">
         <v>39</v>
       </c>
-      <c r="B41" s="200" t="s">
+      <c r="B41" s="202" t="s">
         <v>254</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -39140,7 +39127,7 @@
       <c r="A42" s="36">
         <v>40</v>
       </c>
-      <c r="B42" s="201"/>
+      <c r="B42" s="203"/>
       <c r="C42" s="4" t="s">
         <v>1045</v>
       </c>
@@ -39204,7 +39191,7 @@
       <c r="A44" s="36">
         <v>42</v>
       </c>
-      <c r="B44" s="200" t="s">
+      <c r="B44" s="202" t="s">
         <v>260</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -39237,7 +39224,7 @@
       <c r="A45" s="36">
         <v>43</v>
       </c>
-      <c r="B45" s="201"/>
+      <c r="B45" s="203"/>
       <c r="C45" s="4" t="s">
         <v>1052</v>
       </c>
@@ -39332,7 +39319,7 @@
       <c r="A48" s="36">
         <v>46</v>
       </c>
-      <c r="B48" s="200" t="s">
+      <c r="B48" s="202" t="s">
         <v>271</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -39356,7 +39343,7 @@
       <c r="I48" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J48" s="203" t="s">
+      <c r="J48" s="209" t="s">
         <v>274</v>
       </c>
       <c r="K48" s="90" t="s">
@@ -39367,7 +39354,7 @@
       <c r="A49" s="36">
         <v>47</v>
       </c>
-      <c r="B49" s="202"/>
+      <c r="B49" s="204"/>
       <c r="C49" s="4" t="s">
         <v>1060</v>
       </c>
@@ -39389,7 +39376,7 @@
       <c r="I49" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J49" s="203"/>
+      <c r="J49" s="209"/>
       <c r="K49" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39398,7 +39385,7 @@
       <c r="A50" s="36">
         <v>48</v>
       </c>
-      <c r="B50" s="202"/>
+      <c r="B50" s="204"/>
       <c r="C50" s="4" t="s">
         <v>1064</v>
       </c>
@@ -39420,7 +39407,7 @@
       <c r="I50" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J50" s="203"/>
+      <c r="J50" s="209"/>
       <c r="K50" s="135" t="s">
         <v>349</v>
       </c>
@@ -39429,7 +39416,7 @@
       <c r="A51" s="36">
         <v>49</v>
       </c>
-      <c r="B51" s="202"/>
+      <c r="B51" s="204"/>
       <c r="C51" s="4" t="s">
         <v>1067</v>
       </c>
@@ -39451,7 +39438,7 @@
       <c r="I51" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J51" s="203"/>
+      <c r="J51" s="209"/>
       <c r="K51" s="135" t="s">
         <v>1070</v>
       </c>
@@ -39460,7 +39447,7 @@
       <c r="A52" s="36">
         <v>50</v>
       </c>
-      <c r="B52" s="202"/>
+      <c r="B52" s="204"/>
       <c r="C52" s="4" t="s">
         <v>1071</v>
       </c>
@@ -39482,7 +39469,7 @@
       <c r="I52" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J52" s="203"/>
+      <c r="J52" s="209"/>
       <c r="K52" s="135" t="s">
         <v>1074</v>
       </c>
@@ -39491,7 +39478,7 @@
       <c r="A53" s="36">
         <v>51</v>
       </c>
-      <c r="B53" s="202"/>
+      <c r="B53" s="204"/>
       <c r="C53" s="4" t="s">
         <v>1075</v>
       </c>
@@ -39513,7 +39500,7 @@
       <c r="I53" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J53" s="203"/>
+      <c r="J53" s="209"/>
       <c r="K53" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39522,7 +39509,7 @@
       <c r="A54" s="36">
         <v>52</v>
       </c>
-      <c r="B54" s="202"/>
+      <c r="B54" s="204"/>
       <c r="C54" s="4" t="s">
         <v>1078</v>
       </c>
@@ -39544,7 +39531,7 @@
       <c r="I54" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J54" s="203"/>
+      <c r="J54" s="209"/>
       <c r="K54" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39553,7 +39540,7 @@
       <c r="A55" s="36">
         <v>53</v>
       </c>
-      <c r="B55" s="202"/>
+      <c r="B55" s="204"/>
       <c r="C55" s="4" t="s">
         <v>1081</v>
       </c>
@@ -39575,7 +39562,7 @@
       <c r="I55" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J55" s="203"/>
+      <c r="J55" s="209"/>
       <c r="K55" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39584,7 +39571,7 @@
       <c r="A56" s="36">
         <v>54</v>
       </c>
-      <c r="B56" s="202"/>
+      <c r="B56" s="204"/>
       <c r="C56" s="4" t="s">
         <v>1084</v>
       </c>
@@ -39602,7 +39589,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="89"/>
-      <c r="J56" s="203"/>
+      <c r="J56" s="209"/>
       <c r="K56" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39611,7 +39598,7 @@
       <c r="A57" s="36">
         <v>55</v>
       </c>
-      <c r="B57" s="201"/>
+      <c r="B57" s="203"/>
       <c r="C57" s="4" t="s">
         <v>1087</v>
       </c>
@@ -39633,7 +39620,7 @@
       <c r="I57" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J57" s="203"/>
+      <c r="J57" s="209"/>
       <c r="K57" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39642,7 +39629,7 @@
       <c r="A58" s="36">
         <v>56</v>
       </c>
-      <c r="B58" s="196" t="s">
+      <c r="B58" s="205" t="s">
         <v>271</v>
       </c>
       <c r="C58" s="4" t="s">
@@ -39666,7 +39653,7 @@
       <c r="I58" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J58" s="199" t="s">
+      <c r="J58" s="208" t="s">
         <v>274</v>
       </c>
       <c r="K58" s="135" t="s">
@@ -39677,7 +39664,7 @@
       <c r="A59" s="36">
         <v>57</v>
       </c>
-      <c r="B59" s="197"/>
+      <c r="B59" s="206"/>
       <c r="C59" s="4" t="s">
         <v>1093</v>
       </c>
@@ -39699,7 +39686,7 @@
       <c r="I59" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J59" s="199"/>
+      <c r="J59" s="208"/>
       <c r="K59" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39708,7 +39695,7 @@
       <c r="A60" s="36">
         <v>58</v>
       </c>
-      <c r="B60" s="197"/>
+      <c r="B60" s="206"/>
       <c r="C60" s="4" t="s">
         <v>1096</v>
       </c>
@@ -39730,7 +39717,7 @@
       <c r="I60" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J60" s="199"/>
+      <c r="J60" s="208"/>
       <c r="K60" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39739,7 +39726,7 @@
       <c r="A61" s="36">
         <v>59</v>
       </c>
-      <c r="B61" s="197"/>
+      <c r="B61" s="206"/>
       <c r="C61" s="4" t="s">
         <v>1099</v>
       </c>
@@ -39761,7 +39748,7 @@
       <c r="I61" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J61" s="199"/>
+      <c r="J61" s="208"/>
       <c r="K61" s="139" t="s">
         <v>66</v>
       </c>
@@ -39770,7 +39757,7 @@
       <c r="A62" s="36">
         <v>60</v>
       </c>
-      <c r="B62" s="197"/>
+      <c r="B62" s="206"/>
       <c r="C62" s="4" t="s">
         <v>1102</v>
       </c>
@@ -39792,7 +39779,7 @@
       <c r="I62" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J62" s="199"/>
+      <c r="J62" s="208"/>
       <c r="K62" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39801,7 +39788,7 @@
       <c r="A63" s="36">
         <v>61</v>
       </c>
-      <c r="B63" s="197"/>
+      <c r="B63" s="206"/>
       <c r="C63" s="4" t="s">
         <v>1104</v>
       </c>
@@ -39823,7 +39810,7 @@
       <c r="I63" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J63" s="199"/>
+      <c r="J63" s="208"/>
       <c r="K63" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39832,7 +39819,7 @@
       <c r="A64" s="36">
         <v>62</v>
       </c>
-      <c r="B64" s="197"/>
+      <c r="B64" s="206"/>
       <c r="C64" s="4" t="s">
         <v>963</v>
       </c>
@@ -39854,7 +39841,7 @@
       <c r="I64" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J64" s="199"/>
+      <c r="J64" s="208"/>
       <c r="K64" s="139" t="s">
         <v>1109</v>
       </c>
@@ -39863,7 +39850,7 @@
       <c r="A65" s="36">
         <v>63</v>
       </c>
-      <c r="B65" s="197"/>
+      <c r="B65" s="206"/>
       <c r="C65" s="4" t="s">
         <v>1110</v>
       </c>
@@ -39885,14 +39872,14 @@
       <c r="I65" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J65" s="199"/>
+      <c r="J65" s="208"/>
       <c r="K65" s="135" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="114" x14ac:dyDescent="0.25">
       <c r="A66" s="36"/>
-      <c r="B66" s="197"/>
+      <c r="B66" s="206"/>
       <c r="C66" s="4" t="s">
         <v>1113</v>
       </c>
@@ -39912,14 +39899,14 @@
         <v>60</v>
       </c>
       <c r="I66" s="39"/>
-      <c r="J66" s="199"/>
+      <c r="J66" s="208"/>
       <c r="K66" s="135" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A67" s="36"/>
-      <c r="B67" s="197"/>
+      <c r="B67" s="206"/>
       <c r="C67" s="41" t="s">
         <v>1116</v>
       </c>
@@ -39939,7 +39926,7 @@
         <v>30</v>
       </c>
       <c r="I67" s="39"/>
-      <c r="J67" s="199"/>
+      <c r="J67" s="208"/>
       <c r="K67" s="139" t="s">
         <v>1119</v>
       </c>
@@ -39948,7 +39935,7 @@
       <c r="A68" s="36">
         <v>64</v>
       </c>
-      <c r="B68" s="197"/>
+      <c r="B68" s="206"/>
       <c r="C68" s="131" t="s">
         <v>1120</v>
       </c>
@@ -39970,7 +39957,7 @@
       <c r="I68" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J68" s="199"/>
+      <c r="J68" s="208"/>
       <c r="K68" s="139" t="s">
         <v>1123</v>
       </c>
@@ -39979,7 +39966,7 @@
       <c r="A69" s="36">
         <v>65</v>
       </c>
-      <c r="B69" s="197"/>
+      <c r="B69" s="206"/>
       <c r="C69" s="4" t="s">
         <v>1124</v>
       </c>
@@ -40001,7 +39988,7 @@
       <c r="I69" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J69" s="199"/>
+      <c r="J69" s="208"/>
       <c r="K69" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40010,7 +39997,7 @@
       <c r="A70" s="36">
         <v>66</v>
       </c>
-      <c r="B70" s="197"/>
+      <c r="B70" s="206"/>
       <c r="C70" s="4" t="s">
         <v>1127</v>
       </c>
@@ -40032,7 +40019,7 @@
       <c r="I70" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J70" s="199"/>
+      <c r="J70" s="208"/>
       <c r="K70" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40041,7 +40028,7 @@
       <c r="A71" s="36">
         <v>67</v>
       </c>
-      <c r="B71" s="197"/>
+      <c r="B71" s="206"/>
       <c r="C71" s="4" t="s">
         <v>1130</v>
       </c>
@@ -40063,7 +40050,7 @@
       <c r="I71" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J71" s="199"/>
+      <c r="J71" s="208"/>
       <c r="K71" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40072,7 +40059,7 @@
       <c r="A72" s="36">
         <v>68</v>
       </c>
-      <c r="B72" s="197"/>
+      <c r="B72" s="206"/>
       <c r="C72" s="4" t="s">
         <v>1133</v>
       </c>
@@ -40094,7 +40081,7 @@
       <c r="I72" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J72" s="199"/>
+      <c r="J72" s="208"/>
       <c r="K72" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40103,7 +40090,7 @@
       <c r="A73" s="36">
         <v>69</v>
       </c>
-      <c r="B73" s="197"/>
+      <c r="B73" s="206"/>
       <c r="C73" s="4" t="s">
         <v>1135</v>
       </c>
@@ -40125,7 +40112,7 @@
       <c r="I73" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J73" s="199"/>
+      <c r="J73" s="208"/>
       <c r="K73" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40134,7 +40121,7 @@
       <c r="A74" s="36">
         <v>70</v>
       </c>
-      <c r="B74" s="197"/>
+      <c r="B74" s="206"/>
       <c r="C74" s="131" t="s">
         <v>1138</v>
       </c>
@@ -40154,7 +40141,7 @@
         <v>20</v>
       </c>
       <c r="I74" s="44"/>
-      <c r="J74" s="199"/>
+      <c r="J74" s="208"/>
       <c r="K74" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40163,7 +40150,7 @@
       <c r="A75" s="36">
         <v>70</v>
       </c>
-      <c r="B75" s="198"/>
+      <c r="B75" s="207"/>
       <c r="C75" s="131"/>
       <c r="D75" s="39"/>
       <c r="E75" s="131"/>
@@ -40171,7 +40158,7 @@
       <c r="G75" s="88"/>
       <c r="H75" s="36"/>
       <c r="I75" s="44"/>
-      <c r="J75" s="199"/>
+      <c r="J75" s="208"/>
       <c r="K75" s="72"/>
     </row>
     <row r="76" spans="1:11" s="2" customFormat="1" ht="39.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -40375,6 +40362,12 @@
     </sortState>
   </autoFilter>
   <mergeCells count="13">
+    <mergeCell ref="B58:B75"/>
+    <mergeCell ref="J58:J75"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B48:B57"/>
+    <mergeCell ref="J48:J57"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B14:B15"/>
@@ -40382,12 +40375,6 @@
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B58:B75"/>
-    <mergeCell ref="J58:J75"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B48:B57"/>
-    <mergeCell ref="J48:J57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -40423,18 +40410,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="195" t="s">
         <v>1147</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="192"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="198"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -41689,18 +41676,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="205" t="s">
+      <c r="A1" s="211" t="s">
         <v>1226</v>
       </c>
-      <c r="B1" s="206"/>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="205"/>
-      <c r="H1" s="207"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="208"/>
+      <c r="B1" s="212"/>
+      <c r="C1" s="212"/>
+      <c r="D1" s="212"/>
+      <c r="E1" s="213"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="213"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="214"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -41733,11 +41720,11 @@
       <c r="J2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="219" t="s">
+      <c r="K2" s="192" t="s">
         <v>886</v>
       </c>
       <c r="L2" s="64" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="71.25" x14ac:dyDescent="0.25">
@@ -41857,7 +41844,7 @@
       <c r="C6" s="4" t="s">
         <v>1231</v>
       </c>
-      <c r="D6" s="218" t="s">
+      <c r="D6" s="191" t="s">
         <v>371</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -41887,7 +41874,7 @@
       <c r="A7" s="36">
         <v>5</v>
       </c>
-      <c r="B7" s="203" t="s">
+      <c r="B7" s="209" t="s">
         <v>373</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -41923,7 +41910,7 @@
       <c r="A8" s="36">
         <v>6</v>
       </c>
-      <c r="B8" s="209"/>
+      <c r="B8" s="215"/>
       <c r="C8" s="4" t="s">
         <v>1234</v>
       </c>
@@ -41957,7 +41944,7 @@
       <c r="A9" s="36">
         <v>7</v>
       </c>
-      <c r="B9" s="209"/>
+      <c r="B9" s="215"/>
       <c r="C9" s="4" t="s">
         <v>1237</v>
       </c>
@@ -41991,7 +41978,7 @@
       <c r="A10" s="36">
         <v>8</v>
       </c>
-      <c r="B10" s="209"/>
+      <c r="B10" s="215"/>
       <c r="C10" s="4" t="s">
         <v>1239</v>
       </c>
@@ -42025,7 +42012,7 @@
       <c r="A11" s="36">
         <v>9</v>
       </c>
-      <c r="B11" s="209"/>
+      <c r="B11" s="215"/>
       <c r="C11" s="4" t="s">
         <v>1242</v>
       </c>
@@ -42059,7 +42046,7 @@
       <c r="A12" s="36">
         <v>10</v>
       </c>
-      <c r="B12" s="209"/>
+      <c r="B12" s="215"/>
       <c r="C12" s="4" t="s">
         <v>1245</v>
       </c>
@@ -42093,7 +42080,7 @@
       <c r="A13" s="36">
         <v>11</v>
       </c>
-      <c r="B13" s="209"/>
+      <c r="B13" s="215"/>
       <c r="C13" s="4" t="s">
         <v>1248</v>
       </c>
@@ -42127,7 +42114,7 @@
       <c r="A14" s="36">
         <v>12</v>
       </c>
-      <c r="B14" s="209"/>
+      <c r="B14" s="215"/>
       <c r="C14" s="4" t="s">
         <v>1251</v>
       </c>
@@ -42404,7 +42391,7 @@
       <c r="A22" s="36">
         <v>20</v>
       </c>
-      <c r="B22" s="203" t="s">
+      <c r="B22" s="209" t="s">
         <v>399</v>
       </c>
       <c r="C22" s="22" t="s">
@@ -42440,7 +42427,7 @@
       <c r="A23" s="58">
         <v>21</v>
       </c>
-      <c r="B23" s="210"/>
+      <c r="B23" s="216"/>
       <c r="C23" s="61" t="s">
         <v>1265</v>
       </c>
@@ -42471,7 +42458,7 @@
       <c r="A24" s="36">
         <v>22</v>
       </c>
-      <c r="B24" s="209"/>
+      <c r="B24" s="215"/>
       <c r="C24" s="22" t="s">
         <v>1268</v>
       </c>
@@ -42503,7 +42490,7 @@
       <c r="A25" s="36">
         <v>23</v>
       </c>
-      <c r="B25" s="209"/>
+      <c r="B25" s="215"/>
       <c r="C25" s="22" t="s">
         <v>1271</v>
       </c>
@@ -42535,7 +42522,7 @@
       <c r="A26" s="58">
         <v>24</v>
       </c>
-      <c r="B26" s="210"/>
+      <c r="B26" s="216"/>
       <c r="C26" s="61" t="s">
         <v>1274</v>
       </c>
@@ -42566,7 +42553,7 @@
       <c r="A27" s="36">
         <v>25</v>
       </c>
-      <c r="B27" s="209"/>
+      <c r="B27" s="215"/>
       <c r="C27" s="22" t="s">
         <v>1277</v>
       </c>
@@ -42670,7 +42657,7 @@
       <c r="A30" s="36">
         <v>28</v>
       </c>
-      <c r="B30" s="203" t="s">
+      <c r="B30" s="209" t="s">
         <v>409</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -42706,7 +42693,7 @@
       <c r="A31" s="36">
         <v>29</v>
       </c>
-      <c r="B31" s="209"/>
+      <c r="B31" s="215"/>
       <c r="C31" s="4" t="s">
         <v>1285</v>
       </c>
@@ -42740,7 +42727,7 @@
       <c r="A32" s="36">
         <v>30</v>
       </c>
-      <c r="B32" s="209"/>
+      <c r="B32" s="215"/>
       <c r="C32" s="4" t="s">
         <v>1288</v>
       </c>
@@ -42774,7 +42761,7 @@
       <c r="A33" s="36">
         <v>31</v>
       </c>
-      <c r="B33" s="209"/>
+      <c r="B33" s="215"/>
       <c r="C33" s="4" t="s">
         <v>1291</v>
       </c>
@@ -42814,7 +42801,7 @@
       <c r="C34" s="4" t="s">
         <v>1294</v>
       </c>
-      <c r="D34" s="216" t="s">
+      <c r="D34" s="189" t="s">
         <v>413</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -42994,7 +42981,7 @@
       <c r="A39" s="60">
         <v>37</v>
       </c>
-      <c r="B39" s="202" t="s">
+      <c r="B39" s="204" t="s">
         <v>428</v>
       </c>
       <c r="C39" s="52" t="s">
@@ -43025,7 +43012,7 @@
       <c r="A40" s="36">
         <v>38</v>
       </c>
-      <c r="B40" s="210"/>
+      <c r="B40" s="216"/>
       <c r="C40" s="4" t="s">
         <v>1304</v>
       </c>
@@ -43054,7 +43041,7 @@
       <c r="A41" s="54">
         <v>39</v>
       </c>
-      <c r="B41" s="210"/>
+      <c r="B41" s="216"/>
       <c r="C41" s="53" t="s">
         <v>1307</v>
       </c>
@@ -43081,7 +43068,7 @@
     </row>
     <row r="42" spans="1:12" ht="116.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="36"/>
-      <c r="B42" s="204" t="s">
+      <c r="B42" s="210" t="s">
         <v>1310</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -43117,7 +43104,7 @@
     </row>
     <row r="43" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="36"/>
-      <c r="B43" s="204"/>
+      <c r="B43" s="210"/>
       <c r="C43" s="4" t="s">
         <v>1314</v>
       </c>
@@ -43145,7 +43132,7 @@
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="36"/>
-      <c r="B44" s="204"/>
+      <c r="B44" s="210"/>
       <c r="C44" s="4" t="s">
         <v>1317</v>
       </c>
@@ -43173,13 +43160,13 @@
     </row>
     <row r="45" spans="1:12" ht="57" x14ac:dyDescent="0.25">
       <c r="A45" s="36"/>
-      <c r="B45" s="204" t="s">
+      <c r="B45" s="210" t="s">
         <v>435</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>1320</v>
       </c>
-      <c r="D45" s="215" t="s">
+      <c r="D45" s="188" t="s">
         <v>1321</v>
       </c>
       <c r="E45" s="4" t="s">
@@ -43203,11 +43190,11 @@
     </row>
     <row r="46" spans="1:12" ht="57" x14ac:dyDescent="0.25">
       <c r="A46" s="36"/>
-      <c r="B46" s="204"/>
+      <c r="B46" s="210"/>
       <c r="C46" s="4" t="s">
         <v>1323</v>
       </c>
-      <c r="D46" s="215" t="s">
+      <c r="D46" s="188" t="s">
         <v>1324</v>
       </c>
       <c r="E46" s="4" t="s">
@@ -43257,628 +43244,628 @@
       <c r="L48" s="187"/>
     </row>
     <row r="49" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L49" s="220"/>
+      <c r="L49" s="193"/>
     </row>
     <row r="50" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L50" s="220"/>
+      <c r="L50" s="193"/>
     </row>
     <row r="51" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L51" s="220"/>
+      <c r="L51" s="193"/>
     </row>
     <row r="52" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L52" s="220"/>
+      <c r="L52" s="193"/>
     </row>
     <row r="53" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L53" s="220"/>
+      <c r="L53" s="193"/>
     </row>
     <row r="54" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L54" s="220"/>
+      <c r="L54" s="193"/>
     </row>
     <row r="55" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L55" s="220"/>
+      <c r="L55" s="193"/>
     </row>
     <row r="56" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L56" s="220"/>
+      <c r="L56" s="193"/>
     </row>
     <row r="57" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L57" s="220"/>
+      <c r="L57" s="193"/>
     </row>
     <row r="58" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L58" s="220"/>
+      <c r="L58" s="193"/>
     </row>
     <row r="59" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L59" s="220"/>
+      <c r="L59" s="193"/>
     </row>
     <row r="60" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L60" s="220"/>
+      <c r="L60" s="193"/>
     </row>
     <row r="61" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L61" s="220"/>
+      <c r="L61" s="193"/>
     </row>
     <row r="62" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L62" s="220"/>
+      <c r="L62" s="193"/>
     </row>
     <row r="63" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L63" s="220"/>
+      <c r="L63" s="193"/>
     </row>
     <row r="64" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L64" s="220"/>
+      <c r="L64" s="193"/>
     </row>
     <row r="65" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L65" s="220"/>
+      <c r="L65" s="193"/>
     </row>
     <row r="66" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L66" s="220"/>
+      <c r="L66" s="193"/>
     </row>
     <row r="67" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L67" s="220"/>
+      <c r="L67" s="193"/>
     </row>
     <row r="68" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L68" s="220"/>
+      <c r="L68" s="193"/>
     </row>
     <row r="69" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L69" s="220"/>
+      <c r="L69" s="193"/>
     </row>
     <row r="70" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L70" s="220"/>
+      <c r="L70" s="193"/>
     </row>
     <row r="71" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L71" s="220"/>
+      <c r="L71" s="193"/>
     </row>
     <row r="72" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L72" s="220"/>
+      <c r="L72" s="193"/>
     </row>
     <row r="73" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L73" s="220"/>
+      <c r="L73" s="193"/>
     </row>
     <row r="74" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L74" s="220"/>
+      <c r="L74" s="193"/>
     </row>
     <row r="75" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L75" s="220"/>
+      <c r="L75" s="193"/>
     </row>
     <row r="76" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L76" s="220"/>
+      <c r="L76" s="193"/>
     </row>
     <row r="77" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L77" s="220"/>
+      <c r="L77" s="193"/>
     </row>
     <row r="78" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L78" s="220"/>
+      <c r="L78" s="193"/>
     </row>
     <row r="79" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L79" s="220"/>
+      <c r="L79" s="193"/>
     </row>
     <row r="80" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L80" s="220"/>
+      <c r="L80" s="193"/>
     </row>
     <row r="81" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L81" s="220"/>
+      <c r="L81" s="193"/>
     </row>
     <row r="82" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L82" s="220"/>
+      <c r="L82" s="193"/>
     </row>
     <row r="83" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L83" s="220"/>
+      <c r="L83" s="193"/>
     </row>
     <row r="84" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L84" s="220"/>
+      <c r="L84" s="193"/>
     </row>
     <row r="85" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L85" s="220"/>
+      <c r="L85" s="193"/>
     </row>
     <row r="86" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L86" s="220"/>
+      <c r="L86" s="193"/>
     </row>
     <row r="87" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L87" s="220"/>
+      <c r="L87" s="193"/>
     </row>
     <row r="88" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L88" s="220"/>
+      <c r="L88" s="193"/>
     </row>
     <row r="89" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L89" s="220"/>
+      <c r="L89" s="193"/>
     </row>
     <row r="90" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L90" s="220"/>
+      <c r="L90" s="193"/>
     </row>
     <row r="91" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L91" s="220"/>
+      <c r="L91" s="193"/>
     </row>
     <row r="92" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L92" s="220"/>
+      <c r="L92" s="193"/>
     </row>
     <row r="93" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L93" s="220"/>
+      <c r="L93" s="193"/>
     </row>
     <row r="94" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L94" s="220"/>
+      <c r="L94" s="193"/>
     </row>
     <row r="95" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L95" s="220"/>
+      <c r="L95" s="193"/>
     </row>
     <row r="96" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L96" s="220"/>
+      <c r="L96" s="193"/>
     </row>
     <row r="97" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L97" s="220"/>
+      <c r="L97" s="193"/>
     </row>
     <row r="98" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L98" s="220"/>
+      <c r="L98" s="193"/>
     </row>
     <row r="99" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L99" s="220"/>
+      <c r="L99" s="193"/>
     </row>
     <row r="100" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L100" s="220"/>
+      <c r="L100" s="193"/>
     </row>
     <row r="101" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L101" s="220"/>
+      <c r="L101" s="193"/>
     </row>
     <row r="102" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L102" s="220"/>
+      <c r="L102" s="193"/>
     </row>
     <row r="103" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L103" s="220"/>
+      <c r="L103" s="193"/>
     </row>
     <row r="104" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L104" s="220"/>
+      <c r="L104" s="193"/>
     </row>
     <row r="105" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L105" s="220"/>
+      <c r="L105" s="193"/>
     </row>
     <row r="106" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L106" s="220"/>
+      <c r="L106" s="193"/>
     </row>
     <row r="107" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L107" s="220"/>
+      <c r="L107" s="193"/>
     </row>
     <row r="108" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L108" s="220"/>
+      <c r="L108" s="193"/>
     </row>
     <row r="109" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L109" s="220"/>
+      <c r="L109" s="193"/>
     </row>
     <row r="110" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L110" s="220"/>
+      <c r="L110" s="193"/>
     </row>
     <row r="111" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L111" s="220"/>
+      <c r="L111" s="193"/>
     </row>
     <row r="112" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L112" s="220"/>
+      <c r="L112" s="193"/>
     </row>
     <row r="113" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L113" s="220"/>
+      <c r="L113" s="193"/>
     </row>
     <row r="114" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L114" s="220"/>
+      <c r="L114" s="193"/>
     </row>
     <row r="115" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L115" s="220"/>
+      <c r="L115" s="193"/>
     </row>
     <row r="116" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L116" s="220"/>
+      <c r="L116" s="193"/>
     </row>
     <row r="117" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L117" s="220"/>
+      <c r="L117" s="193"/>
     </row>
     <row r="118" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L118" s="220"/>
+      <c r="L118" s="193"/>
     </row>
     <row r="119" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L119" s="220"/>
+      <c r="L119" s="193"/>
     </row>
     <row r="120" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L120" s="220"/>
+      <c r="L120" s="193"/>
     </row>
     <row r="121" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L121" s="220"/>
+      <c r="L121" s="193"/>
     </row>
     <row r="122" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L122" s="220"/>
+      <c r="L122" s="193"/>
     </row>
     <row r="123" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L123" s="220"/>
+      <c r="L123" s="193"/>
     </row>
     <row r="124" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L124" s="220"/>
+      <c r="L124" s="193"/>
     </row>
     <row r="125" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L125" s="220"/>
+      <c r="L125" s="193"/>
     </row>
     <row r="126" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L126" s="220"/>
+      <c r="L126" s="193"/>
     </row>
     <row r="127" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L127" s="220"/>
+      <c r="L127" s="193"/>
     </row>
     <row r="128" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L128" s="220"/>
+      <c r="L128" s="193"/>
     </row>
     <row r="129" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L129" s="220"/>
+      <c r="L129" s="193"/>
     </row>
     <row r="130" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L130" s="220"/>
+      <c r="L130" s="193"/>
     </row>
     <row r="131" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L131" s="220"/>
+      <c r="L131" s="193"/>
     </row>
     <row r="132" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L132" s="220"/>
+      <c r="L132" s="193"/>
     </row>
     <row r="133" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L133" s="220"/>
+      <c r="L133" s="193"/>
     </row>
     <row r="134" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L134" s="220"/>
+      <c r="L134" s="193"/>
     </row>
     <row r="135" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L135" s="220"/>
+      <c r="L135" s="193"/>
     </row>
     <row r="136" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L136" s="220"/>
+      <c r="L136" s="193"/>
     </row>
     <row r="137" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L137" s="220"/>
+      <c r="L137" s="193"/>
     </row>
     <row r="138" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L138" s="220"/>
+      <c r="L138" s="193"/>
     </row>
     <row r="139" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L139" s="220"/>
+      <c r="L139" s="193"/>
     </row>
     <row r="140" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L140" s="220"/>
+      <c r="L140" s="193"/>
     </row>
     <row r="141" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L141" s="220"/>
+      <c r="L141" s="193"/>
     </row>
     <row r="142" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L142" s="220"/>
+      <c r="L142" s="193"/>
     </row>
     <row r="143" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L143" s="220"/>
+      <c r="L143" s="193"/>
     </row>
     <row r="144" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L144" s="220"/>
+      <c r="L144" s="193"/>
     </row>
     <row r="145" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L145" s="220"/>
+      <c r="L145" s="193"/>
     </row>
     <row r="146" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L146" s="220"/>
+      <c r="L146" s="193"/>
     </row>
     <row r="147" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L147" s="220"/>
+      <c r="L147" s="193"/>
     </row>
     <row r="148" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L148" s="220"/>
+      <c r="L148" s="193"/>
     </row>
     <row r="149" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L149" s="220"/>
+      <c r="L149" s="193"/>
     </row>
     <row r="150" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L150" s="220"/>
+      <c r="L150" s="193"/>
     </row>
     <row r="151" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L151" s="220"/>
+      <c r="L151" s="193"/>
     </row>
     <row r="152" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L152" s="220"/>
+      <c r="L152" s="193"/>
     </row>
     <row r="153" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L153" s="220"/>
+      <c r="L153" s="193"/>
     </row>
     <row r="154" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L154" s="220"/>
+      <c r="L154" s="193"/>
     </row>
     <row r="155" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L155" s="220"/>
+      <c r="L155" s="193"/>
     </row>
     <row r="156" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L156" s="220"/>
+      <c r="L156" s="193"/>
     </row>
     <row r="157" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L157" s="220"/>
+      <c r="L157" s="193"/>
     </row>
     <row r="158" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L158" s="220"/>
+      <c r="L158" s="193"/>
     </row>
     <row r="159" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L159" s="220"/>
+      <c r="L159" s="193"/>
     </row>
     <row r="160" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L160" s="220"/>
+      <c r="L160" s="193"/>
     </row>
     <row r="161" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L161" s="220"/>
+      <c r="L161" s="193"/>
     </row>
     <row r="162" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L162" s="220"/>
+      <c r="L162" s="193"/>
     </row>
     <row r="163" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L163" s="220"/>
+      <c r="L163" s="193"/>
     </row>
     <row r="164" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L164" s="220"/>
+      <c r="L164" s="193"/>
     </row>
     <row r="165" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L165" s="220"/>
+      <c r="L165" s="193"/>
     </row>
     <row r="166" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L166" s="220"/>
+      <c r="L166" s="193"/>
     </row>
     <row r="167" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L167" s="220"/>
+      <c r="L167" s="193"/>
     </row>
     <row r="168" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L168" s="220"/>
+      <c r="L168" s="193"/>
     </row>
     <row r="169" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L169" s="220"/>
+      <c r="L169" s="193"/>
     </row>
     <row r="170" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L170" s="220"/>
+      <c r="L170" s="193"/>
     </row>
     <row r="171" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L171" s="220"/>
+      <c r="L171" s="193"/>
     </row>
     <row r="172" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L172" s="220"/>
+      <c r="L172" s="193"/>
     </row>
     <row r="173" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L173" s="220"/>
+      <c r="L173" s="193"/>
     </row>
     <row r="174" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L174" s="220"/>
+      <c r="L174" s="193"/>
     </row>
     <row r="175" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L175" s="220"/>
+      <c r="L175" s="193"/>
     </row>
     <row r="176" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L176" s="220"/>
+      <c r="L176" s="193"/>
     </row>
     <row r="177" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L177" s="220"/>
+      <c r="L177" s="193"/>
     </row>
     <row r="178" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L178" s="220"/>
+      <c r="L178" s="193"/>
     </row>
     <row r="179" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L179" s="220"/>
+      <c r="L179" s="193"/>
     </row>
     <row r="180" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L180" s="220"/>
+      <c r="L180" s="193"/>
     </row>
     <row r="181" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L181" s="220"/>
+      <c r="L181" s="193"/>
     </row>
     <row r="182" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L182" s="220"/>
+      <c r="L182" s="193"/>
     </row>
     <row r="183" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L183" s="220"/>
+      <c r="L183" s="193"/>
     </row>
     <row r="184" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L184" s="220"/>
+      <c r="L184" s="193"/>
     </row>
     <row r="185" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L185" s="220"/>
+      <c r="L185" s="193"/>
     </row>
     <row r="186" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L186" s="220"/>
+      <c r="L186" s="193"/>
     </row>
     <row r="187" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L187" s="220"/>
+      <c r="L187" s="193"/>
     </row>
     <row r="188" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L188" s="220"/>
+      <c r="L188" s="193"/>
     </row>
     <row r="189" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L189" s="220"/>
+      <c r="L189" s="193"/>
     </row>
     <row r="190" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L190" s="220"/>
+      <c r="L190" s="193"/>
     </row>
     <row r="191" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L191" s="220"/>
+      <c r="L191" s="193"/>
     </row>
     <row r="192" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L192" s="220"/>
+      <c r="L192" s="193"/>
     </row>
     <row r="193" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L193" s="220"/>
+      <c r="L193" s="193"/>
     </row>
     <row r="194" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L194" s="220"/>
+      <c r="L194" s="193"/>
     </row>
     <row r="195" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L195" s="220"/>
+      <c r="L195" s="193"/>
     </row>
     <row r="196" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L196" s="220"/>
+      <c r="L196" s="193"/>
     </row>
     <row r="197" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L197" s="220"/>
+      <c r="L197" s="193"/>
     </row>
     <row r="198" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L198" s="220"/>
+      <c r="L198" s="193"/>
     </row>
     <row r="199" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L199" s="220"/>
+      <c r="L199" s="193"/>
     </row>
     <row r="200" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L200" s="220"/>
+      <c r="L200" s="193"/>
     </row>
     <row r="201" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L201" s="220"/>
+      <c r="L201" s="193"/>
     </row>
     <row r="202" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L202" s="220"/>
+      <c r="L202" s="193"/>
     </row>
     <row r="203" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L203" s="220"/>
+      <c r="L203" s="193"/>
     </row>
     <row r="204" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L204" s="220"/>
+      <c r="L204" s="193"/>
     </row>
     <row r="205" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L205" s="220"/>
+      <c r="L205" s="193"/>
     </row>
     <row r="206" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L206" s="220"/>
+      <c r="L206" s="193"/>
     </row>
     <row r="207" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L207" s="220"/>
+      <c r="L207" s="193"/>
     </row>
     <row r="208" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L208" s="220"/>
+      <c r="L208" s="193"/>
     </row>
     <row r="209" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L209" s="220"/>
+      <c r="L209" s="193"/>
     </row>
     <row r="210" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L210" s="220"/>
+      <c r="L210" s="193"/>
     </row>
     <row r="211" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L211" s="220"/>
+      <c r="L211" s="193"/>
     </row>
     <row r="212" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L212" s="220"/>
+      <c r="L212" s="193"/>
     </row>
     <row r="213" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L213" s="220"/>
+      <c r="L213" s="193"/>
     </row>
     <row r="214" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L214" s="220"/>
+      <c r="L214" s="193"/>
     </row>
     <row r="215" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L215" s="220"/>
+      <c r="L215" s="193"/>
     </row>
     <row r="216" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L216" s="220"/>
+      <c r="L216" s="193"/>
     </row>
     <row r="217" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L217" s="220"/>
+      <c r="L217" s="193"/>
     </row>
     <row r="218" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L218" s="220"/>
+      <c r="L218" s="193"/>
     </row>
     <row r="219" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L219" s="220"/>
+      <c r="L219" s="193"/>
     </row>
     <row r="220" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L220" s="220"/>
+      <c r="L220" s="193"/>
     </row>
     <row r="221" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L221" s="220"/>
+      <c r="L221" s="193"/>
     </row>
     <row r="222" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L222" s="220"/>
+      <c r="L222" s="193"/>
     </row>
     <row r="223" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L223" s="220"/>
+      <c r="L223" s="193"/>
     </row>
     <row r="224" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L224" s="220"/>
+      <c r="L224" s="193"/>
     </row>
     <row r="225" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L225" s="220"/>
+      <c r="L225" s="193"/>
     </row>
     <row r="226" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L226" s="220"/>
+      <c r="L226" s="193"/>
     </row>
     <row r="227" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L227" s="220"/>
+      <c r="L227" s="193"/>
     </row>
     <row r="228" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L228" s="220"/>
+      <c r="L228" s="193"/>
     </row>
     <row r="229" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L229" s="220"/>
+      <c r="L229" s="193"/>
     </row>
     <row r="230" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L230" s="220"/>
+      <c r="L230" s="193"/>
     </row>
     <row r="231" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L231" s="220"/>
+      <c r="L231" s="193"/>
     </row>
     <row r="232" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L232" s="220"/>
+      <c r="L232" s="193"/>
     </row>
     <row r="233" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L233" s="220"/>
+      <c r="L233" s="193"/>
     </row>
     <row r="234" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L234" s="220"/>
+      <c r="L234" s="193"/>
     </row>
     <row r="235" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L235" s="220"/>
+      <c r="L235" s="193"/>
     </row>
     <row r="236" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L236" s="220"/>
+      <c r="L236" s="193"/>
     </row>
     <row r="237" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L237" s="220"/>
+      <c r="L237" s="193"/>
     </row>
     <row r="238" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L238" s="220"/>
+      <c r="L238" s="193"/>
     </row>
     <row r="239" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L239" s="220"/>
+      <c r="L239" s="193"/>
     </row>
     <row r="240" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L240" s="220"/>
+      <c r="L240" s="193"/>
     </row>
     <row r="241" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L241" s="220"/>
+      <c r="L241" s="193"/>
     </row>
     <row r="242" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L242" s="220"/>
+      <c r="L242" s="193"/>
     </row>
     <row r="243" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L243" s="220"/>
+      <c r="L243" s="193"/>
     </row>
     <row r="244" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L244" s="220"/>
+      <c r="L244" s="193"/>
     </row>
     <row r="245" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L245" s="220"/>
+      <c r="L245" s="193"/>
     </row>
     <row r="246" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L246" s="220"/>
+      <c r="L246" s="193"/>
     </row>
     <row r="247" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L247" s="220"/>
+      <c r="L247" s="193"/>
     </row>
     <row r="248" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L248" s="220"/>
+      <c r="L248" s="193"/>
     </row>
     <row r="249" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L249" s="220"/>
+      <c r="L249" s="193"/>
     </row>
     <row r="250" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L250" s="220"/>
+      <c r="L250" s="193"/>
     </row>
     <row r="251" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L251" s="220"/>
+      <c r="L251" s="193"/>
     </row>
     <row r="252" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L252" s="220"/>
+      <c r="L252" s="193"/>
     </row>
     <row r="253" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L253" s="220"/>
+      <c r="L253" s="193"/>
     </row>
     <row r="254" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L254" s="220"/>
+      <c r="L254" s="193"/>
     </row>
     <row r="255" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L255" s="220"/>
+      <c r="L255" s="193"/>
     </row>
     <row r="256" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L256" s="220"/>
+      <c r="L256" s="193"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:K46" xr:uid="{00000000-0009-0000-0000-000006000000}">
@@ -43911,7 +43898,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -43932,18 +43919,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="195" t="s">
         <v>1883</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="192"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="198"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -43980,7 +43967,7 @@
         <v>886</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
@@ -44022,13 +44009,13 @@
       <c r="A4" s="36">
         <v>40</v>
       </c>
-      <c r="B4" s="200" t="s">
+      <c r="B4" s="202" t="s">
         <v>431</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1326</v>
       </c>
-      <c r="D4" s="218" t="s">
+      <c r="D4" s="191" t="s">
         <v>1327</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -44056,11 +44043,11 @@
       <c r="A5" s="54">
         <v>41</v>
       </c>
-      <c r="B5" s="202"/>
+      <c r="B5" s="204"/>
       <c r="C5" s="53" t="s">
         <v>1329</v>
       </c>
-      <c r="D5" s="217" t="s">
+      <c r="D5" s="190" t="s">
         <v>1330</v>
       </c>
       <c r="E5" s="132" t="s">
@@ -44110,8 +44097,8 @@
         <v>444</v>
       </c>
       <c r="K6" s="39"/>
-      <c r="L6" s="39" t="s">
-        <v>1897</v>
+      <c r="L6" s="4" t="s">
+        <v>1898</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
@@ -44181,18 +44168,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="195" t="s">
         <v>1333</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="192"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="208"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="211"/>
-      <c r="H1" s="192"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="208"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="214"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="217"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="214"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -44676,41 +44663,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -44917,32 +44869,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7F7E23-FE37-4AB8-A4B3-5025B5D9E450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44959,4 +44921,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Priority to Reg Proc Feature
</commit_message>
<xml_diff>
--- a/_files/requirements/Pending_Backlog_Stories_25Jun19_Updated.xlsx
+++ b/_files/requirements/Pending_Backlog_Stories_25Jun19_Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip-docs.wiki\_files\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A61F10-F909-4D7F-816D-94D521FBF8A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67231E0-79BC-4679-BA44-8BCD1B52FBDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="12" r:id="rId1"/>
@@ -34,13 +34,13 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Partner Management'!$A$2:$J$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Pre-registration'!$A$2:$J$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Registration Client'!$A$2:$J$78</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Registration Processor'!$A$2:$J$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Registration Processor'!$A$2:$J$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Resident Services'!$A$2:$J$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RoadmapFeatures!$B$3:$E$37</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId13"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5208" uniqueCount="1903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5227" uniqueCount="1904">
   <si>
     <t>Category</t>
   </si>
@@ -6648,6 +6648,9 @@
   </si>
   <si>
     <t>Requiered for all Modules</t>
+  </si>
+  <si>
+    <t>P!</t>
   </si>
 </sst>
 </file>
@@ -7261,7 +7264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7762,9 +7765,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7794,12 +7794,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -7831,6 +7825,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7855,15 +7852,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7875,6 +7863,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -7910,6 +7907,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -15060,7 +15069,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:D32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -15978,18 +15987,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="196" t="s">
         <v>1343</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="201"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="199"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -16439,7 +16448,7 @@
       <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="202" t="s">
+      <c r="B17" s="200" t="s">
         <v>503</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -16471,7 +16480,7 @@
       <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="204"/>
+      <c r="B18" s="202"/>
       <c r="C18" s="4" t="s">
         <v>1362</v>
       </c>
@@ -16811,19 +16820,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="196" t="s">
         <v>1367</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="201"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="197"/>
+      <c r="K1" s="199"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="153" t="s">
@@ -22138,18 +22147,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="196" t="s">
         <v>1732</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="201"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="199"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="38" t="s">
@@ -22187,7 +22196,7 @@
       <c r="A3" s="39">
         <v>1</v>
       </c>
-      <c r="B3" s="221" t="s">
+      <c r="B3" s="219" t="s">
         <v>527</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -22213,7 +22222,7 @@
       <c r="A4" s="39">
         <v>2</v>
       </c>
-      <c r="B4" s="222"/>
+      <c r="B4" s="220"/>
       <c r="C4" s="4" t="s">
         <v>1736</v>
       </c>
@@ -22235,7 +22244,7 @@
       <c r="A5" s="39">
         <v>3</v>
       </c>
-      <c r="B5" s="221" t="s">
+      <c r="B5" s="219" t="s">
         <v>530</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -22261,7 +22270,7 @@
       <c r="A6" s="39">
         <v>4</v>
       </c>
-      <c r="B6" s="223"/>
+      <c r="B6" s="221"/>
       <c r="C6" s="19" t="s">
         <v>1741</v>
       </c>
@@ -22285,7 +22294,7 @@
       <c r="A7" s="39">
         <v>5</v>
       </c>
-      <c r="B7" s="223"/>
+      <c r="B7" s="221"/>
       <c r="C7" s="19" t="s">
         <v>1744</v>
       </c>
@@ -22307,7 +22316,7 @@
       <c r="A8" s="39">
         <v>6</v>
       </c>
-      <c r="B8" s="223"/>
+      <c r="B8" s="221"/>
       <c r="C8" s="19" t="s">
         <v>1746</v>
       </c>
@@ -22329,7 +22338,7 @@
       <c r="A9" s="39">
         <v>7</v>
       </c>
-      <c r="B9" s="223"/>
+      <c r="B9" s="221"/>
       <c r="C9" s="19" t="s">
         <v>1748</v>
       </c>
@@ -22351,7 +22360,7 @@
       <c r="A10" s="39">
         <v>8</v>
       </c>
-      <c r="B10" s="223"/>
+      <c r="B10" s="221"/>
       <c r="C10" s="19" t="s">
         <v>1750</v>
       </c>
@@ -22373,7 +22382,7 @@
       <c r="A11" s="39">
         <v>9</v>
       </c>
-      <c r="B11" s="223"/>
+      <c r="B11" s="221"/>
       <c r="C11" s="19" t="s">
         <v>1752</v>
       </c>
@@ -22395,7 +22404,7 @@
       <c r="A12" s="39">
         <v>10</v>
       </c>
-      <c r="B12" s="223"/>
+      <c r="B12" s="221"/>
       <c r="C12" s="19" t="s">
         <v>1754</v>
       </c>
@@ -22417,7 +22426,7 @@
       <c r="A13" s="39">
         <v>11</v>
       </c>
-      <c r="B13" s="223"/>
+      <c r="B13" s="221"/>
       <c r="C13" s="19" t="s">
         <v>1756</v>
       </c>
@@ -22439,7 +22448,7 @@
       <c r="A14" s="39">
         <v>12</v>
       </c>
-      <c r="B14" s="223"/>
+      <c r="B14" s="221"/>
       <c r="C14" s="19" t="s">
         <v>1758</v>
       </c>
@@ -22463,7 +22472,7 @@
       <c r="A15" s="39">
         <v>13</v>
       </c>
-      <c r="B15" s="223"/>
+      <c r="B15" s="221"/>
       <c r="C15" s="19" t="s">
         <v>1761</v>
       </c>
@@ -22487,7 +22496,7 @@
       <c r="A16" s="39">
         <v>14</v>
       </c>
-      <c r="B16" s="222"/>
+      <c r="B16" s="220"/>
       <c r="C16" s="19" t="s">
         <v>1763</v>
       </c>
@@ -22609,7 +22618,7 @@
       <c r="A21" s="39">
         <v>19</v>
       </c>
-      <c r="B21" s="221" t="s">
+      <c r="B21" s="219" t="s">
         <v>545</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -22633,7 +22642,7 @@
       <c r="A22" s="39">
         <v>20</v>
       </c>
-      <c r="B22" s="223"/>
+      <c r="B22" s="221"/>
       <c r="C22" s="4" t="s">
         <v>1771</v>
       </c>
@@ -22655,7 +22664,7 @@
       <c r="A23" s="39">
         <v>21</v>
       </c>
-      <c r="B23" s="223"/>
+      <c r="B23" s="221"/>
       <c r="C23" s="4" t="s">
         <v>1773</v>
       </c>
@@ -22677,7 +22686,7 @@
       <c r="A24" s="39">
         <v>22</v>
       </c>
-      <c r="B24" s="223"/>
+      <c r="B24" s="221"/>
       <c r="C24" s="4" t="s">
         <v>1775</v>
       </c>
@@ -22699,7 +22708,7 @@
       <c r="A25" s="39">
         <v>23</v>
       </c>
-      <c r="B25" s="223"/>
+      <c r="B25" s="221"/>
       <c r="C25" s="4" t="s">
         <v>1777</v>
       </c>
@@ -22721,7 +22730,7 @@
       <c r="A26" s="39">
         <v>24</v>
       </c>
-      <c r="B26" s="222"/>
+      <c r="B26" s="220"/>
       <c r="C26" s="4" t="s">
         <v>1779</v>
       </c>
@@ -22743,7 +22752,7 @@
       <c r="A27" s="39">
         <v>25</v>
       </c>
-      <c r="B27" s="221" t="s">
+      <c r="B27" s="219" t="s">
         <v>548</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -22767,7 +22776,7 @@
       <c r="A28" s="39">
         <v>26</v>
       </c>
-      <c r="B28" s="222"/>
+      <c r="B28" s="220"/>
       <c r="C28" s="4" t="s">
         <v>1783</v>
       </c>
@@ -22789,7 +22798,7 @@
       <c r="A29" s="39">
         <v>27</v>
       </c>
-      <c r="B29" s="221" t="s">
+      <c r="B29" s="219" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -22813,7 +22822,7 @@
       <c r="A30" s="39">
         <v>28</v>
       </c>
-      <c r="B30" s="222"/>
+      <c r="B30" s="220"/>
       <c r="C30" s="4" t="s">
         <v>1787</v>
       </c>
@@ -22835,7 +22844,7 @@
       <c r="A31" s="39">
         <v>29</v>
       </c>
-      <c r="B31" s="221" t="s">
+      <c r="B31" s="219" t="s">
         <v>553</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -22859,7 +22868,7 @@
       <c r="A32" s="39">
         <v>30</v>
       </c>
-      <c r="B32" s="223"/>
+      <c r="B32" s="221"/>
       <c r="C32" s="4" t="s">
         <v>1791</v>
       </c>
@@ -22881,7 +22890,7 @@
       <c r="A33" s="39">
         <v>31</v>
       </c>
-      <c r="B33" s="223"/>
+      <c r="B33" s="221"/>
       <c r="C33" s="4" t="s">
         <v>1793</v>
       </c>
@@ -22903,7 +22912,7 @@
       <c r="A34" s="39">
         <v>32</v>
       </c>
-      <c r="B34" s="223"/>
+      <c r="B34" s="221"/>
       <c r="C34" s="4" t="s">
         <v>1795</v>
       </c>
@@ -22925,7 +22934,7 @@
       <c r="A35" s="39">
         <v>33</v>
       </c>
-      <c r="B35" s="222"/>
+      <c r="B35" s="220"/>
       <c r="C35" s="4" t="s">
         <v>1797</v>
       </c>
@@ -22947,7 +22956,7 @@
       <c r="A36" s="39">
         <v>34</v>
       </c>
-      <c r="B36" s="221" t="s">
+      <c r="B36" s="219" t="s">
         <v>556</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -22971,7 +22980,7 @@
       <c r="A37" s="39">
         <v>35</v>
       </c>
-      <c r="B37" s="223"/>
+      <c r="B37" s="221"/>
       <c r="C37" s="4" t="s">
         <v>1801</v>
       </c>
@@ -22993,7 +23002,7 @@
       <c r="A38" s="39">
         <v>36</v>
       </c>
-      <c r="B38" s="223"/>
+      <c r="B38" s="221"/>
       <c r="C38" s="4" t="s">
         <v>1803</v>
       </c>
@@ -23015,7 +23024,7 @@
       <c r="A39" s="39">
         <v>37</v>
       </c>
-      <c r="B39" s="222"/>
+      <c r="B39" s="220"/>
       <c r="C39" s="4" t="s">
         <v>1805</v>
       </c>
@@ -23037,7 +23046,7 @@
       <c r="A40" s="39">
         <v>38</v>
       </c>
-      <c r="B40" s="221" t="s">
+      <c r="B40" s="219" t="s">
         <v>559</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -23061,7 +23070,7 @@
       <c r="A41" s="39">
         <v>39</v>
       </c>
-      <c r="B41" s="222"/>
+      <c r="B41" s="220"/>
       <c r="C41" s="4" t="s">
         <v>1809</v>
       </c>
@@ -23107,7 +23116,7 @@
       <c r="A43" s="39">
         <v>41</v>
       </c>
-      <c r="B43" s="221" t="s">
+      <c r="B43" s="219" t="s">
         <v>565</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -23131,7 +23140,7 @@
       <c r="A44" s="39">
         <v>42</v>
       </c>
-      <c r="B44" s="223"/>
+      <c r="B44" s="221"/>
       <c r="C44" s="4" t="s">
         <v>1814</v>
       </c>
@@ -23153,7 +23162,7 @@
       <c r="A45" s="39">
         <v>43</v>
       </c>
-      <c r="B45" s="223"/>
+      <c r="B45" s="221"/>
       <c r="C45" s="4" t="s">
         <v>1816</v>
       </c>
@@ -23175,7 +23184,7 @@
       <c r="A46" s="39">
         <v>44</v>
       </c>
-      <c r="B46" s="223"/>
+      <c r="B46" s="221"/>
       <c r="C46" s="4" t="s">
         <v>1818</v>
       </c>
@@ -23199,7 +23208,7 @@
       <c r="A47" s="39">
         <v>45</v>
       </c>
-      <c r="B47" s="223"/>
+      <c r="B47" s="221"/>
       <c r="C47" s="4" t="s">
         <v>1821</v>
       </c>
@@ -23221,7 +23230,7 @@
       <c r="A48" s="39">
         <v>46</v>
       </c>
-      <c r="B48" s="223"/>
+      <c r="B48" s="221"/>
       <c r="C48" s="4" t="s">
         <v>1823</v>
       </c>
@@ -23243,7 +23252,7 @@
       <c r="A49" s="39">
         <v>47</v>
       </c>
-      <c r="B49" s="223"/>
+      <c r="B49" s="221"/>
       <c r="C49" s="4" t="s">
         <v>1825</v>
       </c>
@@ -23265,7 +23274,7 @@
       <c r="A50" s="39">
         <v>48</v>
       </c>
-      <c r="B50" s="223"/>
+      <c r="B50" s="221"/>
       <c r="C50" s="4" t="s">
         <v>1827</v>
       </c>
@@ -23289,7 +23298,7 @@
       <c r="A51" s="39">
         <v>49</v>
       </c>
-      <c r="B51" s="223"/>
+      <c r="B51" s="221"/>
       <c r="C51" s="4" t="s">
         <v>1829</v>
       </c>
@@ -23311,7 +23320,7 @@
       <c r="A52" s="39">
         <v>50</v>
       </c>
-      <c r="B52" s="223"/>
+      <c r="B52" s="221"/>
       <c r="C52" s="4" t="s">
         <v>1831</v>
       </c>
@@ -23333,7 +23342,7 @@
       <c r="A53" s="39">
         <v>51</v>
       </c>
-      <c r="B53" s="223"/>
+      <c r="B53" s="221"/>
       <c r="C53" s="4" t="s">
         <v>1833</v>
       </c>
@@ -23355,7 +23364,7 @@
       <c r="A54" s="39">
         <v>52</v>
       </c>
-      <c r="B54" s="222"/>
+      <c r="B54" s="220"/>
       <c r="C54" s="4" t="s">
         <v>1835</v>
       </c>
@@ -23388,16 +23397,16 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="10">
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B43:B54"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B35"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B16"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B43:B54"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -23438,26 +23447,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="198" t="s">
+      <c r="B2" s="196" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="200"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="199"/>
-      <c r="O2" s="199"/>
-      <c r="P2" s="199"/>
-      <c r="Q2" s="199"/>
-      <c r="R2" s="199"/>
-      <c r="S2" s="201"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="197"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="197"/>
+      <c r="O2" s="197"/>
+      <c r="P2" s="197"/>
+      <c r="Q2" s="197"/>
+      <c r="R2" s="197"/>
+      <c r="S2" s="199"/>
     </row>
     <row r="3" spans="2:19" ht="70" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
@@ -25459,7 +25468,7 @@
       <c r="R62" s="94"/>
       <c r="S62" s="47"/>
     </row>
-    <row r="63" spans="2:19" ht="168" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:19" ht="154" x14ac:dyDescent="0.35">
       <c r="B63" s="96">
         <v>60</v>
       </c>
@@ -25642,7 +25651,7 @@
       <c r="C68" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="D68" s="197" t="s">
+      <c r="D68" s="195" t="s">
         <v>222</v>
       </c>
       <c r="E68" s="124"/>
@@ -25676,7 +25685,7 @@
       <c r="C69" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="D69" s="197"/>
+      <c r="D69" s="195"/>
       <c r="E69" s="124"/>
       <c r="F69" s="47" t="s">
         <v>225</v>
@@ -27049,7 +27058,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="109" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:19" ht="28" x14ac:dyDescent="0.35">
       <c r="B109" s="96">
         <v>106</v>
       </c>
@@ -27085,7 +27094,7 @@
       <c r="R109" s="94"/>
       <c r="S109" s="47"/>
     </row>
-    <row r="110" spans="2:19" ht="70" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:19" ht="56" x14ac:dyDescent="0.35">
       <c r="B110" s="96">
         <v>107</v>
       </c>
@@ -27861,7 +27870,7 @@
       <c r="R131" s="94"/>
       <c r="S131" s="47"/>
     </row>
-    <row r="132" spans="2:19" ht="154" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:19" ht="140" x14ac:dyDescent="0.35">
       <c r="B132" s="96">
         <v>129</v>
       </c>
@@ -35421,12 +35430,12 @@
       <c r="F1" s="41"/>
     </row>
     <row r="2" spans="2:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="198" t="s">
+      <c r="B2" s="196" t="s">
         <v>885</v>
       </c>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="201"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="199"/>
       <c r="F2" s="41"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
@@ -36991,18 +37000,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="196" t="s">
         <v>907</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="201"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="199"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -37043,7 +37052,7 @@
       <c r="A3" s="36">
         <v>1</v>
       </c>
-      <c r="B3" s="202" t="s">
+      <c r="B3" s="200" t="s">
         <v>116</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -37078,7 +37087,7 @@
       <c r="A4" s="36">
         <v>2</v>
       </c>
-      <c r="B4" s="203"/>
+      <c r="B4" s="201"/>
       <c r="C4" s="22" t="s">
         <v>920</v>
       </c>
@@ -37111,7 +37120,7 @@
       <c r="A5" s="36">
         <v>3</v>
       </c>
-      <c r="B5" s="203"/>
+      <c r="B5" s="201"/>
       <c r="C5" s="4" t="s">
         <v>924</v>
       </c>
@@ -37144,7 +37153,7 @@
       <c r="A6" s="36">
         <v>4</v>
       </c>
-      <c r="B6" s="203"/>
+      <c r="B6" s="201"/>
       <c r="C6" s="4" t="s">
         <v>927</v>
       </c>
@@ -37177,7 +37186,7 @@
       <c r="A7" s="36">
         <v>5</v>
       </c>
-      <c r="B7" s="203"/>
+      <c r="B7" s="201"/>
       <c r="C7" s="4" t="s">
         <v>930</v>
       </c>
@@ -37208,7 +37217,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="36"/>
-      <c r="B8" s="203"/>
+      <c r="B8" s="201"/>
       <c r="C8" s="4" t="s">
         <v>934</v>
       </c>
@@ -37233,7 +37242,7 @@
       <c r="A9" s="36">
         <v>6</v>
       </c>
-      <c r="B9" s="204"/>
+      <c r="B9" s="202"/>
       <c r="C9" s="4" t="s">
         <v>936</v>
       </c>
@@ -37487,7 +37496,7 @@
       <c r="A17" s="36">
         <v>14</v>
       </c>
-      <c r="B17" s="202" t="s">
+      <c r="B17" s="200" t="s">
         <v>143</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -37520,7 +37529,7 @@
       <c r="A18" s="36">
         <v>15</v>
       </c>
-      <c r="B18" s="204"/>
+      <c r="B18" s="202"/>
       <c r="C18" s="4" t="s">
         <v>954</v>
       </c>
@@ -37551,7 +37560,7 @@
       <c r="A19" s="36">
         <v>16</v>
       </c>
-      <c r="B19" s="202" t="s">
+      <c r="B19" s="200" t="s">
         <v>146</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -37584,7 +37593,7 @@
       <c r="A20" s="36">
         <v>17</v>
       </c>
-      <c r="B20" s="204"/>
+      <c r="B20" s="202"/>
       <c r="C20" s="4" t="s">
         <v>960</v>
       </c>
@@ -37841,18 +37850,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="196" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="201"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="199"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -37926,7 +37935,7 @@
       <c r="A4" s="36">
         <v>2</v>
       </c>
-      <c r="B4" s="205" t="s">
+      <c r="B4" s="207" t="s">
         <v>158</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -37957,7 +37966,7 @@
       <c r="A5" s="36">
         <v>3</v>
       </c>
-      <c r="B5" s="206"/>
+      <c r="B5" s="208"/>
       <c r="C5" s="4" t="s">
         <v>974</v>
       </c>
@@ -38056,7 +38065,7 @@
       <c r="A8" s="36">
         <v>6</v>
       </c>
-      <c r="B8" s="205" t="s">
+      <c r="B8" s="207" t="s">
         <v>169</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -38089,7 +38098,7 @@
       <c r="A9" s="36">
         <v>11</v>
       </c>
-      <c r="B9" s="206"/>
+      <c r="B9" s="208"/>
       <c r="C9" s="4" t="s">
         <v>984</v>
       </c>
@@ -38248,7 +38257,7 @@
       <c r="A14" s="36">
         <v>12</v>
       </c>
-      <c r="B14" s="205" t="s">
+      <c r="B14" s="207" t="s">
         <v>182</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -38281,7 +38290,7 @@
       <c r="A15" s="36">
         <v>13</v>
       </c>
-      <c r="B15" s="206"/>
+      <c r="B15" s="208"/>
       <c r="C15" s="4" t="s">
         <v>1000</v>
       </c>
@@ -38516,7 +38525,7 @@
       <c r="A22" s="36">
         <v>20</v>
       </c>
-      <c r="B22" s="205" t="s">
+      <c r="B22" s="207" t="s">
         <v>1009</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -38549,7 +38558,7 @@
       <c r="A23" s="36">
         <v>21</v>
       </c>
-      <c r="B23" s="207"/>
+      <c r="B23" s="209"/>
       <c r="C23" s="4" t="s">
         <v>1013</v>
       </c>
@@ -38579,7 +38588,7 @@
       <c r="A24" s="36">
         <v>22</v>
       </c>
-      <c r="B24" s="206"/>
+      <c r="B24" s="208"/>
       <c r="C24" s="4" t="s">
         <v>1016</v>
       </c>
@@ -38771,7 +38780,7 @@
       <c r="A30" s="36">
         <v>28</v>
       </c>
-      <c r="B30" s="205" t="s">
+      <c r="B30" s="207" t="s">
         <v>222</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -38804,7 +38813,7 @@
       <c r="A31" s="36">
         <v>29</v>
       </c>
-      <c r="B31" s="206"/>
+      <c r="B31" s="208"/>
       <c r="C31" s="4" t="s">
         <v>1029</v>
       </c>
@@ -38835,7 +38844,7 @@
       <c r="A32" s="36">
         <v>30</v>
       </c>
-      <c r="B32" s="205" t="s">
+      <c r="B32" s="207" t="s">
         <v>226</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -38868,7 +38877,7 @@
       <c r="A33" s="36">
         <v>31</v>
       </c>
-      <c r="B33" s="206"/>
+      <c r="B33" s="208"/>
       <c r="C33" s="4" t="s">
         <v>1033</v>
       </c>
@@ -39130,7 +39139,7 @@
       <c r="A41" s="36">
         <v>39</v>
       </c>
-      <c r="B41" s="205" t="s">
+      <c r="B41" s="207" t="s">
         <v>254</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -39163,7 +39172,7 @@
       <c r="A42" s="36">
         <v>40</v>
       </c>
-      <c r="B42" s="206"/>
+      <c r="B42" s="208"/>
       <c r="C42" s="4" t="s">
         <v>1045</v>
       </c>
@@ -39227,7 +39236,7 @@
       <c r="A44" s="36">
         <v>42</v>
       </c>
-      <c r="B44" s="205" t="s">
+      <c r="B44" s="207" t="s">
         <v>260</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -39260,7 +39269,7 @@
       <c r="A45" s="36">
         <v>43</v>
       </c>
-      <c r="B45" s="206"/>
+      <c r="B45" s="208"/>
       <c r="C45" s="4" t="s">
         <v>1052</v>
       </c>
@@ -39351,11 +39360,11 @@
         <v>349</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="98" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="84" x14ac:dyDescent="0.35">
       <c r="A48" s="36">
         <v>46</v>
       </c>
-      <c r="B48" s="205" t="s">
+      <c r="B48" s="207" t="s">
         <v>271</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -39379,7 +39388,7 @@
       <c r="I48" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J48" s="212" t="s">
+      <c r="J48" s="210" t="s">
         <v>274</v>
       </c>
       <c r="K48" s="90" t="s">
@@ -39390,7 +39399,7 @@
       <c r="A49" s="36">
         <v>47</v>
       </c>
-      <c r="B49" s="207"/>
+      <c r="B49" s="209"/>
       <c r="C49" s="4" t="s">
         <v>1060</v>
       </c>
@@ -39412,7 +39421,7 @@
       <c r="I49" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J49" s="212"/>
+      <c r="J49" s="210"/>
       <c r="K49" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39421,7 +39430,7 @@
       <c r="A50" s="36">
         <v>48</v>
       </c>
-      <c r="B50" s="207"/>
+      <c r="B50" s="209"/>
       <c r="C50" s="4" t="s">
         <v>1064</v>
       </c>
@@ -39443,7 +39452,7 @@
       <c r="I50" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J50" s="212"/>
+      <c r="J50" s="210"/>
       <c r="K50" s="135" t="s">
         <v>349</v>
       </c>
@@ -39452,7 +39461,7 @@
       <c r="A51" s="36">
         <v>49</v>
       </c>
-      <c r="B51" s="207"/>
+      <c r="B51" s="209"/>
       <c r="C51" s="4" t="s">
         <v>1067</v>
       </c>
@@ -39474,7 +39483,7 @@
       <c r="I51" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J51" s="212"/>
+      <c r="J51" s="210"/>
       <c r="K51" s="135" t="s">
         <v>1070</v>
       </c>
@@ -39483,7 +39492,7 @@
       <c r="A52" s="36">
         <v>50</v>
       </c>
-      <c r="B52" s="207"/>
+      <c r="B52" s="209"/>
       <c r="C52" s="4" t="s">
         <v>1071</v>
       </c>
@@ -39505,7 +39514,7 @@
       <c r="I52" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J52" s="212"/>
+      <c r="J52" s="210"/>
       <c r="K52" s="135" t="s">
         <v>1074</v>
       </c>
@@ -39514,7 +39523,7 @@
       <c r="A53" s="36">
         <v>51</v>
       </c>
-      <c r="B53" s="207"/>
+      <c r="B53" s="209"/>
       <c r="C53" s="4" t="s">
         <v>1075</v>
       </c>
@@ -39536,7 +39545,7 @@
       <c r="I53" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J53" s="212"/>
+      <c r="J53" s="210"/>
       <c r="K53" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39545,7 +39554,7 @@
       <c r="A54" s="36">
         <v>52</v>
       </c>
-      <c r="B54" s="207"/>
+      <c r="B54" s="209"/>
       <c r="C54" s="4" t="s">
         <v>1078</v>
       </c>
@@ -39567,7 +39576,7 @@
       <c r="I54" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J54" s="212"/>
+      <c r="J54" s="210"/>
       <c r="K54" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39576,7 +39585,7 @@
       <c r="A55" s="36">
         <v>53</v>
       </c>
-      <c r="B55" s="207"/>
+      <c r="B55" s="209"/>
       <c r="C55" s="4" t="s">
         <v>1081</v>
       </c>
@@ -39598,7 +39607,7 @@
       <c r="I55" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J55" s="212"/>
+      <c r="J55" s="210"/>
       <c r="K55" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39607,7 +39616,7 @@
       <c r="A56" s="36">
         <v>54</v>
       </c>
-      <c r="B56" s="207"/>
+      <c r="B56" s="209"/>
       <c r="C56" s="4" t="s">
         <v>1084</v>
       </c>
@@ -39625,7 +39634,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="89"/>
-      <c r="J56" s="212"/>
+      <c r="J56" s="210"/>
       <c r="K56" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39634,7 +39643,7 @@
       <c r="A57" s="36">
         <v>55</v>
       </c>
-      <c r="B57" s="206"/>
+      <c r="B57" s="208"/>
       <c r="C57" s="4" t="s">
         <v>1087</v>
       </c>
@@ -39656,7 +39665,7 @@
       <c r="I57" s="89" t="s">
         <v>969</v>
       </c>
-      <c r="J57" s="212"/>
+      <c r="J57" s="210"/>
       <c r="K57" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39665,7 +39674,7 @@
       <c r="A58" s="36">
         <v>56</v>
       </c>
-      <c r="B58" s="208" t="s">
+      <c r="B58" s="203" t="s">
         <v>271</v>
       </c>
       <c r="C58" s="4" t="s">
@@ -39689,7 +39698,7 @@
       <c r="I58" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J58" s="211" t="s">
+      <c r="J58" s="206" t="s">
         <v>274</v>
       </c>
       <c r="K58" s="135" t="s">
@@ -39700,7 +39709,7 @@
       <c r="A59" s="36">
         <v>57</v>
       </c>
-      <c r="B59" s="209"/>
+      <c r="B59" s="204"/>
       <c r="C59" s="4" t="s">
         <v>1093</v>
       </c>
@@ -39722,7 +39731,7 @@
       <c r="I59" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J59" s="211"/>
+      <c r="J59" s="206"/>
       <c r="K59" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39731,7 +39740,7 @@
       <c r="A60" s="36">
         <v>58</v>
       </c>
-      <c r="B60" s="209"/>
+      <c r="B60" s="204"/>
       <c r="C60" s="4" t="s">
         <v>1096</v>
       </c>
@@ -39753,7 +39762,7 @@
       <c r="I60" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J60" s="211"/>
+      <c r="J60" s="206"/>
       <c r="K60" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39762,7 +39771,7 @@
       <c r="A61" s="36">
         <v>59</v>
       </c>
-      <c r="B61" s="209"/>
+      <c r="B61" s="204"/>
       <c r="C61" s="4" t="s">
         <v>1099</v>
       </c>
@@ -39784,16 +39793,16 @@
       <c r="I61" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J61" s="211"/>
+      <c r="J61" s="206"/>
       <c r="K61" s="139" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="42" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" ht="28" x14ac:dyDescent="0.35">
       <c r="A62" s="36">
         <v>60</v>
       </c>
-      <c r="B62" s="209"/>
+      <c r="B62" s="204"/>
       <c r="C62" s="4" t="s">
         <v>1102</v>
       </c>
@@ -39815,7 +39824,7 @@
       <c r="I62" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J62" s="211"/>
+      <c r="J62" s="206"/>
       <c r="K62" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39824,7 +39833,7 @@
       <c r="A63" s="36">
         <v>61</v>
       </c>
-      <c r="B63" s="209"/>
+      <c r="B63" s="204"/>
       <c r="C63" s="4" t="s">
         <v>1104</v>
       </c>
@@ -39846,7 +39855,7 @@
       <c r="I63" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J63" s="211"/>
+      <c r="J63" s="206"/>
       <c r="K63" s="135" t="s">
         <v>1063</v>
       </c>
@@ -39855,7 +39864,7 @@
       <c r="A64" s="36">
         <v>62</v>
       </c>
-      <c r="B64" s="209"/>
+      <c r="B64" s="204"/>
       <c r="C64" s="4" t="s">
         <v>963</v>
       </c>
@@ -39877,7 +39886,7 @@
       <c r="I64" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J64" s="211"/>
+      <c r="J64" s="206"/>
       <c r="K64" s="139" t="s">
         <v>1109</v>
       </c>
@@ -39886,7 +39895,7 @@
       <c r="A65" s="36">
         <v>63</v>
       </c>
-      <c r="B65" s="209"/>
+      <c r="B65" s="204"/>
       <c r="C65" s="4" t="s">
         <v>1110</v>
       </c>
@@ -39908,14 +39917,14 @@
       <c r="I65" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J65" s="211"/>
+      <c r="J65" s="206"/>
       <c r="K65" s="135" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="98" x14ac:dyDescent="0.35">
       <c r="A66" s="36"/>
-      <c r="B66" s="209"/>
+      <c r="B66" s="204"/>
       <c r="C66" s="4" t="s">
         <v>1113</v>
       </c>
@@ -39935,14 +39944,14 @@
         <v>60</v>
       </c>
       <c r="I66" s="39"/>
-      <c r="J66" s="211"/>
+      <c r="J66" s="206"/>
       <c r="K66" s="135" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="70" x14ac:dyDescent="0.35">
       <c r="A67" s="36"/>
-      <c r="B67" s="209"/>
+      <c r="B67" s="204"/>
       <c r="C67" s="41" t="s">
         <v>1116</v>
       </c>
@@ -39962,7 +39971,7 @@
         <v>30</v>
       </c>
       <c r="I67" s="39"/>
-      <c r="J67" s="211"/>
+      <c r="J67" s="206"/>
       <c r="K67" s="139" t="s">
         <v>1119</v>
       </c>
@@ -39971,7 +39980,7 @@
       <c r="A68" s="36">
         <v>64</v>
       </c>
-      <c r="B68" s="209"/>
+      <c r="B68" s="204"/>
       <c r="C68" s="131" t="s">
         <v>1120</v>
       </c>
@@ -39993,7 +40002,7 @@
       <c r="I68" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J68" s="211"/>
+      <c r="J68" s="206"/>
       <c r="K68" s="139" t="s">
         <v>1123</v>
       </c>
@@ -40002,7 +40011,7 @@
       <c r="A69" s="36">
         <v>65</v>
       </c>
-      <c r="B69" s="209"/>
+      <c r="B69" s="204"/>
       <c r="C69" s="4" t="s">
         <v>1124</v>
       </c>
@@ -40024,7 +40033,7 @@
       <c r="I69" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J69" s="211"/>
+      <c r="J69" s="206"/>
       <c r="K69" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40033,7 +40042,7 @@
       <c r="A70" s="36">
         <v>66</v>
       </c>
-      <c r="B70" s="209"/>
+      <c r="B70" s="204"/>
       <c r="C70" s="4" t="s">
         <v>1127</v>
       </c>
@@ -40055,7 +40064,7 @@
       <c r="I70" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J70" s="211"/>
+      <c r="J70" s="206"/>
       <c r="K70" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40064,7 +40073,7 @@
       <c r="A71" s="36">
         <v>67</v>
       </c>
-      <c r="B71" s="209"/>
+      <c r="B71" s="204"/>
       <c r="C71" s="4" t="s">
         <v>1130</v>
       </c>
@@ -40086,7 +40095,7 @@
       <c r="I71" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J71" s="211"/>
+      <c r="J71" s="206"/>
       <c r="K71" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40095,7 +40104,7 @@
       <c r="A72" s="36">
         <v>68</v>
       </c>
-      <c r="B72" s="209"/>
+      <c r="B72" s="204"/>
       <c r="C72" s="4" t="s">
         <v>1133</v>
       </c>
@@ -40117,7 +40126,7 @@
       <c r="I72" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J72" s="211"/>
+      <c r="J72" s="206"/>
       <c r="K72" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40126,7 +40135,7 @@
       <c r="A73" s="36">
         <v>69</v>
       </c>
-      <c r="B73" s="209"/>
+      <c r="B73" s="204"/>
       <c r="C73" s="4" t="s">
         <v>1135</v>
       </c>
@@ -40148,7 +40157,7 @@
       <c r="I73" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J73" s="211"/>
+      <c r="J73" s="206"/>
       <c r="K73" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40157,7 +40166,7 @@
       <c r="A74" s="36">
         <v>70</v>
       </c>
-      <c r="B74" s="209"/>
+      <c r="B74" s="204"/>
       <c r="C74" s="131" t="s">
         <v>1138</v>
       </c>
@@ -40177,7 +40186,7 @@
         <v>20</v>
       </c>
       <c r="I74" s="44"/>
-      <c r="J74" s="211"/>
+      <c r="J74" s="206"/>
       <c r="K74" s="139" t="s">
         <v>1063</v>
       </c>
@@ -40186,7 +40195,7 @@
       <c r="A75" s="36">
         <v>70</v>
       </c>
-      <c r="B75" s="210"/>
+      <c r="B75" s="205"/>
       <c r="C75" s="131"/>
       <c r="D75" s="39"/>
       <c r="E75" s="131"/>
@@ -40194,7 +40203,7 @@
       <c r="G75" s="88"/>
       <c r="H75" s="36"/>
       <c r="I75" s="44"/>
-      <c r="J75" s="211"/>
+      <c r="J75" s="206"/>
       <c r="K75" s="72"/>
     </row>
     <row r="76" spans="1:11" s="2" customFormat="1" ht="39.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -40398,12 +40407,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="13">
-    <mergeCell ref="B58:B75"/>
-    <mergeCell ref="J58:J75"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B48:B57"/>
-    <mergeCell ref="J48:J57"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B14:B15"/>
@@ -40411,6 +40414,12 @@
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B58:B75"/>
+    <mergeCell ref="J58:J75"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B48:B57"/>
+    <mergeCell ref="J48:J57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -40419,13 +40428,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:J1"/>
+      <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -40441,23 +40451,23 @@
     <col min="9" max="9" width="13.453125" style="2" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="16.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="67.453125" style="41" customWidth="1"/>
-    <col min="12" max="12" width="42.7265625" style="41" customWidth="1"/>
+    <col min="12" max="12" width="22.81640625" style="41" customWidth="1"/>
     <col min="13" max="16384" width="9.1796875" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="196" t="s">
         <v>1147</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="201"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="199"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -40493,6 +40503,9 @@
       <c r="K2" s="37" t="s">
         <v>1148</v>
       </c>
+      <c r="L2" s="65" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="168" x14ac:dyDescent="0.35">
       <c r="A3" s="170">
@@ -40528,7 +40541,9 @@
       <c r="K3" s="172" t="s">
         <v>1152</v>
       </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="4" t="s">
+        <v>1890</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="112" x14ac:dyDescent="0.35">
       <c r="A4" s="170">
@@ -40564,6 +40579,9 @@
       <c r="K4" s="172" t="s">
         <v>1156</v>
       </c>
+      <c r="L4" s="39" t="s">
+        <v>1890</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.35">
       <c r="A5" s="170">
@@ -40599,6 +40617,9 @@
       <c r="K5" s="172" t="s">
         <v>1160</v>
       </c>
+      <c r="L5" s="39" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="98" x14ac:dyDescent="0.35">
       <c r="A6" s="170">
@@ -40634,7 +40655,9 @@
       <c r="K6" s="172" t="s">
         <v>1164</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="4" t="s">
+        <v>1903</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="98" x14ac:dyDescent="0.35">
       <c r="A7" s="170">
@@ -40669,6 +40692,9 @@
       </c>
       <c r="K7" s="172" t="s">
         <v>1168</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>1890</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="168" x14ac:dyDescent="0.35">
@@ -40705,6 +40731,9 @@
       <c r="K8" s="172" t="s">
         <v>1172</v>
       </c>
+      <c r="L8" s="39" t="s">
+        <v>1890</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="98" x14ac:dyDescent="0.35">
       <c r="A9" s="170">
@@ -40740,13 +40769,15 @@
       <c r="K9" s="172" t="s">
         <v>1175</v>
       </c>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="1:12" ht="140" x14ac:dyDescent="0.35">
+      <c r="L9" s="4" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="170">
         <v>8</v>
       </c>
-      <c r="B10" s="175" t="s">
+      <c r="B10" s="174" t="s">
         <v>1176</v>
       </c>
       <c r="C10" s="172" t="s">
@@ -40770,14 +40801,14 @@
       <c r="I10" s="45" t="s">
         <v>939</v>
       </c>
-      <c r="J10" s="176" t="s">
+      <c r="J10" s="175" t="s">
         <v>1178</v>
       </c>
       <c r="K10" s="172" t="s">
         <v>1179</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="170">
         <v>9</v>
       </c>
@@ -40809,7 +40840,7 @@
       <c r="K11" s="169"/>
       <c r="L11" s="41"/>
     </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="170">
         <v>10</v>
       </c>
@@ -40841,7 +40872,7 @@
       <c r="K12" s="169"/>
       <c r="L12" s="41"/>
     </row>
-    <row r="13" spans="1:12" s="2" customFormat="1" ht="70" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" s="2" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="170">
         <v>11</v>
       </c>
@@ -40907,6 +40938,9 @@
       <c r="K14" s="172" t="s">
         <v>1184</v>
       </c>
+      <c r="L14" s="39" t="s">
+        <v>1889</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="28" x14ac:dyDescent="0.35">
       <c r="A15" s="170">
@@ -40940,6 +40974,9 @@
         <v>902</v>
       </c>
       <c r="K15" s="45"/>
+      <c r="L15" s="39" t="s">
+        <v>1887</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="28" x14ac:dyDescent="0.35">
       <c r="A16" s="170">
@@ -40973,6 +41010,9 @@
         <v>902</v>
       </c>
       <c r="K16" s="45"/>
+      <c r="L16" s="39" t="s">
+        <v>1887</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="84" x14ac:dyDescent="0.35">
       <c r="A17" s="170">
@@ -40981,13 +41021,13 @@
       <c r="B17" s="171" t="s">
         <v>1187</v>
       </c>
-      <c r="C17" s="176" t="s">
+      <c r="C17" s="175" t="s">
         <v>315</v>
       </c>
-      <c r="D17" s="177" t="s">
+      <c r="D17" s="176" t="s">
         <v>316</v>
       </c>
-      <c r="E17" s="176" t="s">
+      <c r="E17" s="175" t="s">
         <v>317</v>
       </c>
       <c r="F17" s="45" t="s">
@@ -41008,8 +41048,11 @@
       <c r="K17" s="172" t="s">
         <v>1188</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+      <c r="L17" s="39" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="2" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="170">
         <v>16</v>
       </c>
@@ -41073,8 +41116,11 @@
       <c r="K19" s="172" t="s">
         <v>1191</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+      <c r="L19" s="39" t="s">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="2" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="170">
         <v>18</v>
       </c>
@@ -41106,11 +41152,11 @@
       <c r="K20" s="169"/>
       <c r="L20" s="41"/>
     </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="170">
         <v>19</v>
       </c>
-      <c r="B21" s="178" t="s">
+      <c r="B21" s="177" t="s">
         <v>328</v>
       </c>
       <c r="C21" s="172"/>
@@ -41128,7 +41174,7 @@
       <c r="K21" s="169"/>
       <c r="L21" s="41"/>
     </row>
-    <row r="22" spans="1:12" s="2" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" s="2" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="170">
         <v>20</v>
       </c>
@@ -41160,7 +41206,7 @@
       <c r="K22" s="169"/>
       <c r="L22" s="41"/>
     </row>
-    <row r="23" spans="1:12" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" s="2" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="170">
         <v>21</v>
       </c>
@@ -41182,7 +41228,7 @@
       <c r="G23" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="179"/>
+      <c r="H23" s="178"/>
       <c r="I23" s="45" t="s">
         <v>939</v>
       </c>
@@ -41192,39 +41238,39 @@
       <c r="K23" s="169"/>
       <c r="L23" s="41"/>
     </row>
-    <row r="24" spans="1:12" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.35">
-      <c r="A24" s="180">
+    <row r="24" spans="1:12" s="2" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="179">
         <v>22</v>
       </c>
-      <c r="B24" s="181" t="s">
+      <c r="B24" s="180" t="s">
         <v>1195</v>
       </c>
-      <c r="C24" s="179" t="s">
+      <c r="C24" s="178" t="s">
         <v>1196</v>
       </c>
-      <c r="D24" s="182" t="s">
+      <c r="D24" s="181" t="s">
         <v>1197</v>
       </c>
-      <c r="E24" s="179" t="s">
+      <c r="E24" s="178" t="s">
         <v>1198</v>
       </c>
-      <c r="F24" s="182" t="s">
+      <c r="F24" s="181" t="s">
         <v>917</v>
       </c>
-      <c r="G24" s="182" t="s">
+      <c r="G24" s="181" t="s">
         <v>1199</v>
       </c>
       <c r="H24" s="45"/>
-      <c r="I24" s="182" t="s">
+      <c r="I24" s="181" t="s">
         <v>939</v>
       </c>
-      <c r="J24" s="183" t="s">
+      <c r="J24" s="182" t="s">
         <v>56</v>
       </c>
       <c r="K24" s="169"/>
       <c r="L24" s="41"/>
     </row>
-    <row r="25" spans="1:12" s="2" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" s="2" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="170">
         <v>23</v>
       </c>
@@ -41250,13 +41296,13 @@
       <c r="I25" s="45" t="s">
         <v>939</v>
       </c>
-      <c r="J25" s="176" t="s">
+      <c r="J25" s="175" t="s">
         <v>1201</v>
       </c>
       <c r="K25" s="169"/>
       <c r="L25" s="41"/>
     </row>
-    <row r="26" spans="1:12" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" s="2" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="170">
         <v>24</v>
       </c>
@@ -41278,7 +41324,7 @@
       <c r="G26" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="H26" s="182"/>
+      <c r="H26" s="181"/>
       <c r="I26" s="45" t="s">
         <v>939</v>
       </c>
@@ -41298,10 +41344,10 @@
       <c r="C27" s="172" t="s">
         <v>1203</v>
       </c>
-      <c r="D27" s="176" t="s">
+      <c r="D27" s="175" t="s">
         <v>344</v>
       </c>
-      <c r="E27" s="184" t="s">
+      <c r="E27" s="183" t="s">
         <v>345</v>
       </c>
       <c r="F27" s="45" t="s">
@@ -41310,7 +41356,7 @@
       <c r="G27" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="178">
+      <c r="H27" s="177">
         <v>0</v>
       </c>
       <c r="I27" s="45" t="s">
@@ -41322,103 +41368,105 @@
       <c r="K27" s="172" t="s">
         <v>1204</v>
       </c>
-      <c r="L27" s="5"/>
-    </row>
-    <row r="28" spans="1:12" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.35">
-      <c r="A28" s="180">
+      <c r="L27" s="4" t="s">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="2" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="179">
         <v>26</v>
       </c>
-      <c r="B28" s="181" t="s">
+      <c r="B28" s="180" t="s">
         <v>1205</v>
       </c>
-      <c r="C28" s="179" t="s">
+      <c r="C28" s="178" t="s">
         <v>1206</v>
       </c>
-      <c r="D28" s="182" t="s">
+      <c r="D28" s="181" t="s">
         <v>1207</v>
       </c>
-      <c r="E28" s="179" t="s">
+      <c r="E28" s="178" t="s">
         <v>1208</v>
       </c>
-      <c r="F28" s="182" t="s">
+      <c r="F28" s="181" t="s">
         <v>917</v>
       </c>
-      <c r="G28" s="182" t="s">
+      <c r="G28" s="181" t="s">
         <v>73</v>
       </c>
       <c r="H28" s="172"/>
-      <c r="I28" s="182" t="s">
+      <c r="I28" s="181" t="s">
         <v>939</v>
       </c>
-      <c r="J28" s="179" t="s">
+      <c r="J28" s="178" t="s">
         <v>1209</v>
       </c>
       <c r="K28" s="169"/>
       <c r="L28" s="41"/>
     </row>
-    <row r="29" spans="1:12" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.35">
-      <c r="A29" s="180">
+    <row r="29" spans="1:12" s="2" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="179">
         <v>27</v>
       </c>
-      <c r="B29" s="181" t="s">
+      <c r="B29" s="180" t="s">
         <v>1210</v>
       </c>
-      <c r="C29" s="179" t="s">
+      <c r="C29" s="178" t="s">
         <v>1211</v>
       </c>
-      <c r="D29" s="182" t="s">
+      <c r="D29" s="181" t="s">
         <v>1212</v>
       </c>
-      <c r="E29" s="179" t="s">
+      <c r="E29" s="178" t="s">
         <v>1213</v>
       </c>
-      <c r="F29" s="182" t="s">
+      <c r="F29" s="181" t="s">
         <v>917</v>
       </c>
-      <c r="G29" s="182" t="s">
+      <c r="G29" s="181" t="s">
         <v>73</v>
       </c>
       <c r="H29" s="172"/>
-      <c r="I29" s="182" t="s">
+      <c r="I29" s="181" t="s">
         <v>939</v>
       </c>
-      <c r="J29" s="179" t="s">
+      <c r="J29" s="178" t="s">
         <v>1209</v>
       </c>
       <c r="K29" s="169"/>
       <c r="L29" s="41"/>
     </row>
-    <row r="30" spans="1:12" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.35">
-      <c r="A30" s="180">
+    <row r="30" spans="1:12" s="2" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="179">
         <v>28</v>
       </c>
-      <c r="B30" s="181" t="s">
+      <c r="B30" s="180" t="s">
         <v>1214</v>
       </c>
-      <c r="C30" s="179" t="s">
+      <c r="C30" s="178" t="s">
         <v>1215</v>
       </c>
-      <c r="D30" s="182" t="s">
+      <c r="D30" s="181" t="s">
         <v>1216</v>
       </c>
-      <c r="E30" s="179" t="s">
+      <c r="E30" s="178" t="s">
         <v>1217</v>
       </c>
-      <c r="F30" s="182" t="s">
+      <c r="F30" s="181" t="s">
         <v>917</v>
       </c>
-      <c r="G30" s="182" t="s">
+      <c r="G30" s="181" t="s">
         <v>73</v>
       </c>
       <c r="H30" s="172"/>
-      <c r="I30" s="182"/>
-      <c r="J30" s="179" t="s">
+      <c r="I30" s="181"/>
+      <c r="J30" s="178" t="s">
         <v>1209</v>
       </c>
       <c r="K30" s="169"/>
       <c r="L30" s="41"/>
     </row>
-    <row r="31" spans="1:12" s="2" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" s="2" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="170">
         <v>29</v>
       </c>
@@ -41450,7 +41498,7 @@
       <c r="K31" s="169"/>
       <c r="L31" s="41"/>
     </row>
-    <row r="32" spans="1:12" s="2" customFormat="1" ht="70" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" s="2" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="170">
         <v>30</v>
       </c>
@@ -41478,7 +41526,7 @@
       <c r="K32" s="169"/>
       <c r="L32" s="41"/>
     </row>
-    <row r="33" spans="1:11" s="2" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" s="2" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="170">
         <v>31</v>
       </c>
@@ -41505,7 +41553,7 @@
       </c>
       <c r="K33" s="169"/>
     </row>
-    <row r="34" spans="1:11" ht="112" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="112" x14ac:dyDescent="0.35">
       <c r="A34" s="170">
         <v>32</v>
       </c>
@@ -41535,8 +41583,11 @@
       <c r="K34" s="172" t="s">
         <v>1222</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L34" s="39" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="170">
         <v>33</v>
       </c>
@@ -41564,116 +41615,135 @@
       <c r="I35" s="172"/>
       <c r="J35" s="172"/>
       <c r="K35" s="45"/>
-    </row>
-    <row r="36" spans="1:11" ht="28" x14ac:dyDescent="0.35">
-      <c r="A36" s="170">
+      <c r="L35" s="39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="28" x14ac:dyDescent="0.35">
+      <c r="A36" s="222">
         <v>34</v>
       </c>
-      <c r="B36" s="171" t="s">
+      <c r="B36" s="223" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="172" t="s">
+      <c r="C36" s="224" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="172" t="s">
+      <c r="D36" s="224" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="172" t="s">
+      <c r="E36" s="224" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="45" t="s">
+      <c r="F36" s="225" t="s">
         <v>1224</v>
       </c>
-      <c r="G36" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="H36" s="170" t="s">
+      <c r="G36" s="225" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="222" t="s">
         <v>1225</v>
       </c>
       <c r="I36" s="172"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45" t="s">
+      <c r="J36" s="225"/>
+      <c r="K36" s="225" t="s">
         <v>1225</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="28" x14ac:dyDescent="0.35">
-      <c r="A37" s="185">
+      <c r="L36" s="39" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="28" x14ac:dyDescent="0.35">
+      <c r="A37" s="170">
         <v>35</v>
       </c>
-      <c r="B37" s="186" t="s">
+      <c r="B37" s="171" t="s">
         <v>1869</v>
       </c>
-      <c r="C37" s="174" t="s">
+      <c r="C37" s="172" t="s">
         <v>1870</v>
       </c>
-      <c r="D37" s="169" t="s">
+      <c r="D37" s="45" t="s">
         <v>1873</v>
       </c>
-      <c r="E37" s="174" t="s">
+      <c r="E37" s="172" t="s">
         <v>1870</v>
       </c>
-      <c r="F37" s="169" t="s">
+      <c r="F37" s="45" t="s">
         <v>917</v>
       </c>
-      <c r="G37" s="169" t="s">
-        <v>5</v>
-      </c>
-      <c r="H37" s="185"/>
+      <c r="G37" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="170"/>
       <c r="I37" s="169"/>
-      <c r="J37" s="174"/>
-      <c r="K37" s="169" t="s">
+      <c r="J37" s="172"/>
+      <c r="K37" s="45" t="s">
         <v>1874</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="28" x14ac:dyDescent="0.35">
-      <c r="A38" s="185">
+      <c r="L37" s="194" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="28" x14ac:dyDescent="0.35">
+      <c r="A38" s="170">
         <v>36</v>
       </c>
-      <c r="B38" s="186" t="s">
+      <c r="B38" s="171" t="s">
         <v>1869</v>
       </c>
-      <c r="C38" s="174" t="s">
+      <c r="C38" s="172" t="s">
         <v>1871</v>
       </c>
-      <c r="D38" s="169" t="s">
+      <c r="D38" s="45" t="s">
         <v>1872</v>
       </c>
-      <c r="E38" s="174" t="s">
+      <c r="E38" s="172" t="s">
         <v>1871</v>
       </c>
-      <c r="F38" s="169" t="s">
+      <c r="F38" s="45" t="s">
         <v>917</v>
       </c>
-      <c r="G38" s="169" t="s">
-        <v>5</v>
-      </c>
-      <c r="H38" s="185"/>
+      <c r="G38" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="170"/>
       <c r="I38" s="169"/>
-      <c r="J38" s="174"/>
-      <c r="K38" s="169" t="s">
+      <c r="J38" s="172"/>
+      <c r="K38" s="45" t="s">
         <v>1874</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L38" s="39" t="s">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="I39" s="41"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="I40" s="41"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="I41" s="41"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="I42" s="41"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="I43" s="41"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="I44" s="41"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J36" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <autoFilter ref="A2:J38" xr:uid="{00000000-0009-0000-0000-000005000000}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Vital"/>
+        <filter val="Vital?"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
@@ -41688,10 +41758,10 @@
   <dimension ref="A1:L256"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M37" sqref="M37"/>
+      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -41712,18 +41782,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="212" t="s">
         <v>1226</v>
       </c>
-      <c r="B1" s="215"/>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="214"/>
-      <c r="H1" s="216"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="217"/>
+      <c r="B1" s="213"/>
+      <c r="C1" s="213"/>
+      <c r="D1" s="213"/>
+      <c r="E1" s="214"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="212"/>
+      <c r="H1" s="214"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="215"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -41756,7 +41826,7 @@
       <c r="J2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="192" t="s">
+      <c r="K2" s="189" t="s">
         <v>886</v>
       </c>
       <c r="L2" s="64" t="s">
@@ -41866,7 +41936,7 @@
       <c r="J5" s="59" t="s">
         <v>369</v>
       </c>
-      <c r="K5" s="195" t="s">
+      <c r="K5" s="192" t="s">
         <v>349</v>
       </c>
       <c r="L5" s="39"/>
@@ -41881,7 +41951,7 @@
       <c r="C6" s="4" t="s">
         <v>1231</v>
       </c>
-      <c r="D6" s="191" t="s">
+      <c r="D6" s="188" t="s">
         <v>371</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -41911,7 +41981,7 @@
       <c r="A7" s="36">
         <v>5</v>
       </c>
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="210" t="s">
         <v>373</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -41947,7 +42017,7 @@
       <c r="A8" s="36">
         <v>6</v>
       </c>
-      <c r="B8" s="218"/>
+      <c r="B8" s="216"/>
       <c r="C8" s="4" t="s">
         <v>1234</v>
       </c>
@@ -41977,11 +42047,11 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="84" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="70" x14ac:dyDescent="0.35">
       <c r="A9" s="36">
         <v>7</v>
       </c>
-      <c r="B9" s="218"/>
+      <c r="B9" s="216"/>
       <c r="C9" s="4" t="s">
         <v>1237</v>
       </c>
@@ -42015,7 +42085,7 @@
       <c r="A10" s="36">
         <v>8</v>
       </c>
-      <c r="B10" s="218"/>
+      <c r="B10" s="216"/>
       <c r="C10" s="4" t="s">
         <v>1239</v>
       </c>
@@ -42049,7 +42119,7 @@
       <c r="A11" s="36">
         <v>9</v>
       </c>
-      <c r="B11" s="218"/>
+      <c r="B11" s="216"/>
       <c r="C11" s="4" t="s">
         <v>1242</v>
       </c>
@@ -42083,7 +42153,7 @@
       <c r="A12" s="36">
         <v>10</v>
       </c>
-      <c r="B12" s="218"/>
+      <c r="B12" s="216"/>
       <c r="C12" s="4" t="s">
         <v>1245</v>
       </c>
@@ -42117,7 +42187,7 @@
       <c r="A13" s="36">
         <v>11</v>
       </c>
-      <c r="B13" s="218"/>
+      <c r="B13" s="216"/>
       <c r="C13" s="4" t="s">
         <v>1248</v>
       </c>
@@ -42151,7 +42221,7 @@
       <c r="A14" s="36">
         <v>12</v>
       </c>
-      <c r="B14" s="218"/>
+      <c r="B14" s="216"/>
       <c r="C14" s="4" t="s">
         <v>1251</v>
       </c>
@@ -42287,7 +42357,7 @@
       </c>
       <c r="L17" s="39"/>
     </row>
-    <row r="18" spans="1:12" ht="126" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="112" x14ac:dyDescent="0.35">
       <c r="A18" s="36">
         <v>16</v>
       </c>
@@ -42316,7 +42386,7 @@
         <v>1229</v>
       </c>
       <c r="J18" s="4"/>
-      <c r="K18" s="196" t="s">
+      <c r="K18" s="193" t="s">
         <v>474</v>
       </c>
       <c r="L18" s="4" t="s">
@@ -42433,7 +42503,7 @@
       <c r="A22" s="36">
         <v>20</v>
       </c>
-      <c r="B22" s="212" t="s">
+      <c r="B22" s="210" t="s">
         <v>399</v>
       </c>
       <c r="C22" s="22" t="s">
@@ -42469,7 +42539,7 @@
       <c r="A23" s="58">
         <v>21</v>
       </c>
-      <c r="B23" s="219"/>
+      <c r="B23" s="217"/>
       <c r="C23" s="61" t="s">
         <v>1265</v>
       </c>
@@ -42501,7 +42571,7 @@
       <c r="A24" s="36">
         <v>22</v>
       </c>
-      <c r="B24" s="218"/>
+      <c r="B24" s="216"/>
       <c r="C24" s="22" t="s">
         <v>1268</v>
       </c>
@@ -42533,7 +42603,7 @@
       <c r="A25" s="36">
         <v>23</v>
       </c>
-      <c r="B25" s="218"/>
+      <c r="B25" s="216"/>
       <c r="C25" s="22" t="s">
         <v>1271</v>
       </c>
@@ -42565,7 +42635,7 @@
       <c r="A26" s="58">
         <v>24</v>
       </c>
-      <c r="B26" s="219"/>
+      <c r="B26" s="217"/>
       <c r="C26" s="61" t="s">
         <v>1274</v>
       </c>
@@ -42597,7 +42667,7 @@
       <c r="A27" s="36">
         <v>25</v>
       </c>
-      <c r="B27" s="218"/>
+      <c r="B27" s="216"/>
       <c r="C27" s="22" t="s">
         <v>1277</v>
       </c>
@@ -42701,7 +42771,7 @@
       <c r="A30" s="36">
         <v>28</v>
       </c>
-      <c r="B30" s="212" t="s">
+      <c r="B30" s="210" t="s">
         <v>409</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -42737,7 +42807,7 @@
       <c r="A31" s="36">
         <v>29</v>
       </c>
-      <c r="B31" s="218"/>
+      <c r="B31" s="216"/>
       <c r="C31" s="4" t="s">
         <v>1285</v>
       </c>
@@ -42771,7 +42841,7 @@
       <c r="A32" s="36">
         <v>30</v>
       </c>
-      <c r="B32" s="218"/>
+      <c r="B32" s="216"/>
       <c r="C32" s="4" t="s">
         <v>1288</v>
       </c>
@@ -42805,7 +42875,7 @@
       <c r="A33" s="36">
         <v>31</v>
       </c>
-      <c r="B33" s="218"/>
+      <c r="B33" s="216"/>
       <c r="C33" s="4" t="s">
         <v>1291</v>
       </c>
@@ -42845,7 +42915,7 @@
       <c r="C34" s="4" t="s">
         <v>1294</v>
       </c>
-      <c r="D34" s="189" t="s">
+      <c r="D34" s="186" t="s">
         <v>413</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -43025,7 +43095,7 @@
       <c r="A39" s="60">
         <v>37</v>
       </c>
-      <c r="B39" s="207" t="s">
+      <c r="B39" s="209" t="s">
         <v>428</v>
       </c>
       <c r="C39" s="52" t="s">
@@ -43057,7 +43127,7 @@
       <c r="A40" s="36">
         <v>38</v>
       </c>
-      <c r="B40" s="219"/>
+      <c r="B40" s="217"/>
       <c r="C40" s="4" t="s">
         <v>1304</v>
       </c>
@@ -43087,7 +43157,7 @@
       <c r="A41" s="54">
         <v>39</v>
       </c>
-      <c r="B41" s="219"/>
+      <c r="B41" s="217"/>
       <c r="C41" s="53" t="s">
         <v>1307</v>
       </c>
@@ -43115,7 +43185,7 @@
     </row>
     <row r="42" spans="1:12" ht="116.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="36"/>
-      <c r="B42" s="213" t="s">
+      <c r="B42" s="211" t="s">
         <v>1310</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -43151,7 +43221,7 @@
     </row>
     <row r="43" spans="1:12" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="36"/>
-      <c r="B43" s="213"/>
+      <c r="B43" s="211"/>
       <c r="C43" s="4" t="s">
         <v>1314</v>
       </c>
@@ -43179,7 +43249,7 @@
     </row>
     <row r="44" spans="1:12" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="36"/>
-      <c r="B44" s="213"/>
+      <c r="B44" s="211"/>
       <c r="C44" s="4" t="s">
         <v>1317</v>
       </c>
@@ -43207,13 +43277,13 @@
     </row>
     <row r="45" spans="1:12" ht="56" x14ac:dyDescent="0.35">
       <c r="A45" s="36"/>
-      <c r="B45" s="213" t="s">
+      <c r="B45" s="211" t="s">
         <v>435</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>1320</v>
       </c>
-      <c r="D45" s="188" t="s">
+      <c r="D45" s="185" t="s">
         <v>1321</v>
       </c>
       <c r="E45" s="4" t="s">
@@ -43237,11 +43307,11 @@
     </row>
     <row r="46" spans="1:12" ht="56" x14ac:dyDescent="0.35">
       <c r="A46" s="36"/>
-      <c r="B46" s="213"/>
+      <c r="B46" s="211"/>
       <c r="C46" s="4" t="s">
         <v>1323</v>
       </c>
-      <c r="D46" s="188" t="s">
+      <c r="D46" s="185" t="s">
         <v>1324</v>
       </c>
       <c r="E46" s="4" t="s">
@@ -43288,631 +43358,631 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="L48" s="187"/>
+      <c r="L48" s="184"/>
     </row>
     <row r="49" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L49" s="193"/>
+      <c r="L49" s="190"/>
     </row>
     <row r="50" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L50" s="193"/>
+      <c r="L50" s="190"/>
     </row>
     <row r="51" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L51" s="193"/>
+      <c r="L51" s="190"/>
     </row>
     <row r="52" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L52" s="193"/>
+      <c r="L52" s="190"/>
     </row>
     <row r="53" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L53" s="193"/>
+      <c r="L53" s="190"/>
     </row>
     <row r="54" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L54" s="193"/>
+      <c r="L54" s="190"/>
     </row>
     <row r="55" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L55" s="193"/>
+      <c r="L55" s="190"/>
     </row>
     <row r="56" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L56" s="193"/>
+      <c r="L56" s="190"/>
     </row>
     <row r="57" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L57" s="193"/>
+      <c r="L57" s="190"/>
     </row>
     <row r="58" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L58" s="193"/>
+      <c r="L58" s="190"/>
     </row>
     <row r="59" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L59" s="193"/>
+      <c r="L59" s="190"/>
     </row>
     <row r="60" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L60" s="193"/>
+      <c r="L60" s="190"/>
     </row>
     <row r="61" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L61" s="193"/>
+      <c r="L61" s="190"/>
     </row>
     <row r="62" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L62" s="193"/>
+      <c r="L62" s="190"/>
     </row>
     <row r="63" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L63" s="193"/>
+      <c r="L63" s="190"/>
     </row>
     <row r="64" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L64" s="193"/>
+      <c r="L64" s="190"/>
     </row>
     <row r="65" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L65" s="193"/>
+      <c r="L65" s="190"/>
     </row>
     <row r="66" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L66" s="193"/>
+      <c r="L66" s="190"/>
     </row>
     <row r="67" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L67" s="193"/>
+      <c r="L67" s="190"/>
     </row>
     <row r="68" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L68" s="193"/>
+      <c r="L68" s="190"/>
     </row>
     <row r="69" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L69" s="193"/>
+      <c r="L69" s="190"/>
     </row>
     <row r="70" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L70" s="193"/>
+      <c r="L70" s="190"/>
     </row>
     <row r="71" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L71" s="193"/>
+      <c r="L71" s="190"/>
     </row>
     <row r="72" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L72" s="193"/>
+      <c r="L72" s="190"/>
     </row>
     <row r="73" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L73" s="193"/>
+      <c r="L73" s="190"/>
     </row>
     <row r="74" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L74" s="193"/>
+      <c r="L74" s="190"/>
     </row>
     <row r="75" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L75" s="193"/>
+      <c r="L75" s="190"/>
     </row>
     <row r="76" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L76" s="193"/>
+      <c r="L76" s="190"/>
     </row>
     <row r="77" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L77" s="193"/>
+      <c r="L77" s="190"/>
     </row>
     <row r="78" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L78" s="193"/>
+      <c r="L78" s="190"/>
     </row>
     <row r="79" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L79" s="193"/>
+      <c r="L79" s="190"/>
     </row>
     <row r="80" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L80" s="193"/>
+      <c r="L80" s="190"/>
     </row>
     <row r="81" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L81" s="193"/>
+      <c r="L81" s="190"/>
     </row>
     <row r="82" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L82" s="193"/>
+      <c r="L82" s="190"/>
     </row>
     <row r="83" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L83" s="193"/>
+      <c r="L83" s="190"/>
     </row>
     <row r="84" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L84" s="193"/>
+      <c r="L84" s="190"/>
     </row>
     <row r="85" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L85" s="193"/>
+      <c r="L85" s="190"/>
     </row>
     <row r="86" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L86" s="193"/>
+      <c r="L86" s="190"/>
     </row>
     <row r="87" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L87" s="193"/>
+      <c r="L87" s="190"/>
     </row>
     <row r="88" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L88" s="193"/>
+      <c r="L88" s="190"/>
     </row>
     <row r="89" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L89" s="193"/>
+      <c r="L89" s="190"/>
     </row>
     <row r="90" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L90" s="193"/>
+      <c r="L90" s="190"/>
     </row>
     <row r="91" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L91" s="193"/>
+      <c r="L91" s="190"/>
     </row>
     <row r="92" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L92" s="193"/>
+      <c r="L92" s="190"/>
     </row>
     <row r="93" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L93" s="193"/>
+      <c r="L93" s="190"/>
     </row>
     <row r="94" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L94" s="193"/>
+      <c r="L94" s="190"/>
     </row>
     <row r="95" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L95" s="193"/>
+      <c r="L95" s="190"/>
     </row>
     <row r="96" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L96" s="193"/>
+      <c r="L96" s="190"/>
     </row>
     <row r="97" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L97" s="193"/>
+      <c r="L97" s="190"/>
     </row>
     <row r="98" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L98" s="193"/>
+      <c r="L98" s="190"/>
     </row>
     <row r="99" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L99" s="193"/>
+      <c r="L99" s="190"/>
     </row>
     <row r="100" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L100" s="193"/>
+      <c r="L100" s="190"/>
     </row>
     <row r="101" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L101" s="193"/>
+      <c r="L101" s="190"/>
     </row>
     <row r="102" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L102" s="193"/>
+      <c r="L102" s="190"/>
     </row>
     <row r="103" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L103" s="193"/>
+      <c r="L103" s="190"/>
     </row>
     <row r="104" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L104" s="193"/>
+      <c r="L104" s="190"/>
     </row>
     <row r="105" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L105" s="193"/>
+      <c r="L105" s="190"/>
     </row>
     <row r="106" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L106" s="193"/>
+      <c r="L106" s="190"/>
     </row>
     <row r="107" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L107" s="193"/>
+      <c r="L107" s="190"/>
     </row>
     <row r="108" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L108" s="193"/>
+      <c r="L108" s="190"/>
     </row>
     <row r="109" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L109" s="193"/>
+      <c r="L109" s="190"/>
     </row>
     <row r="110" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L110" s="193"/>
+      <c r="L110" s="190"/>
     </row>
     <row r="111" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L111" s="193"/>
+      <c r="L111" s="190"/>
     </row>
     <row r="112" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L112" s="193"/>
+      <c r="L112" s="190"/>
     </row>
     <row r="113" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L113" s="193"/>
+      <c r="L113" s="190"/>
     </row>
     <row r="114" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L114" s="193"/>
+      <c r="L114" s="190"/>
     </row>
     <row r="115" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L115" s="193"/>
+      <c r="L115" s="190"/>
     </row>
     <row r="116" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L116" s="193"/>
+      <c r="L116" s="190"/>
     </row>
     <row r="117" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L117" s="193"/>
+      <c r="L117" s="190"/>
     </row>
     <row r="118" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L118" s="193"/>
+      <c r="L118" s="190"/>
     </row>
     <row r="119" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L119" s="193"/>
+      <c r="L119" s="190"/>
     </row>
     <row r="120" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L120" s="193"/>
+      <c r="L120" s="190"/>
     </row>
     <row r="121" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L121" s="193"/>
+      <c r="L121" s="190"/>
     </row>
     <row r="122" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L122" s="193"/>
+      <c r="L122" s="190"/>
     </row>
     <row r="123" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L123" s="193"/>
+      <c r="L123" s="190"/>
     </row>
     <row r="124" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L124" s="193"/>
+      <c r="L124" s="190"/>
     </row>
     <row r="125" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L125" s="193"/>
+      <c r="L125" s="190"/>
     </row>
     <row r="126" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L126" s="193"/>
+      <c r="L126" s="190"/>
     </row>
     <row r="127" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L127" s="193"/>
+      <c r="L127" s="190"/>
     </row>
     <row r="128" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L128" s="193"/>
+      <c r="L128" s="190"/>
     </row>
     <row r="129" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L129" s="193"/>
+      <c r="L129" s="190"/>
     </row>
     <row r="130" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L130" s="193"/>
+      <c r="L130" s="190"/>
     </row>
     <row r="131" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L131" s="193"/>
+      <c r="L131" s="190"/>
     </row>
     <row r="132" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L132" s="193"/>
+      <c r="L132" s="190"/>
     </row>
     <row r="133" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L133" s="193"/>
+      <c r="L133" s="190"/>
     </row>
     <row r="134" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L134" s="193"/>
+      <c r="L134" s="190"/>
     </row>
     <row r="135" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L135" s="193"/>
+      <c r="L135" s="190"/>
     </row>
     <row r="136" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L136" s="193"/>
+      <c r="L136" s="190"/>
     </row>
     <row r="137" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L137" s="193"/>
+      <c r="L137" s="190"/>
     </row>
     <row r="138" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L138" s="193"/>
+      <c r="L138" s="190"/>
     </row>
     <row r="139" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L139" s="193"/>
+      <c r="L139" s="190"/>
     </row>
     <row r="140" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L140" s="193"/>
+      <c r="L140" s="190"/>
     </row>
     <row r="141" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L141" s="193"/>
+      <c r="L141" s="190"/>
     </row>
     <row r="142" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L142" s="193"/>
+      <c r="L142" s="190"/>
     </row>
     <row r="143" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L143" s="193"/>
+      <c r="L143" s="190"/>
     </row>
     <row r="144" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L144" s="193"/>
+      <c r="L144" s="190"/>
     </row>
     <row r="145" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L145" s="193"/>
+      <c r="L145" s="190"/>
     </row>
     <row r="146" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L146" s="193"/>
+      <c r="L146" s="190"/>
     </row>
     <row r="147" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L147" s="193"/>
+      <c r="L147" s="190"/>
     </row>
     <row r="148" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L148" s="193"/>
+      <c r="L148" s="190"/>
     </row>
     <row r="149" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L149" s="193"/>
+      <c r="L149" s="190"/>
     </row>
     <row r="150" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L150" s="193"/>
+      <c r="L150" s="190"/>
     </row>
     <row r="151" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L151" s="193"/>
+      <c r="L151" s="190"/>
     </row>
     <row r="152" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L152" s="193"/>
+      <c r="L152" s="190"/>
     </row>
     <row r="153" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L153" s="193"/>
+      <c r="L153" s="190"/>
     </row>
     <row r="154" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L154" s="193"/>
+      <c r="L154" s="190"/>
     </row>
     <row r="155" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L155" s="193"/>
+      <c r="L155" s="190"/>
     </row>
     <row r="156" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L156" s="193"/>
+      <c r="L156" s="190"/>
     </row>
     <row r="157" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L157" s="193"/>
+      <c r="L157" s="190"/>
     </row>
     <row r="158" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L158" s="193"/>
+      <c r="L158" s="190"/>
     </row>
     <row r="159" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L159" s="193"/>
+      <c r="L159" s="190"/>
     </row>
     <row r="160" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L160" s="193"/>
+      <c r="L160" s="190"/>
     </row>
     <row r="161" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L161" s="193"/>
+      <c r="L161" s="190"/>
     </row>
     <row r="162" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L162" s="193"/>
+      <c r="L162" s="190"/>
     </row>
     <row r="163" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L163" s="193"/>
+      <c r="L163" s="190"/>
     </row>
     <row r="164" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L164" s="193"/>
+      <c r="L164" s="190"/>
     </row>
     <row r="165" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L165" s="193"/>
+      <c r="L165" s="190"/>
     </row>
     <row r="166" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L166" s="193"/>
+      <c r="L166" s="190"/>
     </row>
     <row r="167" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L167" s="193"/>
+      <c r="L167" s="190"/>
     </row>
     <row r="168" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L168" s="193"/>
+      <c r="L168" s="190"/>
     </row>
     <row r="169" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L169" s="193"/>
+      <c r="L169" s="190"/>
     </row>
     <row r="170" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L170" s="193"/>
+      <c r="L170" s="190"/>
     </row>
     <row r="171" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L171" s="193"/>
+      <c r="L171" s="190"/>
     </row>
     <row r="172" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L172" s="193"/>
+      <c r="L172" s="190"/>
     </row>
     <row r="173" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L173" s="193"/>
+      <c r="L173" s="190"/>
     </row>
     <row r="174" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L174" s="193"/>
+      <c r="L174" s="190"/>
     </row>
     <row r="175" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L175" s="193"/>
+      <c r="L175" s="190"/>
     </row>
     <row r="176" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L176" s="193"/>
+      <c r="L176" s="190"/>
     </row>
     <row r="177" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L177" s="193"/>
+      <c r="L177" s="190"/>
     </row>
     <row r="178" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L178" s="193"/>
+      <c r="L178" s="190"/>
     </row>
     <row r="179" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L179" s="193"/>
+      <c r="L179" s="190"/>
     </row>
     <row r="180" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L180" s="193"/>
+      <c r="L180" s="190"/>
     </row>
     <row r="181" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L181" s="193"/>
+      <c r="L181" s="190"/>
     </row>
     <row r="182" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L182" s="193"/>
+      <c r="L182" s="190"/>
     </row>
     <row r="183" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L183" s="193"/>
+      <c r="L183" s="190"/>
     </row>
     <row r="184" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L184" s="193"/>
+      <c r="L184" s="190"/>
     </row>
     <row r="185" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L185" s="193"/>
+      <c r="L185" s="190"/>
     </row>
     <row r="186" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L186" s="193"/>
+      <c r="L186" s="190"/>
     </row>
     <row r="187" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L187" s="193"/>
+      <c r="L187" s="190"/>
     </row>
     <row r="188" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L188" s="193"/>
+      <c r="L188" s="190"/>
     </row>
     <row r="189" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L189" s="193"/>
+      <c r="L189" s="190"/>
     </row>
     <row r="190" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L190" s="193"/>
+      <c r="L190" s="190"/>
     </row>
     <row r="191" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L191" s="193"/>
+      <c r="L191" s="190"/>
     </row>
     <row r="192" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L192" s="193"/>
+      <c r="L192" s="190"/>
     </row>
     <row r="193" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L193" s="193"/>
+      <c r="L193" s="190"/>
     </row>
     <row r="194" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L194" s="193"/>
+      <c r="L194" s="190"/>
     </row>
     <row r="195" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L195" s="193"/>
+      <c r="L195" s="190"/>
     </row>
     <row r="196" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L196" s="193"/>
+      <c r="L196" s="190"/>
     </row>
     <row r="197" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L197" s="193"/>
+      <c r="L197" s="190"/>
     </row>
     <row r="198" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L198" s="193"/>
+      <c r="L198" s="190"/>
     </row>
     <row r="199" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L199" s="193"/>
+      <c r="L199" s="190"/>
     </row>
     <row r="200" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L200" s="193"/>
+      <c r="L200" s="190"/>
     </row>
     <row r="201" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L201" s="193"/>
+      <c r="L201" s="190"/>
     </row>
     <row r="202" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L202" s="193"/>
+      <c r="L202" s="190"/>
     </row>
     <row r="203" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L203" s="193"/>
+      <c r="L203" s="190"/>
     </row>
     <row r="204" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L204" s="193"/>
+      <c r="L204" s="190"/>
     </row>
     <row r="205" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L205" s="193"/>
+      <c r="L205" s="190"/>
     </row>
     <row r="206" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L206" s="193"/>
+      <c r="L206" s="190"/>
     </row>
     <row r="207" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L207" s="193"/>
+      <c r="L207" s="190"/>
     </row>
     <row r="208" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L208" s="193"/>
+      <c r="L208" s="190"/>
     </row>
     <row r="209" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L209" s="193"/>
+      <c r="L209" s="190"/>
     </row>
     <row r="210" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L210" s="193"/>
+      <c r="L210" s="190"/>
     </row>
     <row r="211" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L211" s="193"/>
+      <c r="L211" s="190"/>
     </row>
     <row r="212" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L212" s="193"/>
+      <c r="L212" s="190"/>
     </row>
     <row r="213" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L213" s="193"/>
+      <c r="L213" s="190"/>
     </row>
     <row r="214" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L214" s="193"/>
+      <c r="L214" s="190"/>
     </row>
     <row r="215" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L215" s="193"/>
+      <c r="L215" s="190"/>
     </row>
     <row r="216" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L216" s="193"/>
+      <c r="L216" s="190"/>
     </row>
     <row r="217" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L217" s="193"/>
+      <c r="L217" s="190"/>
     </row>
     <row r="218" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L218" s="193"/>
+      <c r="L218" s="190"/>
     </row>
     <row r="219" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L219" s="193"/>
+      <c r="L219" s="190"/>
     </row>
     <row r="220" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L220" s="193"/>
+      <c r="L220" s="190"/>
     </row>
     <row r="221" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L221" s="193"/>
+      <c r="L221" s="190"/>
     </row>
     <row r="222" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L222" s="193"/>
+      <c r="L222" s="190"/>
     </row>
     <row r="223" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L223" s="193"/>
+      <c r="L223" s="190"/>
     </row>
     <row r="224" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L224" s="193"/>
+      <c r="L224" s="190"/>
     </row>
     <row r="225" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L225" s="193"/>
+      <c r="L225" s="190"/>
     </row>
     <row r="226" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L226" s="193"/>
+      <c r="L226" s="190"/>
     </row>
     <row r="227" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L227" s="193"/>
+      <c r="L227" s="190"/>
     </row>
     <row r="228" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L228" s="193"/>
+      <c r="L228" s="190"/>
     </row>
     <row r="229" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L229" s="193"/>
+      <c r="L229" s="190"/>
     </row>
     <row r="230" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L230" s="193"/>
+      <c r="L230" s="190"/>
     </row>
     <row r="231" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L231" s="193"/>
+      <c r="L231" s="190"/>
     </row>
     <row r="232" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L232" s="193"/>
+      <c r="L232" s="190"/>
     </row>
     <row r="233" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L233" s="193"/>
+      <c r="L233" s="190"/>
     </row>
     <row r="234" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L234" s="193"/>
+      <c r="L234" s="190"/>
     </row>
     <row r="235" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L235" s="193"/>
+      <c r="L235" s="190"/>
     </row>
     <row r="236" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L236" s="193"/>
+      <c r="L236" s="190"/>
     </row>
     <row r="237" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L237" s="193"/>
+      <c r="L237" s="190"/>
     </row>
     <row r="238" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L238" s="193"/>
+      <c r="L238" s="190"/>
     </row>
     <row r="239" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L239" s="193"/>
+      <c r="L239" s="190"/>
     </row>
     <row r="240" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L240" s="193"/>
+      <c r="L240" s="190"/>
     </row>
     <row r="241" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L241" s="193"/>
+      <c r="L241" s="190"/>
     </row>
     <row r="242" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L242" s="193"/>
+      <c r="L242" s="190"/>
     </row>
     <row r="243" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L243" s="193"/>
+      <c r="L243" s="190"/>
     </row>
     <row r="244" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L244" s="193"/>
+      <c r="L244" s="190"/>
     </row>
     <row r="245" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L245" s="193"/>
+      <c r="L245" s="190"/>
     </row>
     <row r="246" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L246" s="193"/>
+      <c r="L246" s="190"/>
     </row>
     <row r="247" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L247" s="193"/>
+      <c r="L247" s="190"/>
     </row>
     <row r="248" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L248" s="193"/>
+      <c r="L248" s="190"/>
     </row>
     <row r="249" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L249" s="193"/>
+      <c r="L249" s="190"/>
     </row>
     <row r="250" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L250" s="193"/>
+      <c r="L250" s="190"/>
     </row>
     <row r="251" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L251" s="193"/>
+      <c r="L251" s="190"/>
     </row>
     <row r="252" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L252" s="193"/>
+      <c r="L252" s="190"/>
     </row>
     <row r="253" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L253" s="193"/>
+      <c r="L253" s="190"/>
     </row>
     <row r="254" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L254" s="193"/>
+      <c r="L254" s="190"/>
     </row>
     <row r="255" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L255" s="193"/>
+      <c r="L255" s="190"/>
     </row>
     <row r="256" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L256" s="193"/>
+      <c r="L256" s="190"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:L47" xr:uid="{83965C4A-B8AA-4AB6-9432-148FE2887E50}">
@@ -43944,8 +44014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -43966,18 +44036,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="196" t="s">
         <v>1883</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="201"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="199"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -44056,13 +44126,13 @@
       <c r="A4" s="36">
         <v>40</v>
       </c>
-      <c r="B4" s="205" t="s">
+      <c r="B4" s="207" t="s">
         <v>431</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1326</v>
       </c>
-      <c r="D4" s="191" t="s">
+      <c r="D4" s="188" t="s">
         <v>1327</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -44090,11 +44160,11 @@
       <c r="A5" s="54">
         <v>41</v>
       </c>
-      <c r="B5" s="207"/>
+      <c r="B5" s="209"/>
       <c r="C5" s="53" t="s">
         <v>1329</v>
       </c>
-      <c r="D5" s="190" t="s">
+      <c r="D5" s="187" t="s">
         <v>1330</v>
       </c>
       <c r="E5" s="132" t="s">
@@ -44178,7 +44248,7 @@
     </row>
     <row r="8" spans="1:12" ht="70" x14ac:dyDescent="0.35">
       <c r="A8" s="36"/>
-      <c r="B8" s="194" t="s">
+      <c r="B8" s="191" t="s">
         <v>1900</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -44245,18 +44315,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="196" t="s">
         <v>1333</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="217"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="215"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -44740,32 +44810,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -44972,6 +45016,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -44982,23 +45052,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7F7E23-FE37-4AB8-A4B3-5025B5D9E450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -45017,6 +45070,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Modified Pending Backlog Stories
</commit_message>
<xml_diff>
--- a/_files/requirements/Pending_Backlog_Stories_25Jun19_Updated.xlsx
+++ b/_files/requirements/Pending_Backlog_Stories_25Jun19_Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip-docs.wiki\_files\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B0D333-F612-45CE-8F88-4712EE1808DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3BB2E4-B64A-4B19-A2F9-65D8CE05122B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="12" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5359" uniqueCount="1945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5366" uniqueCount="1950">
   <si>
     <t>Category</t>
   </si>
@@ -6739,6 +6739,21 @@
   </si>
   <si>
     <t>De-Scoped</t>
+  </si>
+  <si>
+    <t>Will be taken Care in Re-Printing</t>
+  </si>
+  <si>
+    <t>Tech Story - Move Packet Generator to Secure Zone</t>
+  </si>
+  <si>
+    <t>Packet Generator</t>
+  </si>
+  <si>
+    <t>Move Packet Generator to Secure Zone</t>
+  </si>
+  <si>
+    <t>MOS-27343</t>
   </si>
 </sst>
 </file>
@@ -7324,7 +7339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="242">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7951,6 +7966,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -8018,15 +8045,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -16095,18 +16113,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="217" t="s">
+      <c r="A1" s="221" t="s">
         <v>1341</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="220"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="224"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -16556,7 +16574,7 @@
       <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="221" t="s">
+      <c r="B17" s="225" t="s">
         <v>503</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -16588,7 +16606,7 @@
       <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="222"/>
+      <c r="B18" s="226"/>
       <c r="C18" s="4" t="s">
         <v>1360</v>
       </c>
@@ -16928,19 +16946,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="217" t="s">
+      <c r="A1" s="221" t="s">
         <v>1365</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="218"/>
-      <c r="K1" s="220"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="222"/>
+      <c r="K1" s="224"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="146" t="s">
@@ -22282,18 +22300,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="217" t="s">
+      <c r="A1" s="221" t="s">
         <v>1730</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="220"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="224"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="38" t="s">
@@ -22331,7 +22349,7 @@
       <c r="A3" s="39">
         <v>1</v>
       </c>
-      <c r="B3" s="236" t="s">
+      <c r="B3" s="240" t="s">
         <v>527</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -22357,7 +22375,7 @@
       <c r="A4" s="39">
         <v>2</v>
       </c>
-      <c r="B4" s="237"/>
+      <c r="B4" s="241"/>
       <c r="C4" s="4" t="s">
         <v>1734</v>
       </c>
@@ -22379,7 +22397,7 @@
       <c r="A5" s="39">
         <v>3</v>
       </c>
-      <c r="B5" s="236" t="s">
+      <c r="B5" s="240" t="s">
         <v>530</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -22405,7 +22423,7 @@
       <c r="A6" s="39">
         <v>4</v>
       </c>
-      <c r="B6" s="238"/>
+      <c r="B6" s="242"/>
       <c r="C6" s="19" t="s">
         <v>1739</v>
       </c>
@@ -22429,7 +22447,7 @@
       <c r="A7" s="39">
         <v>5</v>
       </c>
-      <c r="B7" s="238"/>
+      <c r="B7" s="242"/>
       <c r="C7" s="19" t="s">
         <v>1742</v>
       </c>
@@ -22451,7 +22469,7 @@
       <c r="A8" s="39">
         <v>6</v>
       </c>
-      <c r="B8" s="238"/>
+      <c r="B8" s="242"/>
       <c r="C8" s="19" t="s">
         <v>1744</v>
       </c>
@@ -22473,7 +22491,7 @@
       <c r="A9" s="39">
         <v>7</v>
       </c>
-      <c r="B9" s="238"/>
+      <c r="B9" s="242"/>
       <c r="C9" s="19" t="s">
         <v>1746</v>
       </c>
@@ -22495,7 +22513,7 @@
       <c r="A10" s="39">
         <v>8</v>
       </c>
-      <c r="B10" s="238"/>
+      <c r="B10" s="242"/>
       <c r="C10" s="19" t="s">
         <v>1748</v>
       </c>
@@ -22517,7 +22535,7 @@
       <c r="A11" s="39">
         <v>9</v>
       </c>
-      <c r="B11" s="238"/>
+      <c r="B11" s="242"/>
       <c r="C11" s="19" t="s">
         <v>1750</v>
       </c>
@@ -22539,7 +22557,7 @@
       <c r="A12" s="39">
         <v>10</v>
       </c>
-      <c r="B12" s="238"/>
+      <c r="B12" s="242"/>
       <c r="C12" s="19" t="s">
         <v>1752</v>
       </c>
@@ -22561,7 +22579,7 @@
       <c r="A13" s="39">
         <v>11</v>
       </c>
-      <c r="B13" s="238"/>
+      <c r="B13" s="242"/>
       <c r="C13" s="19" t="s">
         <v>1754</v>
       </c>
@@ -22583,7 +22601,7 @@
       <c r="A14" s="39">
         <v>12</v>
       </c>
-      <c r="B14" s="238"/>
+      <c r="B14" s="242"/>
       <c r="C14" s="19" t="s">
         <v>1756</v>
       </c>
@@ -22607,7 +22625,7 @@
       <c r="A15" s="39">
         <v>13</v>
       </c>
-      <c r="B15" s="238"/>
+      <c r="B15" s="242"/>
       <c r="C15" s="19" t="s">
         <v>1759</v>
       </c>
@@ -22631,7 +22649,7 @@
       <c r="A16" s="39">
         <v>14</v>
       </c>
-      <c r="B16" s="237"/>
+      <c r="B16" s="241"/>
       <c r="C16" s="19" t="s">
         <v>1761</v>
       </c>
@@ -22753,7 +22771,7 @@
       <c r="A21" s="39">
         <v>19</v>
       </c>
-      <c r="B21" s="236" t="s">
+      <c r="B21" s="240" t="s">
         <v>545</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -22777,7 +22795,7 @@
       <c r="A22" s="39">
         <v>20</v>
       </c>
-      <c r="B22" s="238"/>
+      <c r="B22" s="242"/>
       <c r="C22" s="4" t="s">
         <v>1769</v>
       </c>
@@ -22799,7 +22817,7 @@
       <c r="A23" s="39">
         <v>21</v>
       </c>
-      <c r="B23" s="238"/>
+      <c r="B23" s="242"/>
       <c r="C23" s="4" t="s">
         <v>1771</v>
       </c>
@@ -22821,7 +22839,7 @@
       <c r="A24" s="39">
         <v>22</v>
       </c>
-      <c r="B24" s="238"/>
+      <c r="B24" s="242"/>
       <c r="C24" s="4" t="s">
         <v>1773</v>
       </c>
@@ -22843,7 +22861,7 @@
       <c r="A25" s="39">
         <v>23</v>
       </c>
-      <c r="B25" s="238"/>
+      <c r="B25" s="242"/>
       <c r="C25" s="4" t="s">
         <v>1775</v>
       </c>
@@ -22865,7 +22883,7 @@
       <c r="A26" s="39">
         <v>24</v>
       </c>
-      <c r="B26" s="237"/>
+      <c r="B26" s="241"/>
       <c r="C26" s="4" t="s">
         <v>1777</v>
       </c>
@@ -22887,7 +22905,7 @@
       <c r="A27" s="39">
         <v>25</v>
       </c>
-      <c r="B27" s="236" t="s">
+      <c r="B27" s="240" t="s">
         <v>548</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -22911,7 +22929,7 @@
       <c r="A28" s="39">
         <v>26</v>
       </c>
-      <c r="B28" s="237"/>
+      <c r="B28" s="241"/>
       <c r="C28" s="4" t="s">
         <v>1781</v>
       </c>
@@ -22933,7 +22951,7 @@
       <c r="A29" s="39">
         <v>27</v>
       </c>
-      <c r="B29" s="236" t="s">
+      <c r="B29" s="240" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -22957,7 +22975,7 @@
       <c r="A30" s="39">
         <v>28</v>
       </c>
-      <c r="B30" s="237"/>
+      <c r="B30" s="241"/>
       <c r="C30" s="4" t="s">
         <v>1785</v>
       </c>
@@ -22979,7 +22997,7 @@
       <c r="A31" s="39">
         <v>29</v>
       </c>
-      <c r="B31" s="236" t="s">
+      <c r="B31" s="240" t="s">
         <v>553</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -23003,7 +23021,7 @@
       <c r="A32" s="39">
         <v>30</v>
       </c>
-      <c r="B32" s="238"/>
+      <c r="B32" s="242"/>
       <c r="C32" s="4" t="s">
         <v>1789</v>
       </c>
@@ -23025,7 +23043,7 @@
       <c r="A33" s="39">
         <v>31</v>
       </c>
-      <c r="B33" s="238"/>
+      <c r="B33" s="242"/>
       <c r="C33" s="4" t="s">
         <v>1791</v>
       </c>
@@ -23047,7 +23065,7 @@
       <c r="A34" s="39">
         <v>32</v>
       </c>
-      <c r="B34" s="238"/>
+      <c r="B34" s="242"/>
       <c r="C34" s="4" t="s">
         <v>1793</v>
       </c>
@@ -23069,7 +23087,7 @@
       <c r="A35" s="39">
         <v>33</v>
       </c>
-      <c r="B35" s="237"/>
+      <c r="B35" s="241"/>
       <c r="C35" s="4" t="s">
         <v>1795</v>
       </c>
@@ -23091,7 +23109,7 @@
       <c r="A36" s="39">
         <v>34</v>
       </c>
-      <c r="B36" s="236" t="s">
+      <c r="B36" s="240" t="s">
         <v>556</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -23115,7 +23133,7 @@
       <c r="A37" s="39">
         <v>35</v>
       </c>
-      <c r="B37" s="238"/>
+      <c r="B37" s="242"/>
       <c r="C37" s="4" t="s">
         <v>1799</v>
       </c>
@@ -23137,7 +23155,7 @@
       <c r="A38" s="39">
         <v>36</v>
       </c>
-      <c r="B38" s="238"/>
+      <c r="B38" s="242"/>
       <c r="C38" s="4" t="s">
         <v>1801</v>
       </c>
@@ -23159,7 +23177,7 @@
       <c r="A39" s="39">
         <v>37</v>
       </c>
-      <c r="B39" s="237"/>
+      <c r="B39" s="241"/>
       <c r="C39" s="4" t="s">
         <v>1803</v>
       </c>
@@ -23181,7 +23199,7 @@
       <c r="A40" s="39">
         <v>38</v>
       </c>
-      <c r="B40" s="236" t="s">
+      <c r="B40" s="240" t="s">
         <v>559</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -23205,7 +23223,7 @@
       <c r="A41" s="39">
         <v>39</v>
       </c>
-      <c r="B41" s="237"/>
+      <c r="B41" s="241"/>
       <c r="C41" s="4" t="s">
         <v>1807</v>
       </c>
@@ -23251,7 +23269,7 @@
       <c r="A43" s="39">
         <v>41</v>
       </c>
-      <c r="B43" s="236" t="s">
+      <c r="B43" s="240" t="s">
         <v>565</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -23275,7 +23293,7 @@
       <c r="A44" s="39">
         <v>42</v>
       </c>
-      <c r="B44" s="238"/>
+      <c r="B44" s="242"/>
       <c r="C44" s="4" t="s">
         <v>1812</v>
       </c>
@@ -23297,7 +23315,7 @@
       <c r="A45" s="39">
         <v>43</v>
       </c>
-      <c r="B45" s="238"/>
+      <c r="B45" s="242"/>
       <c r="C45" s="4" t="s">
         <v>1814</v>
       </c>
@@ -23319,7 +23337,7 @@
       <c r="A46" s="39">
         <v>44</v>
       </c>
-      <c r="B46" s="238"/>
+      <c r="B46" s="242"/>
       <c r="C46" s="4" t="s">
         <v>1816</v>
       </c>
@@ -23343,7 +23361,7 @@
       <c r="A47" s="39">
         <v>45</v>
       </c>
-      <c r="B47" s="238"/>
+      <c r="B47" s="242"/>
       <c r="C47" s="4" t="s">
         <v>1819</v>
       </c>
@@ -23365,7 +23383,7 @@
       <c r="A48" s="39">
         <v>46</v>
       </c>
-      <c r="B48" s="238"/>
+      <c r="B48" s="242"/>
       <c r="C48" s="4" t="s">
         <v>1821</v>
       </c>
@@ -23387,7 +23405,7 @@
       <c r="A49" s="39">
         <v>47</v>
       </c>
-      <c r="B49" s="238"/>
+      <c r="B49" s="242"/>
       <c r="C49" s="4" t="s">
         <v>1823</v>
       </c>
@@ -23409,7 +23427,7 @@
       <c r="A50" s="39">
         <v>48</v>
       </c>
-      <c r="B50" s="238"/>
+      <c r="B50" s="242"/>
       <c r="C50" s="4" t="s">
         <v>1825</v>
       </c>
@@ -23433,7 +23451,7 @@
       <c r="A51" s="39">
         <v>49</v>
       </c>
-      <c r="B51" s="238"/>
+      <c r="B51" s="242"/>
       <c r="C51" s="4" t="s">
         <v>1827</v>
       </c>
@@ -23455,7 +23473,7 @@
       <c r="A52" s="39">
         <v>50</v>
       </c>
-      <c r="B52" s="238"/>
+      <c r="B52" s="242"/>
       <c r="C52" s="4" t="s">
         <v>1829</v>
       </c>
@@ -23477,7 +23495,7 @@
       <c r="A53" s="39">
         <v>51</v>
       </c>
-      <c r="B53" s="238"/>
+      <c r="B53" s="242"/>
       <c r="C53" s="4" t="s">
         <v>1831</v>
       </c>
@@ -23499,7 +23517,7 @@
       <c r="A54" s="39">
         <v>52</v>
       </c>
-      <c r="B54" s="237"/>
+      <c r="B54" s="241"/>
       <c r="C54" s="4" t="s">
         <v>1833</v>
       </c>
@@ -23532,16 +23550,16 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="10">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="B36:B39"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="B43:B54"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B35"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B36:B39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -23582,26 +23600,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="217" t="s">
+      <c r="B2" s="221" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="218"/>
-      <c r="G2" s="218"/>
-      <c r="H2" s="218"/>
-      <c r="I2" s="219"/>
-      <c r="J2" s="218"/>
-      <c r="K2" s="218"/>
-      <c r="L2" s="218"/>
-      <c r="M2" s="218"/>
-      <c r="N2" s="218"/>
-      <c r="O2" s="218"/>
-      <c r="P2" s="218"/>
-      <c r="Q2" s="218"/>
-      <c r="R2" s="218"/>
-      <c r="S2" s="220"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
+      <c r="I2" s="223"/>
+      <c r="J2" s="222"/>
+      <c r="K2" s="222"/>
+      <c r="L2" s="222"/>
+      <c r="M2" s="222"/>
+      <c r="N2" s="222"/>
+      <c r="O2" s="222"/>
+      <c r="P2" s="222"/>
+      <c r="Q2" s="222"/>
+      <c r="R2" s="222"/>
+      <c r="S2" s="224"/>
     </row>
     <row r="3" spans="2:19" ht="70" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
@@ -25603,7 +25621,7 @@
       <c r="R62" s="89"/>
       <c r="S62" s="47"/>
     </row>
-    <row r="63" spans="2:19" ht="168" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:19" ht="154" x14ac:dyDescent="0.35">
       <c r="B63" s="91">
         <v>60</v>
       </c>
@@ -25786,7 +25804,7 @@
       <c r="C68" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="D68" s="216" t="s">
+      <c r="D68" s="220" t="s">
         <v>222</v>
       </c>
       <c r="E68" s="119"/>
@@ -25820,7 +25838,7 @@
       <c r="C69" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="D69" s="216"/>
+      <c r="D69" s="220"/>
       <c r="E69" s="119"/>
       <c r="F69" s="47" t="s">
         <v>225</v>
@@ -27193,7 +27211,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="109" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:19" ht="28" x14ac:dyDescent="0.35">
       <c r="B109" s="91">
         <v>106</v>
       </c>
@@ -27229,7 +27247,7 @@
       <c r="R109" s="89"/>
       <c r="S109" s="47"/>
     </row>
-    <row r="110" spans="2:19" ht="70" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:19" ht="56" x14ac:dyDescent="0.35">
       <c r="B110" s="91">
         <v>107</v>
       </c>
@@ -28005,7 +28023,7 @@
       <c r="R131" s="89"/>
       <c r="S131" s="47"/>
     </row>
-    <row r="132" spans="2:19" ht="154" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:19" ht="140" x14ac:dyDescent="0.35">
       <c r="B132" s="91">
         <v>129</v>
       </c>
@@ -35565,12 +35583,12 @@
       <c r="F1" s="41"/>
     </row>
     <row r="2" spans="2:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="217" t="s">
+      <c r="B2" s="221" t="s">
         <v>885</v>
       </c>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="220"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="224"/>
       <c r="F2" s="41"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
@@ -37135,18 +37153,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="217" t="s">
+      <c r="A1" s="221" t="s">
         <v>907</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="220"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="224"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -37647,7 +37665,7 @@
       <c r="A17" s="36">
         <v>14</v>
       </c>
-      <c r="B17" s="221" t="s">
+      <c r="B17" s="225" t="s">
         <v>143</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -37680,7 +37698,7 @@
       <c r="A18" s="36">
         <v>15</v>
       </c>
-      <c r="B18" s="222"/>
+      <c r="B18" s="226"/>
       <c r="C18" s="4" t="s">
         <v>954</v>
       </c>
@@ -37711,7 +37729,7 @@
       <c r="A19" s="36">
         <v>16</v>
       </c>
-      <c r="B19" s="221" t="s">
+      <c r="B19" s="225" t="s">
         <v>146</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -37744,7 +37762,7 @@
       <c r="A20" s="36">
         <v>17</v>
       </c>
-      <c r="B20" s="222"/>
+      <c r="B20" s="226"/>
       <c r="C20" s="4" t="s">
         <v>960</v>
       </c>
@@ -38029,18 +38047,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="217" t="s">
+      <c r="A1" s="221" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="220"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="224"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -38120,7 +38138,7 @@
       <c r="A4" s="36">
         <v>2</v>
       </c>
-      <c r="B4" s="224" t="s">
+      <c r="B4" s="228" t="s">
         <v>158</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -38151,7 +38169,7 @@
       <c r="A5" s="36">
         <v>3</v>
       </c>
-      <c r="B5" s="225"/>
+      <c r="B5" s="229"/>
       <c r="C5" s="4" t="s">
         <v>974</v>
       </c>
@@ -38256,7 +38274,7 @@
       <c r="A8" s="36">
         <v>6</v>
       </c>
-      <c r="B8" s="224" t="s">
+      <c r="B8" s="228" t="s">
         <v>169</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -38289,7 +38307,7 @@
       <c r="A9" s="36">
         <v>11</v>
       </c>
-      <c r="B9" s="225"/>
+      <c r="B9" s="229"/>
       <c r="C9" s="4" t="s">
         <v>984</v>
       </c>
@@ -38448,7 +38466,7 @@
       <c r="A14" s="36">
         <v>12</v>
       </c>
-      <c r="B14" s="224" t="s">
+      <c r="B14" s="228" t="s">
         <v>182</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -38481,7 +38499,7 @@
       <c r="A15" s="36">
         <v>13</v>
       </c>
-      <c r="B15" s="225"/>
+      <c r="B15" s="229"/>
       <c r="C15" s="4" t="s">
         <v>1000</v>
       </c>
@@ -38734,7 +38752,7 @@
       <c r="A22" s="36">
         <v>20</v>
       </c>
-      <c r="B22" s="224" t="s">
+      <c r="B22" s="228" t="s">
         <v>1009</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -38770,7 +38788,7 @@
       <c r="A23" s="36">
         <v>21</v>
       </c>
-      <c r="B23" s="227"/>
+      <c r="B23" s="231"/>
       <c r="C23" s="4" t="s">
         <v>1013</v>
       </c>
@@ -38803,7 +38821,7 @@
       <c r="A24" s="36">
         <v>22</v>
       </c>
-      <c r="B24" s="225"/>
+      <c r="B24" s="229"/>
       <c r="C24" s="4" t="s">
         <v>1016</v>
       </c>
@@ -39004,7 +39022,7 @@
       <c r="A30" s="36">
         <v>28</v>
       </c>
-      <c r="B30" s="224" t="s">
+      <c r="B30" s="228" t="s">
         <v>222</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -39037,7 +39055,7 @@
       <c r="A31" s="36">
         <v>29</v>
       </c>
-      <c r="B31" s="225"/>
+      <c r="B31" s="229"/>
       <c r="C31" s="4" t="s">
         <v>1029</v>
       </c>
@@ -39068,7 +39086,7 @@
       <c r="A32" s="36">
         <v>30</v>
       </c>
-      <c r="B32" s="224" t="s">
+      <c r="B32" s="228" t="s">
         <v>226</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -39101,7 +39119,7 @@
       <c r="A33" s="36">
         <v>31</v>
       </c>
-      <c r="B33" s="225"/>
+      <c r="B33" s="229"/>
       <c r="C33" s="4" t="s">
         <v>1033</v>
       </c>
@@ -39369,7 +39387,7 @@
       <c r="A41" s="36">
         <v>39</v>
       </c>
-      <c r="B41" s="224" t="s">
+      <c r="B41" s="228" t="s">
         <v>254</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -39402,7 +39420,7 @@
       <c r="A42" s="36">
         <v>40</v>
       </c>
-      <c r="B42" s="225"/>
+      <c r="B42" s="229"/>
       <c r="C42" s="4" t="s">
         <v>1045</v>
       </c>
@@ -39466,7 +39484,7 @@
       <c r="A44" s="36">
         <v>42</v>
       </c>
-      <c r="B44" s="224" t="s">
+      <c r="B44" s="228" t="s">
         <v>260</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -39499,7 +39517,7 @@
       <c r="A45" s="36">
         <v>43</v>
       </c>
-      <c r="B45" s="225"/>
+      <c r="B45" s="229"/>
       <c r="C45" s="4" t="s">
         <v>1052</v>
       </c>
@@ -39618,7 +39636,7 @@
       <c r="I48" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J48" s="226" t="s">
+      <c r="J48" s="230" t="s">
         <v>274</v>
       </c>
       <c r="K48" s="85" t="s">
@@ -39653,7 +39671,7 @@
       <c r="I49" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J49" s="226"/>
+      <c r="J49" s="230"/>
       <c r="K49" s="130" t="s">
         <v>1063</v>
       </c>
@@ -39686,7 +39704,7 @@
       <c r="I50" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J50" s="226"/>
+      <c r="J50" s="230"/>
       <c r="K50" s="130" t="s">
         <v>349</v>
       </c>
@@ -39719,7 +39737,7 @@
       <c r="I51" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J51" s="226"/>
+      <c r="J51" s="230"/>
       <c r="K51" s="130" t="s">
         <v>1070</v>
       </c>
@@ -39752,7 +39770,7 @@
       <c r="I52" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J52" s="226"/>
+      <c r="J52" s="230"/>
       <c r="K52" s="130" t="s">
         <v>1074</v>
       </c>
@@ -39785,7 +39803,7 @@
       <c r="I53" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J53" s="226"/>
+      <c r="J53" s="230"/>
       <c r="K53" s="130" t="s">
         <v>1063</v>
       </c>
@@ -39818,7 +39836,7 @@
       <c r="I54" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J54" s="226"/>
+      <c r="J54" s="230"/>
       <c r="K54" s="130" t="s">
         <v>1063</v>
       </c>
@@ -39851,7 +39869,7 @@
       <c r="I55" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J55" s="226"/>
+      <c r="J55" s="230"/>
       <c r="K55" s="130" t="s">
         <v>1063</v>
       </c>
@@ -39880,7 +39898,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="84"/>
-      <c r="J56" s="226"/>
+      <c r="J56" s="230"/>
       <c r="K56" s="130" t="s">
         <v>1063</v>
       </c>
@@ -39913,7 +39931,7 @@
       <c r="I57" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J57" s="226"/>
+      <c r="J57" s="230"/>
       <c r="K57" s="130" t="s">
         <v>1063</v>
       </c>
@@ -39949,7 +39967,7 @@
       <c r="I58" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J58" s="223" t="s">
+      <c r="J58" s="227" t="s">
         <v>274</v>
       </c>
       <c r="K58" s="130" t="s">
@@ -39984,7 +40002,7 @@
       <c r="I59" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J59" s="223"/>
+      <c r="J59" s="227"/>
       <c r="K59" s="130" t="s">
         <v>1063</v>
       </c>
@@ -40017,7 +40035,7 @@
       <c r="I60" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J60" s="223"/>
+      <c r="J60" s="227"/>
       <c r="K60" s="130" t="s">
         <v>1063</v>
       </c>
@@ -40050,7 +40068,7 @@
       <c r="I61" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J61" s="223"/>
+      <c r="J61" s="227"/>
       <c r="K61" s="134" t="s">
         <v>66</v>
       </c>
@@ -40083,7 +40101,7 @@
       <c r="I62" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J62" s="223"/>
+      <c r="J62" s="227"/>
       <c r="K62" s="130" t="s">
         <v>1063</v>
       </c>
@@ -40116,7 +40134,7 @@
       <c r="I63" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J63" s="223"/>
+      <c r="J63" s="227"/>
       <c r="K63" s="130" t="s">
         <v>1063</v>
       </c>
@@ -40149,7 +40167,7 @@
       <c r="I64" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J64" s="223"/>
+      <c r="J64" s="227"/>
       <c r="K64" s="134" t="s">
         <v>1109</v>
       </c>
@@ -40182,7 +40200,7 @@
       <c r="I65" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J65" s="223"/>
+      <c r="J65" s="227"/>
       <c r="K65" s="130" t="s">
         <v>1063</v>
       </c>
@@ -40211,7 +40229,7 @@
         <v>60</v>
       </c>
       <c r="I66" s="39"/>
-      <c r="J66" s="223"/>
+      <c r="J66" s="227"/>
       <c r="K66" s="130" t="s">
         <v>1063</v>
       </c>
@@ -40240,7 +40258,7 @@
         <v>30</v>
       </c>
       <c r="I67" s="39"/>
-      <c r="J67" s="223"/>
+      <c r="J67" s="227"/>
       <c r="K67" s="134" t="s">
         <v>1119</v>
       </c>
@@ -40276,7 +40294,7 @@
       <c r="I68" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J68" s="223"/>
+      <c r="J68" s="227"/>
       <c r="K68" s="134" t="s">
         <v>1123</v>
       </c>
@@ -40312,7 +40330,7 @@
       <c r="I69" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J69" s="223"/>
+      <c r="J69" s="227"/>
       <c r="K69" s="134" t="s">
         <v>1063</v>
       </c>
@@ -40345,7 +40363,7 @@
       <c r="I70" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J70" s="223"/>
+      <c r="J70" s="227"/>
       <c r="K70" s="134" t="s">
         <v>1063</v>
       </c>
@@ -40378,7 +40396,7 @@
       <c r="I71" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J71" s="223"/>
+      <c r="J71" s="227"/>
       <c r="K71" s="134" t="s">
         <v>1063</v>
       </c>
@@ -40411,7 +40429,7 @@
       <c r="I72" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J72" s="223"/>
+      <c r="J72" s="227"/>
       <c r="K72" s="134" t="s">
         <v>1063</v>
       </c>
@@ -40444,7 +40462,7 @@
       <c r="I73" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J73" s="223"/>
+      <c r="J73" s="227"/>
       <c r="K73" s="134" t="s">
         <v>1063</v>
       </c>
@@ -40475,7 +40493,7 @@
         <v>20</v>
       </c>
       <c r="I74" s="44"/>
-      <c r="J74" s="223"/>
+      <c r="J74" s="227"/>
       <c r="K74" s="134" t="s">
         <v>1063</v>
       </c>
@@ -40492,7 +40510,7 @@
       <c r="G75" s="83"/>
       <c r="H75" s="36"/>
       <c r="I75" s="44"/>
-      <c r="J75" s="223"/>
+      <c r="J75" s="227"/>
       <c r="K75" s="69"/>
     </row>
     <row r="76" spans="1:12" s="2" customFormat="1" ht="39.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -40758,11 +40776,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -40783,18 +40801,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="217" t="s">
+      <c r="A1" s="221" t="s">
         <v>1147</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="220"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="224"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -40865,7 +40883,7 @@
       <c r="J3" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K3" s="239" t="s">
+      <c r="K3" s="217" t="s">
         <v>1942</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -40903,7 +40921,7 @@
       <c r="J4" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K4" s="239" t="s">
+      <c r="K4" s="217" t="s">
         <v>1155</v>
       </c>
       <c r="L4" s="39" t="s">
@@ -40941,7 +40959,7 @@
       <c r="J5" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K5" s="239" t="s">
+      <c r="K5" s="217" t="s">
         <v>1159</v>
       </c>
       <c r="L5" s="39" t="s">
@@ -40979,7 +40997,7 @@
       <c r="J6" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K6" s="239" t="s">
+      <c r="K6" s="217" t="s">
         <v>1163</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -41017,7 +41035,7 @@
       <c r="J7" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K7" s="239" t="s">
+      <c r="K7" s="217" t="s">
         <v>1167</v>
       </c>
       <c r="L7" s="39" t="s">
@@ -41055,7 +41073,7 @@
       <c r="J8" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K8" s="239" t="s">
+      <c r="K8" s="217" t="s">
         <v>1943</v>
       </c>
       <c r="L8" s="39" t="s">
@@ -41093,7 +41111,7 @@
       <c r="J9" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K9" s="239" t="s">
+      <c r="K9" s="217" t="s">
         <v>1173</v>
       </c>
       <c r="L9" s="4" t="s">
@@ -41131,7 +41149,7 @@
       <c r="J10" s="167" t="s">
         <v>1176</v>
       </c>
-      <c r="K10" s="239" t="s">
+      <c r="K10" s="217" t="s">
         <v>1177</v>
       </c>
       <c r="L10" s="39"/>
@@ -41263,7 +41281,7 @@
       <c r="J14" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K14" s="239" t="s">
+      <c r="K14" s="217" t="s">
         <v>1182</v>
       </c>
       <c r="L14" s="39" t="s">
@@ -41301,7 +41319,7 @@
       <c r="J15" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K15" s="240"/>
+      <c r="K15" s="218"/>
       <c r="L15" s="39" t="s">
         <v>1877</v>
       </c>
@@ -41337,7 +41355,7 @@
       <c r="J16" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K16" s="240"/>
+      <c r="K16" s="218"/>
       <c r="L16" s="39" t="s">
         <v>1877</v>
       </c>
@@ -41373,7 +41391,7 @@
       <c r="J17" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K17" s="239" t="s">
+      <c r="K17" s="217" t="s">
         <v>1186</v>
       </c>
       <c r="L17" s="39" t="s">
@@ -41441,7 +41459,7 @@
       <c r="J19" s="164" t="s">
         <v>902</v>
       </c>
-      <c r="K19" s="239" t="s">
+      <c r="K19" s="217" t="s">
         <v>1189</v>
       </c>
       <c r="L19" s="39" t="s">
@@ -41693,7 +41711,7 @@
       <c r="J27" s="164" t="s">
         <v>349</v>
       </c>
-      <c r="K27" s="239" t="s">
+      <c r="K27" s="217" t="s">
         <v>1202</v>
       </c>
       <c r="L27" s="4" t="s">
@@ -41909,7 +41927,7 @@
       </c>
       <c r="I34" s="161"/>
       <c r="J34" s="164"/>
-      <c r="K34" s="239" t="s">
+      <c r="K34" s="217" t="s">
         <v>1220</v>
       </c>
       <c r="L34" s="39" t="s">
@@ -41943,7 +41961,7 @@
       </c>
       <c r="I35" s="164"/>
       <c r="J35" s="164"/>
-      <c r="K35" s="240"/>
+      <c r="K35" s="218"/>
       <c r="L35" s="39" t="s">
         <v>73</v>
       </c>
@@ -41975,7 +41993,7 @@
       </c>
       <c r="I36" s="164"/>
       <c r="J36" s="189"/>
-      <c r="K36" s="241" t="s">
+      <c r="K36" s="219" t="s">
         <v>1223</v>
       </c>
       <c r="L36" s="39" t="s">
@@ -42004,12 +42022,12 @@
       <c r="G37" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="H37" s="162"/>
+      <c r="H37" s="162">
+        <v>3</v>
+      </c>
       <c r="I37" s="161"/>
       <c r="J37" s="164"/>
-      <c r="K37" s="240" t="s">
-        <v>1866</v>
-      </c>
+      <c r="K37" s="218"/>
       <c r="L37" s="39" t="s">
         <v>1880</v>
       </c>
@@ -42041,7 +42059,7 @@
       </c>
       <c r="I38" s="161"/>
       <c r="J38" s="164"/>
-      <c r="K38" s="240" t="s">
+      <c r="K38" s="218" t="s">
         <v>1866</v>
       </c>
       <c r="L38" s="39" t="s">
@@ -42070,9 +42088,13 @@
       <c r="G39" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="36"/>
+      <c r="H39" s="36">
+        <v>0</v>
+      </c>
       <c r="I39" s="41"/>
-      <c r="K39" s="39"/>
+      <c r="K39" s="39" t="s">
+        <v>1945</v>
+      </c>
       <c r="L39" s="39" t="s">
         <v>1880</v>
       </c>
@@ -42099,7 +42121,9 @@
       <c r="G40" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="H40" s="36"/>
+      <c r="H40" s="36">
+        <v>3</v>
+      </c>
       <c r="I40" s="41"/>
       <c r="K40" s="39"/>
       <c r="L40" s="39" t="s">
@@ -42128,15 +42152,45 @@
       <c r="G41" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="36"/>
+      <c r="H41" s="36">
+        <v>3</v>
+      </c>
       <c r="I41" s="41"/>
       <c r="K41" s="39"/>
       <c r="L41" s="39" t="s">
         <v>1880</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="28" x14ac:dyDescent="0.35">
+      <c r="A42" s="36">
+        <v>40</v>
+      </c>
+      <c r="B42" s="216" t="s">
+        <v>1947</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>1946</v>
+      </c>
+      <c r="D42" s="39" t="s">
+        <v>1949</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>1948</v>
+      </c>
+      <c r="F42" s="39" t="s">
+        <v>917</v>
+      </c>
+      <c r="G42" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" s="36">
+        <v>5</v>
+      </c>
       <c r="I42" s="41"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="39" t="s">
+        <v>1880</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="I43" s="41"/>
@@ -42191,18 +42245,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="229" t="s">
+      <c r="A1" s="233" t="s">
         <v>1224</v>
       </c>
-      <c r="B1" s="230"/>
-      <c r="C1" s="230"/>
-      <c r="D1" s="230"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="229"/>
-      <c r="H1" s="231"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="232"/>
+      <c r="B1" s="234"/>
+      <c r="C1" s="234"/>
+      <c r="D1" s="234"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="233"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="236"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -42390,7 +42444,7 @@
       <c r="A7" s="36">
         <v>5</v>
       </c>
-      <c r="B7" s="226" t="s">
+      <c r="B7" s="230" t="s">
         <v>373</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -42426,7 +42480,7 @@
       <c r="A8" s="36">
         <v>6</v>
       </c>
-      <c r="B8" s="233"/>
+      <c r="B8" s="237"/>
       <c r="C8" s="4" t="s">
         <v>1232</v>
       </c>
@@ -42460,7 +42514,7 @@
       <c r="A9" s="36">
         <v>7</v>
       </c>
-      <c r="B9" s="233"/>
+      <c r="B9" s="237"/>
       <c r="C9" s="4" t="s">
         <v>1235</v>
       </c>
@@ -42494,7 +42548,7 @@
       <c r="A10" s="36">
         <v>8</v>
       </c>
-      <c r="B10" s="233"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>1237</v>
       </c>
@@ -42528,7 +42582,7 @@
       <c r="A11" s="36">
         <v>9</v>
       </c>
-      <c r="B11" s="233"/>
+      <c r="B11" s="237"/>
       <c r="C11" s="4" t="s">
         <v>1240</v>
       </c>
@@ -42562,7 +42616,7 @@
       <c r="A12" s="36">
         <v>10</v>
       </c>
-      <c r="B12" s="233"/>
+      <c r="B12" s="237"/>
       <c r="C12" s="4" t="s">
         <v>1243</v>
       </c>
@@ -42596,7 +42650,7 @@
       <c r="A13" s="36">
         <v>11</v>
       </c>
-      <c r="B13" s="233"/>
+      <c r="B13" s="237"/>
       <c r="C13" s="4" t="s">
         <v>1246</v>
       </c>
@@ -42630,7 +42684,7 @@
       <c r="A14" s="36">
         <v>12</v>
       </c>
-      <c r="B14" s="233"/>
+      <c r="B14" s="237"/>
       <c r="C14" s="4" t="s">
         <v>1249</v>
       </c>
@@ -42912,7 +42966,7 @@
       <c r="A22" s="36">
         <v>20</v>
       </c>
-      <c r="B22" s="226" t="s">
+      <c r="B22" s="230" t="s">
         <v>399</v>
       </c>
       <c r="C22" s="22" t="s">
@@ -42948,7 +43002,7 @@
       <c r="A23" s="56">
         <v>21</v>
       </c>
-      <c r="B23" s="234"/>
+      <c r="B23" s="238"/>
       <c r="C23" s="59" t="s">
         <v>1263</v>
       </c>
@@ -42980,7 +43034,7 @@
       <c r="A24" s="36">
         <v>22</v>
       </c>
-      <c r="B24" s="233"/>
+      <c r="B24" s="237"/>
       <c r="C24" s="22" t="s">
         <v>1266</v>
       </c>
@@ -43012,7 +43066,7 @@
       <c r="A25" s="36">
         <v>23</v>
       </c>
-      <c r="B25" s="233"/>
+      <c r="B25" s="237"/>
       <c r="C25" s="22" t="s">
         <v>1269</v>
       </c>
@@ -43044,7 +43098,7 @@
       <c r="A26" s="56">
         <v>24</v>
       </c>
-      <c r="B26" s="234"/>
+      <c r="B26" s="238"/>
       <c r="C26" s="59" t="s">
         <v>1272</v>
       </c>
@@ -43076,7 +43130,7 @@
       <c r="A27" s="36">
         <v>25</v>
       </c>
-      <c r="B27" s="233"/>
+      <c r="B27" s="237"/>
       <c r="C27" s="22" t="s">
         <v>1275</v>
       </c>
@@ -43180,7 +43234,7 @@
       <c r="A30" s="36">
         <v>28</v>
       </c>
-      <c r="B30" s="226" t="s">
+      <c r="B30" s="230" t="s">
         <v>409</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -43216,7 +43270,7 @@
       <c r="A31" s="36">
         <v>29</v>
       </c>
-      <c r="B31" s="233"/>
+      <c r="B31" s="237"/>
       <c r="C31" s="4" t="s">
         <v>1283</v>
       </c>
@@ -43250,7 +43304,7 @@
       <c r="A32" s="36">
         <v>30</v>
       </c>
-      <c r="B32" s="233"/>
+      <c r="B32" s="237"/>
       <c r="C32" s="4" t="s">
         <v>1286</v>
       </c>
@@ -43284,7 +43338,7 @@
       <c r="A33" s="36">
         <v>31</v>
       </c>
-      <c r="B33" s="233"/>
+      <c r="B33" s="237"/>
       <c r="C33" s="4" t="s">
         <v>1289</v>
       </c>
@@ -43504,7 +43558,7 @@
       <c r="A39" s="58">
         <v>37</v>
       </c>
-      <c r="B39" s="227" t="s">
+      <c r="B39" s="231" t="s">
         <v>428</v>
       </c>
       <c r="C39" s="50" t="s">
@@ -43536,7 +43590,7 @@
       <c r="A40" s="36">
         <v>38</v>
       </c>
-      <c r="B40" s="234"/>
+      <c r="B40" s="238"/>
       <c r="C40" s="4" t="s">
         <v>1302</v>
       </c>
@@ -43566,7 +43620,7 @@
       <c r="A41" s="52">
         <v>39</v>
       </c>
-      <c r="B41" s="234"/>
+      <c r="B41" s="238"/>
       <c r="C41" s="51" t="s">
         <v>1305</v>
       </c>
@@ -43594,7 +43648,7 @@
     </row>
     <row r="42" spans="1:12" ht="116.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="36"/>
-      <c r="B42" s="228" t="s">
+      <c r="B42" s="232" t="s">
         <v>1308</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -43630,7 +43684,7 @@
     </row>
     <row r="43" spans="1:12" ht="14.15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="36"/>
-      <c r="B43" s="228"/>
+      <c r="B43" s="232"/>
       <c r="C43" s="4" t="s">
         <v>1312</v>
       </c>
@@ -43658,7 +43712,7 @@
     </row>
     <row r="44" spans="1:12" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="36"/>
-      <c r="B44" s="228"/>
+      <c r="B44" s="232"/>
       <c r="C44" s="4" t="s">
         <v>1315</v>
       </c>
@@ -43686,7 +43740,7 @@
     </row>
     <row r="45" spans="1:12" ht="56" x14ac:dyDescent="0.35">
       <c r="A45" s="36"/>
-      <c r="B45" s="228" t="s">
+      <c r="B45" s="232" t="s">
         <v>435</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -43716,7 +43770,7 @@
     </row>
     <row r="46" spans="1:12" ht="56" x14ac:dyDescent="0.35">
       <c r="A46" s="36"/>
-      <c r="B46" s="228"/>
+      <c r="B46" s="232"/>
       <c r="C46" s="4" t="s">
         <v>1321</v>
       </c>
@@ -44429,7 +44483,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -44451,18 +44505,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="217" t="s">
+      <c r="A1" s="221" t="s">
         <v>1874</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="220"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="224"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -44541,7 +44595,7 @@
       <c r="A4" s="36">
         <v>40</v>
       </c>
-      <c r="B4" s="224" t="s">
+      <c r="B4" s="228" t="s">
         <v>431</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -44575,7 +44629,7 @@
       <c r="A5" s="52">
         <v>41</v>
       </c>
-      <c r="B5" s="227"/>
+      <c r="B5" s="231"/>
       <c r="C5" s="51" t="s">
         <v>1327</v>
       </c>
@@ -44739,18 +44793,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="217" t="s">
+      <c r="A1" s="221" t="s">
         <v>1331</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="235"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="232"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="224"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="224"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="236"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -45363,15 +45417,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -45578,6 +45623,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -45605,14 +45659,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7F7E23-FE37-4AB8-A4B3-5025B5D9E450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -45627,6 +45673,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
backlog for PRG updated
</commit_message>
<xml_diff>
--- a/_files/requirements/Pending_Backlog_Stories_25Jun19_Updated.xlsx
+++ b/_files/requirements/Pending_Backlog_Stories_25Jun19_Updated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP wiki Open Source\Requirements\_files\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\git-repo\mosip.docs\mosip-docs.wiki\_files\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{52DB2795-C269-45D6-A8BB-B93CD2414096}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BD0D1685-9BA0-454A-AD9B-6FB2D5330F9E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId13"/>
+    <pivotCache cacheId="3" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -8117,6 +8117,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -8185,9 +8188,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -15337,7 +15337,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:D32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -15880,7 +15880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16255,18 +16255,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>1333</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="234"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="236"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -16716,7 +16716,7 @@
       <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="237" t="s">
+      <c r="B17" s="238" t="s">
         <v>503</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -16748,7 +16748,7 @@
       <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="238"/>
+      <c r="B18" s="239"/>
       <c r="C18" s="4" t="s">
         <v>1352</v>
       </c>
@@ -17088,19 +17088,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>1357</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="234"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="234"/>
-      <c r="K1" s="236"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="235"/>
+      <c r="K1" s="237"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="145" t="s">
@@ -22442,18 +22442,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>1722</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="234"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="236"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
@@ -22491,7 +22491,7 @@
       <c r="A3" s="39">
         <v>1</v>
       </c>
-      <c r="B3" s="252" t="s">
+      <c r="B3" s="253" t="s">
         <v>527</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -22517,7 +22517,7 @@
       <c r="A4" s="39">
         <v>2</v>
       </c>
-      <c r="B4" s="253"/>
+      <c r="B4" s="254"/>
       <c r="C4" s="4" t="s">
         <v>1726</v>
       </c>
@@ -22539,7 +22539,7 @@
       <c r="A5" s="39">
         <v>3</v>
       </c>
-      <c r="B5" s="252" t="s">
+      <c r="B5" s="253" t="s">
         <v>530</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -22565,7 +22565,7 @@
       <c r="A6" s="39">
         <v>4</v>
       </c>
-      <c r="B6" s="254"/>
+      <c r="B6" s="255"/>
       <c r="C6" s="19" t="s">
         <v>1731</v>
       </c>
@@ -22589,7 +22589,7 @@
       <c r="A7" s="39">
         <v>5</v>
       </c>
-      <c r="B7" s="254"/>
+      <c r="B7" s="255"/>
       <c r="C7" s="19" t="s">
         <v>1734</v>
       </c>
@@ -22611,7 +22611,7 @@
       <c r="A8" s="39">
         <v>6</v>
       </c>
-      <c r="B8" s="254"/>
+      <c r="B8" s="255"/>
       <c r="C8" s="19" t="s">
         <v>1736</v>
       </c>
@@ -22633,7 +22633,7 @@
       <c r="A9" s="39">
         <v>7</v>
       </c>
-      <c r="B9" s="254"/>
+      <c r="B9" s="255"/>
       <c r="C9" s="19" t="s">
         <v>1738</v>
       </c>
@@ -22655,7 +22655,7 @@
       <c r="A10" s="39">
         <v>8</v>
       </c>
-      <c r="B10" s="254"/>
+      <c r="B10" s="255"/>
       <c r="C10" s="19" t="s">
         <v>1740</v>
       </c>
@@ -22677,7 +22677,7 @@
       <c r="A11" s="39">
         <v>9</v>
       </c>
-      <c r="B11" s="254"/>
+      <c r="B11" s="255"/>
       <c r="C11" s="19" t="s">
         <v>1742</v>
       </c>
@@ -22699,7 +22699,7 @@
       <c r="A12" s="39">
         <v>10</v>
       </c>
-      <c r="B12" s="254"/>
+      <c r="B12" s="255"/>
       <c r="C12" s="19" t="s">
         <v>1744</v>
       </c>
@@ -22721,7 +22721,7 @@
       <c r="A13" s="39">
         <v>11</v>
       </c>
-      <c r="B13" s="254"/>
+      <c r="B13" s="255"/>
       <c r="C13" s="19" t="s">
         <v>1746</v>
       </c>
@@ -22743,7 +22743,7 @@
       <c r="A14" s="39">
         <v>12</v>
       </c>
-      <c r="B14" s="254"/>
+      <c r="B14" s="255"/>
       <c r="C14" s="19" t="s">
         <v>1748</v>
       </c>
@@ -22767,7 +22767,7 @@
       <c r="A15" s="39">
         <v>13</v>
       </c>
-      <c r="B15" s="254"/>
+      <c r="B15" s="255"/>
       <c r="C15" s="19" t="s">
         <v>1751</v>
       </c>
@@ -22791,7 +22791,7 @@
       <c r="A16" s="39">
         <v>14</v>
       </c>
-      <c r="B16" s="253"/>
+      <c r="B16" s="254"/>
       <c r="C16" s="19" t="s">
         <v>1753</v>
       </c>
@@ -22913,7 +22913,7 @@
       <c r="A21" s="39">
         <v>19</v>
       </c>
-      <c r="B21" s="252" t="s">
+      <c r="B21" s="253" t="s">
         <v>545</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -22937,7 +22937,7 @@
       <c r="A22" s="39">
         <v>20</v>
       </c>
-      <c r="B22" s="254"/>
+      <c r="B22" s="255"/>
       <c r="C22" s="4" t="s">
         <v>1761</v>
       </c>
@@ -22959,7 +22959,7 @@
       <c r="A23" s="39">
         <v>21</v>
       </c>
-      <c r="B23" s="254"/>
+      <c r="B23" s="255"/>
       <c r="C23" s="4" t="s">
         <v>1763</v>
       </c>
@@ -22981,7 +22981,7 @@
       <c r="A24" s="39">
         <v>22</v>
       </c>
-      <c r="B24" s="254"/>
+      <c r="B24" s="255"/>
       <c r="C24" s="4" t="s">
         <v>1765</v>
       </c>
@@ -23003,7 +23003,7 @@
       <c r="A25" s="39">
         <v>23</v>
       </c>
-      <c r="B25" s="254"/>
+      <c r="B25" s="255"/>
       <c r="C25" s="4" t="s">
         <v>1767</v>
       </c>
@@ -23025,7 +23025,7 @@
       <c r="A26" s="39">
         <v>24</v>
       </c>
-      <c r="B26" s="253"/>
+      <c r="B26" s="254"/>
       <c r="C26" s="4" t="s">
         <v>1769</v>
       </c>
@@ -23047,7 +23047,7 @@
       <c r="A27" s="39">
         <v>25</v>
       </c>
-      <c r="B27" s="252" t="s">
+      <c r="B27" s="253" t="s">
         <v>548</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -23071,7 +23071,7 @@
       <c r="A28" s="39">
         <v>26</v>
       </c>
-      <c r="B28" s="253"/>
+      <c r="B28" s="254"/>
       <c r="C28" s="4" t="s">
         <v>1773</v>
       </c>
@@ -23093,7 +23093,7 @@
       <c r="A29" s="39">
         <v>27</v>
       </c>
-      <c r="B29" s="252" t="s">
+      <c r="B29" s="253" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -23117,7 +23117,7 @@
       <c r="A30" s="39">
         <v>28</v>
       </c>
-      <c r="B30" s="253"/>
+      <c r="B30" s="254"/>
       <c r="C30" s="4" t="s">
         <v>1777</v>
       </c>
@@ -23139,7 +23139,7 @@
       <c r="A31" s="39">
         <v>29</v>
       </c>
-      <c r="B31" s="252" t="s">
+      <c r="B31" s="253" t="s">
         <v>553</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -23163,7 +23163,7 @@
       <c r="A32" s="39">
         <v>30</v>
       </c>
-      <c r="B32" s="254"/>
+      <c r="B32" s="255"/>
       <c r="C32" s="4" t="s">
         <v>1781</v>
       </c>
@@ -23185,7 +23185,7 @@
       <c r="A33" s="39">
         <v>31</v>
       </c>
-      <c r="B33" s="254"/>
+      <c r="B33" s="255"/>
       <c r="C33" s="4" t="s">
         <v>1783</v>
       </c>
@@ -23207,7 +23207,7 @@
       <c r="A34" s="39">
         <v>32</v>
       </c>
-      <c r="B34" s="254"/>
+      <c r="B34" s="255"/>
       <c r="C34" s="4" t="s">
         <v>1785</v>
       </c>
@@ -23229,7 +23229,7 @@
       <c r="A35" s="39">
         <v>33</v>
       </c>
-      <c r="B35" s="253"/>
+      <c r="B35" s="254"/>
       <c r="C35" s="4" t="s">
         <v>1787</v>
       </c>
@@ -23251,7 +23251,7 @@
       <c r="A36" s="39">
         <v>34</v>
       </c>
-      <c r="B36" s="252" t="s">
+      <c r="B36" s="253" t="s">
         <v>556</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -23275,7 +23275,7 @@
       <c r="A37" s="39">
         <v>35</v>
       </c>
-      <c r="B37" s="254"/>
+      <c r="B37" s="255"/>
       <c r="C37" s="4" t="s">
         <v>1791</v>
       </c>
@@ -23297,7 +23297,7 @@
       <c r="A38" s="39">
         <v>36</v>
       </c>
-      <c r="B38" s="254"/>
+      <c r="B38" s="255"/>
       <c r="C38" s="4" t="s">
         <v>1793</v>
       </c>
@@ -23319,7 +23319,7 @@
       <c r="A39" s="39">
         <v>37</v>
       </c>
-      <c r="B39" s="253"/>
+      <c r="B39" s="254"/>
       <c r="C39" s="4" t="s">
         <v>1795</v>
       </c>
@@ -23341,7 +23341,7 @@
       <c r="A40" s="39">
         <v>38</v>
       </c>
-      <c r="B40" s="252" t="s">
+      <c r="B40" s="253" t="s">
         <v>559</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -23365,7 +23365,7 @@
       <c r="A41" s="39">
         <v>39</v>
       </c>
-      <c r="B41" s="253"/>
+      <c r="B41" s="254"/>
       <c r="C41" s="4" t="s">
         <v>1799</v>
       </c>
@@ -23411,7 +23411,7 @@
       <c r="A43" s="39">
         <v>41</v>
       </c>
-      <c r="B43" s="252" t="s">
+      <c r="B43" s="253" t="s">
         <v>565</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -23435,7 +23435,7 @@
       <c r="A44" s="39">
         <v>42</v>
       </c>
-      <c r="B44" s="254"/>
+      <c r="B44" s="255"/>
       <c r="C44" s="4" t="s">
         <v>1804</v>
       </c>
@@ -23457,7 +23457,7 @@
       <c r="A45" s="39">
         <v>43</v>
       </c>
-      <c r="B45" s="254"/>
+      <c r="B45" s="255"/>
       <c r="C45" s="4" t="s">
         <v>1806</v>
       </c>
@@ -23479,7 +23479,7 @@
       <c r="A46" s="39">
         <v>44</v>
       </c>
-      <c r="B46" s="254"/>
+      <c r="B46" s="255"/>
       <c r="C46" s="4" t="s">
         <v>1808</v>
       </c>
@@ -23503,7 +23503,7 @@
       <c r="A47" s="39">
         <v>45</v>
       </c>
-      <c r="B47" s="254"/>
+      <c r="B47" s="255"/>
       <c r="C47" s="4" t="s">
         <v>1811</v>
       </c>
@@ -23525,7 +23525,7 @@
       <c r="A48" s="39">
         <v>46</v>
       </c>
-      <c r="B48" s="254"/>
+      <c r="B48" s="255"/>
       <c r="C48" s="4" t="s">
         <v>1813</v>
       </c>
@@ -23547,7 +23547,7 @@
       <c r="A49" s="39">
         <v>47</v>
       </c>
-      <c r="B49" s="254"/>
+      <c r="B49" s="255"/>
       <c r="C49" s="4" t="s">
         <v>1815</v>
       </c>
@@ -23569,7 +23569,7 @@
       <c r="A50" s="39">
         <v>48</v>
       </c>
-      <c r="B50" s="254"/>
+      <c r="B50" s="255"/>
       <c r="C50" s="4" t="s">
         <v>1817</v>
       </c>
@@ -23593,7 +23593,7 @@
       <c r="A51" s="39">
         <v>49</v>
       </c>
-      <c r="B51" s="254"/>
+      <c r="B51" s="255"/>
       <c r="C51" s="4" t="s">
         <v>1819</v>
       </c>
@@ -23615,7 +23615,7 @@
       <c r="A52" s="39">
         <v>50</v>
       </c>
-      <c r="B52" s="254"/>
+      <c r="B52" s="255"/>
       <c r="C52" s="4" t="s">
         <v>1821</v>
       </c>
@@ -23637,7 +23637,7 @@
       <c r="A53" s="39">
         <v>51</v>
       </c>
-      <c r="B53" s="254"/>
+      <c r="B53" s="255"/>
       <c r="C53" s="4" t="s">
         <v>1823</v>
       </c>
@@ -23659,7 +23659,7 @@
       <c r="A54" s="39">
         <v>52</v>
       </c>
-      <c r="B54" s="253"/>
+      <c r="B54" s="254"/>
       <c r="C54" s="4" t="s">
         <v>1825</v>
       </c>
@@ -23692,16 +23692,16 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="10">
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B43:B54"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B35"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B16"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B43:B54"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -23742,26 +23742,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="233" t="s">
+      <c r="B2" s="234" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="234"/>
-      <c r="D2" s="234"/>
-      <c r="E2" s="234"/>
-      <c r="F2" s="234"/>
-      <c r="G2" s="234"/>
-      <c r="H2" s="234"/>
-      <c r="I2" s="235"/>
-      <c r="J2" s="234"/>
-      <c r="K2" s="234"/>
-      <c r="L2" s="234"/>
-      <c r="M2" s="234"/>
-      <c r="N2" s="234"/>
-      <c r="O2" s="234"/>
-      <c r="P2" s="234"/>
-      <c r="Q2" s="234"/>
-      <c r="R2" s="234"/>
-      <c r="S2" s="236"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="235"/>
+      <c r="G2" s="235"/>
+      <c r="H2" s="235"/>
+      <c r="I2" s="236"/>
+      <c r="J2" s="235"/>
+      <c r="K2" s="235"/>
+      <c r="L2" s="235"/>
+      <c r="M2" s="235"/>
+      <c r="N2" s="235"/>
+      <c r="O2" s="235"/>
+      <c r="P2" s="235"/>
+      <c r="Q2" s="235"/>
+      <c r="R2" s="235"/>
+      <c r="S2" s="237"/>
     </row>
     <row r="3" spans="2:19" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -25946,7 +25946,7 @@
       <c r="C68" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="D68" s="232" t="s">
+      <c r="D68" s="233" t="s">
         <v>222</v>
       </c>
       <c r="E68" s="118"/>
@@ -25980,7 +25980,7 @@
       <c r="C69" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="D69" s="232"/>
+      <c r="D69" s="233"/>
       <c r="E69" s="118"/>
       <c r="F69" s="47" t="s">
         <v>225</v>
@@ -26833,7 +26833,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="94" spans="2:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:19" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B94" s="91">
         <v>91</v>
       </c>
@@ -27805,7 +27805,7 @@
       <c r="R121" s="89"/>
       <c r="S121" s="47"/>
     </row>
-    <row r="122" spans="2:19" ht="114" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:19" ht="99.75" x14ac:dyDescent="0.25">
       <c r="B122" s="91">
         <v>119</v>
       </c>
@@ -28097,7 +28097,7 @@
       <c r="R129" s="89"/>
       <c r="S129" s="47"/>
     </row>
-    <row r="130" spans="2:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:19" ht="57" x14ac:dyDescent="0.25">
       <c r="B130" s="91">
         <v>127</v>
       </c>
@@ -28275,7 +28275,7 @@
       <c r="R134" s="89"/>
       <c r="S134" s="47"/>
     </row>
-    <row r="135" spans="2:19" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:19" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B135" s="91">
         <v>132</v>
       </c>
@@ -28489,7 +28489,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="141" spans="2:19" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:19" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B141" s="91">
         <v>138</v>
       </c>
@@ -28743,7 +28743,7 @@
       <c r="R147" s="89"/>
       <c r="S147" s="47"/>
     </row>
-    <row r="148" spans="2:19" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:19" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B148" s="91">
         <v>145</v>
       </c>
@@ -29067,7 +29067,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="157" spans="2:19" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:19" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B157" s="91">
         <v>154</v>
       </c>
@@ -33305,7 +33305,7 @@
       <c r="T281" s="53"/>
       <c r="U281" s="4"/>
     </row>
-    <row r="282" spans="2:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B282" s="91">
         <v>279</v>
       </c>
@@ -35725,12 +35725,12 @@
       <c r="F1" s="41"/>
     </row>
     <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="233" t="s">
+      <c r="B2" s="234" t="s">
         <v>885</v>
       </c>
-      <c r="C2" s="234"/>
-      <c r="D2" s="234"/>
-      <c r="E2" s="236"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="237"/>
       <c r="F2" s="41"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -37272,7 +37272,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" sqref="A1:J1"/>
@@ -37281,7 +37281,7 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="40"/>
-    <col min="2" max="2" width="33.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="11" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="41" customWidth="1"/>
     <col min="5" max="5" width="38.140625" style="5" customWidth="1"/>
@@ -37290,7 +37290,7 @@
     <col min="8" max="8" width="20.85546875" style="40" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" style="2" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="29.28515625" style="5" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="41" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="41" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="41"/>
     <col min="13" max="13" width="23.7109375" style="41" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.85546875" style="41" customWidth="1"/>
@@ -37298,18 +37298,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>907</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="234"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="236"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -37518,7 +37518,7 @@
       <c r="J7" s="4" t="s">
         <v>923</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="51" t="s">
         <v>349</v>
       </c>
     </row>
@@ -37544,19 +37544,19 @@
         <v>25</v>
       </c>
       <c r="I8" s="53"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="4"/>
       <c r="L8" s="39" t="s">
         <v>1872</v>
       </c>
       <c r="M8" s="39" t="s">
         <v>1942</v>
       </c>
-      <c r="N8" s="41" t="s">
+      <c r="N8" s="39" t="s">
         <v>1970</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="58">
         <v>6</v>
       </c>
@@ -37584,18 +37584,19 @@
       <c r="I9" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="87"/>
       <c r="K9" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="L9" s="41" t="s">
+      <c r="L9" s="39" t="s">
         <v>1869</v>
       </c>
-      <c r="M9" s="41" t="s">
+      <c r="M9" s="39" t="s">
         <v>1965</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="39"/>
+    </row>
+    <row r="10" spans="1:14" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A10" s="36">
         <v>7</v>
       </c>
@@ -37623,18 +37624,19 @@
       <c r="I10" s="39" t="s">
         <v>933</v>
       </c>
-      <c r="J10" s="4"/>
+      <c r="J10" s="87"/>
       <c r="K10" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="L10" s="41" t="s">
+      <c r="L10" s="39" t="s">
         <v>1869</v>
       </c>
-      <c r="M10" s="41" t="s">
+      <c r="M10" s="39" t="s">
         <v>1965</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" s="2" customFormat="1" ht="185.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N10" s="39"/>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" ht="171" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36">
         <v>8</v>
       </c>
@@ -37828,7 +37830,7 @@
       <c r="A17" s="36">
         <v>14</v>
       </c>
-      <c r="B17" s="237" t="s">
+      <c r="B17" s="238" t="s">
         <v>143</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -37861,7 +37863,7 @@
       <c r="A18" s="36">
         <v>15</v>
       </c>
-      <c r="B18" s="238"/>
+      <c r="B18" s="239"/>
       <c r="C18" s="4" t="s">
         <v>954</v>
       </c>
@@ -37892,7 +37894,7 @@
       <c r="A19" s="36">
         <v>16</v>
       </c>
-      <c r="B19" s="237" t="s">
+      <c r="B19" s="238" t="s">
         <v>146</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -37925,7 +37927,7 @@
       <c r="A20" s="36">
         <v>17</v>
       </c>
-      <c r="B20" s="238"/>
+      <c r="B20" s="239"/>
       <c r="C20" s="4" t="s">
         <v>960</v>
       </c>
@@ -37952,7 +37954,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A21" s="36">
         <v>18</v>
       </c>
@@ -37980,18 +37982,19 @@
       <c r="I21" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="87" t="s">
         <v>964</v>
       </c>
       <c r="K21" s="39" t="s">
         <v>349</v>
       </c>
-      <c r="L21" s="41" t="s">
+      <c r="L21" s="39" t="s">
         <v>1869</v>
       </c>
-      <c r="M21" s="41" t="s">
+      <c r="M21" s="39" t="s">
         <v>1944</v>
       </c>
+      <c r="N21" s="39"/>
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36">
@@ -38048,13 +38051,14 @@
         <v>8</v>
       </c>
       <c r="I23" s="41"/>
+      <c r="K23" s="39"/>
       <c r="L23" s="39" t="s">
         <v>1872</v>
       </c>
       <c r="M23" s="39" t="s">
         <v>1942</v>
       </c>
-      <c r="N23" s="41" t="s">
+      <c r="N23" s="39" t="s">
         <v>1970</v>
       </c>
     </row>
@@ -38192,11 +38196,6 @@
       <filters>
         <filter val="Vital"/>
         <filter val="Vital?"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="11">
-      <filters>
-        <filter val="P1"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -38216,7 +38215,7 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
@@ -38241,18 +38240,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="234"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="236"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -38344,7 +38343,7 @@
       <c r="A4" s="36">
         <v>2</v>
       </c>
-      <c r="B4" s="240" t="s">
+      <c r="B4" s="241" t="s">
         <v>158</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -38375,7 +38374,7 @@
       <c r="A5" s="36">
         <v>3</v>
       </c>
-      <c r="B5" s="241"/>
+      <c r="B5" s="242"/>
       <c r="C5" s="4" t="s">
         <v>974</v>
       </c>
@@ -38480,7 +38479,7 @@
       <c r="A8" s="36">
         <v>6</v>
       </c>
-      <c r="B8" s="240" t="s">
+      <c r="B8" s="241" t="s">
         <v>169</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -38513,7 +38512,7 @@
       <c r="A9" s="36">
         <v>11</v>
       </c>
-      <c r="B9" s="241"/>
+      <c r="B9" s="242"/>
       <c r="C9" s="4" t="s">
         <v>984</v>
       </c>
@@ -38672,7 +38671,7 @@
       <c r="A14" s="36">
         <v>12</v>
       </c>
-      <c r="B14" s="240" t="s">
+      <c r="B14" s="241" t="s">
         <v>182</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -38705,7 +38704,7 @@
       <c r="A15" s="36">
         <v>13</v>
       </c>
-      <c r="B15" s="241"/>
+      <c r="B15" s="242"/>
       <c r="C15" s="4" t="s">
         <v>1000</v>
       </c>
@@ -38958,7 +38957,7 @@
       <c r="A22" s="36">
         <v>20</v>
       </c>
-      <c r="B22" s="240" t="s">
+      <c r="B22" s="241" t="s">
         <v>1009</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -38994,7 +38993,7 @@
       <c r="A23" s="36">
         <v>21</v>
       </c>
-      <c r="B23" s="243"/>
+      <c r="B23" s="244"/>
       <c r="C23" s="4" t="s">
         <v>1013</v>
       </c>
@@ -39027,7 +39026,7 @@
       <c r="A24" s="36">
         <v>22</v>
       </c>
-      <c r="B24" s="241"/>
+      <c r="B24" s="242"/>
       <c r="C24" s="4" t="s">
         <v>1016</v>
       </c>
@@ -39228,7 +39227,7 @@
       <c r="A30" s="36">
         <v>28</v>
       </c>
-      <c r="B30" s="240" t="s">
+      <c r="B30" s="241" t="s">
         <v>222</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -39261,7 +39260,7 @@
       <c r="A31" s="36">
         <v>29</v>
       </c>
-      <c r="B31" s="241"/>
+      <c r="B31" s="242"/>
       <c r="C31" s="4" t="s">
         <v>1029</v>
       </c>
@@ -39292,7 +39291,7 @@
       <c r="A32" s="36">
         <v>30</v>
       </c>
-      <c r="B32" s="240" t="s">
+      <c r="B32" s="241" t="s">
         <v>226</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -39325,7 +39324,7 @@
       <c r="A33" s="36">
         <v>31</v>
       </c>
-      <c r="B33" s="241"/>
+      <c r="B33" s="242"/>
       <c r="C33" s="4" t="s">
         <v>1033</v>
       </c>
@@ -39599,7 +39598,7 @@
       <c r="A41" s="36">
         <v>39</v>
       </c>
-      <c r="B41" s="240" t="s">
+      <c r="B41" s="241" t="s">
         <v>254</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -39632,7 +39631,7 @@
       <c r="A42" s="36">
         <v>40</v>
       </c>
-      <c r="B42" s="241"/>
+      <c r="B42" s="242"/>
       <c r="C42" s="4" t="s">
         <v>1045</v>
       </c>
@@ -39696,7 +39695,7 @@
       <c r="A44" s="36">
         <v>42</v>
       </c>
-      <c r="B44" s="240" t="s">
+      <c r="B44" s="241" t="s">
         <v>260</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -39729,7 +39728,7 @@
       <c r="A45" s="36">
         <v>43</v>
       </c>
-      <c r="B45" s="241"/>
+      <c r="B45" s="242"/>
       <c r="C45" s="4" t="s">
         <v>1052</v>
       </c>
@@ -39848,7 +39847,7 @@
       <c r="I48" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J48" s="242" t="s">
+      <c r="J48" s="243" t="s">
         <v>274</v>
       </c>
       <c r="K48" s="85" t="s">
@@ -39883,7 +39882,7 @@
       <c r="I49" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J49" s="242"/>
+      <c r="J49" s="243"/>
       <c r="K49" s="129" t="s">
         <v>1063</v>
       </c>
@@ -39916,7 +39915,7 @@
       <c r="I50" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J50" s="242"/>
+      <c r="J50" s="243"/>
       <c r="K50" s="129" t="s">
         <v>349</v>
       </c>
@@ -39949,7 +39948,7 @@
       <c r="I51" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J51" s="242"/>
+      <c r="J51" s="243"/>
       <c r="K51" s="129" t="s">
         <v>1070</v>
       </c>
@@ -39982,7 +39981,7 @@
       <c r="I52" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J52" s="242"/>
+      <c r="J52" s="243"/>
       <c r="K52" s="129" t="s">
         <v>1074</v>
       </c>
@@ -40015,7 +40014,7 @@
       <c r="I53" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J53" s="242"/>
+      <c r="J53" s="243"/>
       <c r="K53" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40048,7 +40047,7 @@
       <c r="I54" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J54" s="242"/>
+      <c r="J54" s="243"/>
       <c r="K54" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40081,7 +40080,7 @@
       <c r="I55" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J55" s="242"/>
+      <c r="J55" s="243"/>
       <c r="K55" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40110,7 +40109,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="84"/>
-      <c r="J56" s="242"/>
+      <c r="J56" s="243"/>
       <c r="K56" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40143,7 +40142,7 @@
       <c r="I57" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J57" s="242"/>
+      <c r="J57" s="243"/>
       <c r="K57" s="220" t="s">
         <v>1063</v>
       </c>
@@ -40185,7 +40184,7 @@
       <c r="I58" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J58" s="239" t="s">
+      <c r="J58" s="240" t="s">
         <v>274</v>
       </c>
       <c r="K58" s="129" t="s">
@@ -40220,7 +40219,7 @@
       <c r="I59" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J59" s="239"/>
+      <c r="J59" s="240"/>
       <c r="K59" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40253,7 +40252,7 @@
       <c r="I60" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J60" s="239"/>
+      <c r="J60" s="240"/>
       <c r="K60" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40286,7 +40285,7 @@
       <c r="I61" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J61" s="239"/>
+      <c r="J61" s="240"/>
       <c r="K61" s="133" t="s">
         <v>66</v>
       </c>
@@ -40319,7 +40318,7 @@
       <c r="I62" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J62" s="239"/>
+      <c r="J62" s="240"/>
       <c r="K62" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40352,7 +40351,7 @@
       <c r="I63" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J63" s="239"/>
+      <c r="J63" s="240"/>
       <c r="K63" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40385,7 +40384,7 @@
       <c r="I64" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J64" s="239"/>
+      <c r="J64" s="240"/>
       <c r="K64" s="133" t="s">
         <v>1109</v>
       </c>
@@ -40418,7 +40417,7 @@
       <c r="I65" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J65" s="239"/>
+      <c r="J65" s="240"/>
       <c r="K65" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40447,7 +40446,7 @@
         <v>60</v>
       </c>
       <c r="I66" s="39"/>
-      <c r="J66" s="239"/>
+      <c r="J66" s="240"/>
       <c r="K66" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40476,7 +40475,7 @@
         <v>30</v>
       </c>
       <c r="I67" s="39"/>
-      <c r="J67" s="239"/>
+      <c r="J67" s="240"/>
       <c r="K67" s="221" t="s">
         <v>1119</v>
       </c>
@@ -40518,7 +40517,7 @@
       <c r="I68" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J68" s="239"/>
+      <c r="J68" s="240"/>
       <c r="K68" s="133" t="s">
         <v>1123</v>
       </c>
@@ -40554,7 +40553,7 @@
       <c r="I69" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J69" s="239"/>
+      <c r="J69" s="240"/>
       <c r="K69" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40587,7 +40586,7 @@
       <c r="I70" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J70" s="239"/>
+      <c r="J70" s="240"/>
       <c r="K70" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40620,7 +40619,7 @@
       <c r="I71" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J71" s="239"/>
+      <c r="J71" s="240"/>
       <c r="K71" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40653,7 +40652,7 @@
       <c r="I72" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J72" s="239"/>
+      <c r="J72" s="240"/>
       <c r="K72" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40686,7 +40685,7 @@
       <c r="I73" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J73" s="239"/>
+      <c r="J73" s="240"/>
       <c r="K73" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40717,7 +40716,7 @@
         <v>20</v>
       </c>
       <c r="I74" s="44"/>
-      <c r="J74" s="239"/>
+      <c r="J74" s="240"/>
       <c r="K74" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40734,7 +40733,7 @@
       <c r="G75" s="83"/>
       <c r="H75" s="36"/>
       <c r="I75" s="44"/>
-      <c r="J75" s="239"/>
+      <c r="J75" s="240"/>
       <c r="K75" s="69"/>
     </row>
     <row r="76" spans="1:14" s="2" customFormat="1" ht="39.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -41034,8 +41033,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="D37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N42"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -41058,18 +41057,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>1147</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="234"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="236"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -42596,11 +42595,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N259"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
+      <selection pane="bottomRight" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -42622,18 +42621,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="246" t="s">
         <v>1223</v>
       </c>
-      <c r="B1" s="246"/>
-      <c r="C1" s="246"/>
-      <c r="D1" s="246"/>
-      <c r="E1" s="247"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="247"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="248"/>
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="247"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="248"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="249"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -42840,7 +42839,7 @@
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
-      <c r="B7" s="240" t="s">
+      <c r="B7" s="241" t="s">
         <v>373</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -42876,7 +42875,7 @@
     </row>
     <row r="8" spans="1:14" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
-      <c r="B8" s="243"/>
+      <c r="B8" s="244"/>
       <c r="C8" s="4" t="s">
         <v>1969</v>
       </c>
@@ -42912,7 +42911,7 @@
       <c r="A9" s="36">
         <v>5</v>
       </c>
-      <c r="B9" s="243"/>
+      <c r="B9" s="244"/>
       <c r="C9" s="4" t="s">
         <v>1948</v>
       </c>
@@ -42949,7 +42948,7 @@
       <c r="A10" s="36">
         <v>6</v>
       </c>
-      <c r="B10" s="243"/>
+      <c r="B10" s="244"/>
       <c r="C10" s="4" t="s">
         <v>1230</v>
       </c>
@@ -42983,7 +42982,7 @@
       <c r="A11" s="36">
         <v>7</v>
       </c>
-      <c r="B11" s="243"/>
+      <c r="B11" s="244"/>
       <c r="C11" s="4" t="s">
         <v>1233</v>
       </c>
@@ -43017,7 +43016,7 @@
       <c r="A12" s="36">
         <v>8</v>
       </c>
-      <c r="B12" s="243"/>
+      <c r="B12" s="244"/>
       <c r="C12" s="4" t="s">
         <v>1949</v>
       </c>
@@ -43054,7 +43053,7 @@
       <c r="A13" s="36">
         <v>9</v>
       </c>
-      <c r="B13" s="243"/>
+      <c r="B13" s="244"/>
       <c r="C13" s="4" t="s">
         <v>1950</v>
       </c>
@@ -43091,7 +43090,7 @@
       <c r="A14" s="36">
         <v>10</v>
       </c>
-      <c r="B14" s="243"/>
+      <c r="B14" s="244"/>
       <c r="C14" s="4" t="s">
         <v>1951</v>
       </c>
@@ -43128,7 +43127,7 @@
       <c r="A15" s="36">
         <v>11</v>
       </c>
-      <c r="B15" s="243"/>
+      <c r="B15" s="244"/>
       <c r="C15" s="4" t="s">
         <v>1952</v>
       </c>
@@ -43165,7 +43164,7 @@
       <c r="A16" s="36">
         <v>12</v>
       </c>
-      <c r="B16" s="241"/>
+      <c r="B16" s="242"/>
       <c r="C16" s="4" t="s">
         <v>1953</v>
       </c>
@@ -43453,7 +43452,7 @@
       <c r="A24" s="36">
         <v>20</v>
       </c>
-      <c r="B24" s="242" t="s">
+      <c r="B24" s="243" t="s">
         <v>399</v>
       </c>
       <c r="C24" s="22" t="s">
@@ -43489,7 +43488,7 @@
       <c r="A25" s="56">
         <v>21</v>
       </c>
-      <c r="B25" s="249"/>
+      <c r="B25" s="250"/>
       <c r="C25" s="59" t="s">
         <v>1256</v>
       </c>
@@ -43521,7 +43520,7 @@
       <c r="A26" s="36">
         <v>22</v>
       </c>
-      <c r="B26" s="250"/>
+      <c r="B26" s="251"/>
       <c r="C26" s="22" t="s">
         <v>1259</v>
       </c>
@@ -43553,7 +43552,7 @@
       <c r="A27" s="36">
         <v>23</v>
       </c>
-      <c r="B27" s="250"/>
+      <c r="B27" s="251"/>
       <c r="C27" s="22" t="s">
         <v>1262</v>
       </c>
@@ -43585,7 +43584,7 @@
       <c r="A28" s="56">
         <v>24</v>
       </c>
-      <c r="B28" s="249"/>
+      <c r="B28" s="250"/>
       <c r="C28" s="59" t="s">
         <v>1265</v>
       </c>
@@ -43617,7 +43616,7 @@
       <c r="A29" s="36">
         <v>25</v>
       </c>
-      <c r="B29" s="250"/>
+      <c r="B29" s="251"/>
       <c r="C29" s="22" t="s">
         <v>1268</v>
       </c>
@@ -43721,7 +43720,7 @@
       <c r="A32" s="36">
         <v>28</v>
       </c>
-      <c r="B32" s="242" t="s">
+      <c r="B32" s="243" t="s">
         <v>409</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -43757,7 +43756,7 @@
       <c r="A33" s="36">
         <v>29</v>
       </c>
-      <c r="B33" s="250"/>
+      <c r="B33" s="251"/>
       <c r="C33" s="4" t="s">
         <v>1276</v>
       </c>
@@ -43791,7 +43790,7 @@
       <c r="A34" s="36">
         <v>30</v>
       </c>
-      <c r="B34" s="250"/>
+      <c r="B34" s="251"/>
       <c r="C34" s="4" t="s">
         <v>1279</v>
       </c>
@@ -43825,7 +43824,7 @@
       <c r="A35" s="36">
         <v>31</v>
       </c>
-      <c r="B35" s="250"/>
+      <c r="B35" s="251"/>
       <c r="C35" s="4" t="s">
         <v>1282</v>
       </c>
@@ -44097,7 +44096,7 @@
       <c r="A42" s="58">
         <v>37</v>
       </c>
-      <c r="B42" s="243" t="s">
+      <c r="B42" s="244" t="s">
         <v>428</v>
       </c>
       <c r="C42" s="50" t="s">
@@ -44129,7 +44128,7 @@
       <c r="A43" s="36">
         <v>38</v>
       </c>
-      <c r="B43" s="249"/>
+      <c r="B43" s="250"/>
       <c r="C43" s="4" t="s">
         <v>1294</v>
       </c>
@@ -44159,7 +44158,7 @@
       <c r="A44" s="52">
         <v>39</v>
       </c>
-      <c r="B44" s="249"/>
+      <c r="B44" s="250"/>
       <c r="C44" s="51" t="s">
         <v>1297</v>
       </c>
@@ -44187,7 +44186,7 @@
     </row>
     <row r="45" spans="1:14" ht="116.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="36"/>
-      <c r="B45" s="244" t="s">
+      <c r="B45" s="245" t="s">
         <v>1300</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -44229,7 +44228,7 @@
     </row>
     <row r="46" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="36"/>
-      <c r="B46" s="244"/>
+      <c r="B46" s="245"/>
       <c r="C46" s="4" t="s">
         <v>1304</v>
       </c>
@@ -44263,7 +44262,7 @@
     </row>
     <row r="47" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="36"/>
-      <c r="B47" s="244"/>
+      <c r="B47" s="245"/>
       <c r="C47" s="4" t="s">
         <v>1307</v>
       </c>
@@ -44297,7 +44296,7 @@
     </row>
     <row r="48" spans="1:14" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="36"/>
-      <c r="B48" s="244" t="s">
+      <c r="B48" s="245" t="s">
         <v>435</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -44333,7 +44332,7 @@
     </row>
     <row r="49" spans="1:14" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="36"/>
-      <c r="B49" s="244"/>
+      <c r="B49" s="245"/>
       <c r="C49" s="4" t="s">
         <v>1313</v>
       </c>
@@ -44367,7 +44366,7 @@
     </row>
     <row r="50" spans="1:14" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A50" s="52"/>
-      <c r="B50" s="255" t="s">
+      <c r="B50" s="232" t="s">
         <v>1863</v>
       </c>
       <c r="C50" s="51" t="s">
@@ -45117,18 +45116,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>1866</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="234"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="236"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -45219,7 +45218,7 @@
       <c r="A4" s="36">
         <v>40</v>
       </c>
-      <c r="B4" s="240" t="s">
+      <c r="B4" s="241" t="s">
         <v>431</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -45259,7 +45258,7 @@
       <c r="A5" s="52">
         <v>41</v>
       </c>
-      <c r="B5" s="243"/>
+      <c r="B5" s="244"/>
       <c r="C5" s="51" t="s">
         <v>1319</v>
       </c>
@@ -45447,18 +45446,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>1323</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="248"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="251"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="248"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="237"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="237"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="249"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -46169,32 +46168,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -46401,6 +46374,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
   <ds:schemaRefs>
@@ -46410,23 +46409,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7F7E23-FE37-4AB8-A4B3-5025B5D9E450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -46443,4 +46425,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding files requested by Akshaya
</commit_message>
<xml_diff>
--- a/_files/requirements/Pending_Backlog_Stories_25Jun19_Updated.xlsx
+++ b/_files/requirements/Pending_Backlog_Stories_25Jun19_Updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1045476\Documents\GitHub\mosip-docs.wiki\_files\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip-docs.wiki\_files\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{29F39AAC-7973-4B79-B382-16B921D1E829}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D4ED42-87BB-4548-805B-7B7F247EECAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="12" r:id="rId1"/>
@@ -39,13 +39,18 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Resident Services'!$A$2:$J$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RoadmapFeatures!$B$3:$E$37</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId13"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -135,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5569" uniqueCount="1988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5632" uniqueCount="1997">
   <si>
     <t>Category</t>
   </si>
@@ -6863,6 +6868,33 @@
   </si>
   <si>
     <t>Customer Approval Pending</t>
+  </si>
+  <si>
+    <t>Dev In-Progress</t>
+  </si>
+  <si>
+    <t>Discussion Pending</t>
+  </si>
+  <si>
+    <t>MOS-27875</t>
+  </si>
+  <si>
+    <t>Validation - UIN</t>
+  </si>
+  <si>
+    <t>Validate if UIN is Active before performing any Update Operation on the UIN</t>
+  </si>
+  <si>
+    <t>MOS-27818</t>
+  </si>
+  <si>
+    <t>Validation - Device</t>
+  </si>
+  <si>
+    <t>Changes in Device Validation Post Integration with Actual Devices</t>
+  </si>
+  <si>
+    <t>MOS-27829</t>
   </si>
 </sst>
 </file>
@@ -7448,7 +7480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="257">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8051,17 +8083,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -8128,6 +8154,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -8197,6 +8226,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -15346,7 +15384,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:D32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -16264,18 +16302,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="234" t="s">
         <v>1333</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="238"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -16725,7 +16763,7 @@
       <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="239" t="s">
+      <c r="B17" s="238" t="s">
         <v>503</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -16757,7 +16795,7 @@
       <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="240"/>
+      <c r="B18" s="239"/>
       <c r="C18" s="4" t="s">
         <v>1352</v>
       </c>
@@ -17097,19 +17135,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="234" t="s">
         <v>1357</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="236"/>
-      <c r="K1" s="238"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="235"/>
+      <c r="K1" s="237"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="145" t="s">
@@ -22451,18 +22489,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="234" t="s">
         <v>1722</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="238"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="38" t="s">
@@ -22500,7 +22538,7 @@
       <c r="A3" s="39">
         <v>1</v>
       </c>
-      <c r="B3" s="254" t="s">
+      <c r="B3" s="253" t="s">
         <v>527</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -22526,7 +22564,7 @@
       <c r="A4" s="39">
         <v>2</v>
       </c>
-      <c r="B4" s="255"/>
+      <c r="B4" s="254"/>
       <c r="C4" s="4" t="s">
         <v>1726</v>
       </c>
@@ -22548,7 +22586,7 @@
       <c r="A5" s="39">
         <v>3</v>
       </c>
-      <c r="B5" s="254" t="s">
+      <c r="B5" s="253" t="s">
         <v>530</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -22574,7 +22612,7 @@
       <c r="A6" s="39">
         <v>4</v>
       </c>
-      <c r="B6" s="256"/>
+      <c r="B6" s="255"/>
       <c r="C6" s="19" t="s">
         <v>1731</v>
       </c>
@@ -22598,7 +22636,7 @@
       <c r="A7" s="39">
         <v>5</v>
       </c>
-      <c r="B7" s="256"/>
+      <c r="B7" s="255"/>
       <c r="C7" s="19" t="s">
         <v>1734</v>
       </c>
@@ -22620,7 +22658,7 @@
       <c r="A8" s="39">
         <v>6</v>
       </c>
-      <c r="B8" s="256"/>
+      <c r="B8" s="255"/>
       <c r="C8" s="19" t="s">
         <v>1736</v>
       </c>
@@ -22642,7 +22680,7 @@
       <c r="A9" s="39">
         <v>7</v>
       </c>
-      <c r="B9" s="256"/>
+      <c r="B9" s="255"/>
       <c r="C9" s="19" t="s">
         <v>1738</v>
       </c>
@@ -22664,7 +22702,7 @@
       <c r="A10" s="39">
         <v>8</v>
       </c>
-      <c r="B10" s="256"/>
+      <c r="B10" s="255"/>
       <c r="C10" s="19" t="s">
         <v>1740</v>
       </c>
@@ -22686,7 +22724,7 @@
       <c r="A11" s="39">
         <v>9</v>
       </c>
-      <c r="B11" s="256"/>
+      <c r="B11" s="255"/>
       <c r="C11" s="19" t="s">
         <v>1742</v>
       </c>
@@ -22708,7 +22746,7 @@
       <c r="A12" s="39">
         <v>10</v>
       </c>
-      <c r="B12" s="256"/>
+      <c r="B12" s="255"/>
       <c r="C12" s="19" t="s">
         <v>1744</v>
       </c>
@@ -22730,7 +22768,7 @@
       <c r="A13" s="39">
         <v>11</v>
       </c>
-      <c r="B13" s="256"/>
+      <c r="B13" s="255"/>
       <c r="C13" s="19" t="s">
         <v>1746</v>
       </c>
@@ -22752,7 +22790,7 @@
       <c r="A14" s="39">
         <v>12</v>
       </c>
-      <c r="B14" s="256"/>
+      <c r="B14" s="255"/>
       <c r="C14" s="19" t="s">
         <v>1748</v>
       </c>
@@ -22776,7 +22814,7 @@
       <c r="A15" s="39">
         <v>13</v>
       </c>
-      <c r="B15" s="256"/>
+      <c r="B15" s="255"/>
       <c r="C15" s="19" t="s">
         <v>1751</v>
       </c>
@@ -22800,7 +22838,7 @@
       <c r="A16" s="39">
         <v>14</v>
       </c>
-      <c r="B16" s="255"/>
+      <c r="B16" s="254"/>
       <c r="C16" s="19" t="s">
         <v>1753</v>
       </c>
@@ -22922,7 +22960,7 @@
       <c r="A21" s="39">
         <v>19</v>
       </c>
-      <c r="B21" s="254" t="s">
+      <c r="B21" s="253" t="s">
         <v>545</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -22946,7 +22984,7 @@
       <c r="A22" s="39">
         <v>20</v>
       </c>
-      <c r="B22" s="256"/>
+      <c r="B22" s="255"/>
       <c r="C22" s="4" t="s">
         <v>1761</v>
       </c>
@@ -22968,7 +23006,7 @@
       <c r="A23" s="39">
         <v>21</v>
       </c>
-      <c r="B23" s="256"/>
+      <c r="B23" s="255"/>
       <c r="C23" s="4" t="s">
         <v>1763</v>
       </c>
@@ -22990,7 +23028,7 @@
       <c r="A24" s="39">
         <v>22</v>
       </c>
-      <c r="B24" s="256"/>
+      <c r="B24" s="255"/>
       <c r="C24" s="4" t="s">
         <v>1765</v>
       </c>
@@ -23012,7 +23050,7 @@
       <c r="A25" s="39">
         <v>23</v>
       </c>
-      <c r="B25" s="256"/>
+      <c r="B25" s="255"/>
       <c r="C25" s="4" t="s">
         <v>1767</v>
       </c>
@@ -23034,7 +23072,7 @@
       <c r="A26" s="39">
         <v>24</v>
       </c>
-      <c r="B26" s="255"/>
+      <c r="B26" s="254"/>
       <c r="C26" s="4" t="s">
         <v>1769</v>
       </c>
@@ -23056,7 +23094,7 @@
       <c r="A27" s="39">
         <v>25</v>
       </c>
-      <c r="B27" s="254" t="s">
+      <c r="B27" s="253" t="s">
         <v>548</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -23080,7 +23118,7 @@
       <c r="A28" s="39">
         <v>26</v>
       </c>
-      <c r="B28" s="255"/>
+      <c r="B28" s="254"/>
       <c r="C28" s="4" t="s">
         <v>1773</v>
       </c>
@@ -23102,7 +23140,7 @@
       <c r="A29" s="39">
         <v>27</v>
       </c>
-      <c r="B29" s="254" t="s">
+      <c r="B29" s="253" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -23126,7 +23164,7 @@
       <c r="A30" s="39">
         <v>28</v>
       </c>
-      <c r="B30" s="255"/>
+      <c r="B30" s="254"/>
       <c r="C30" s="4" t="s">
         <v>1777</v>
       </c>
@@ -23148,7 +23186,7 @@
       <c r="A31" s="39">
         <v>29</v>
       </c>
-      <c r="B31" s="254" t="s">
+      <c r="B31" s="253" t="s">
         <v>553</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -23172,7 +23210,7 @@
       <c r="A32" s="39">
         <v>30</v>
       </c>
-      <c r="B32" s="256"/>
+      <c r="B32" s="255"/>
       <c r="C32" s="4" t="s">
         <v>1781</v>
       </c>
@@ -23194,7 +23232,7 @@
       <c r="A33" s="39">
         <v>31</v>
       </c>
-      <c r="B33" s="256"/>
+      <c r="B33" s="255"/>
       <c r="C33" s="4" t="s">
         <v>1783</v>
       </c>
@@ -23216,7 +23254,7 @@
       <c r="A34" s="39">
         <v>32</v>
       </c>
-      <c r="B34" s="256"/>
+      <c r="B34" s="255"/>
       <c r="C34" s="4" t="s">
         <v>1785</v>
       </c>
@@ -23238,7 +23276,7 @@
       <c r="A35" s="39">
         <v>33</v>
       </c>
-      <c r="B35" s="255"/>
+      <c r="B35" s="254"/>
       <c r="C35" s="4" t="s">
         <v>1787</v>
       </c>
@@ -23260,7 +23298,7 @@
       <c r="A36" s="39">
         <v>34</v>
       </c>
-      <c r="B36" s="254" t="s">
+      <c r="B36" s="253" t="s">
         <v>556</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -23284,7 +23322,7 @@
       <c r="A37" s="39">
         <v>35</v>
       </c>
-      <c r="B37" s="256"/>
+      <c r="B37" s="255"/>
       <c r="C37" s="4" t="s">
         <v>1791</v>
       </c>
@@ -23306,7 +23344,7 @@
       <c r="A38" s="39">
         <v>36</v>
       </c>
-      <c r="B38" s="256"/>
+      <c r="B38" s="255"/>
       <c r="C38" s="4" t="s">
         <v>1793</v>
       </c>
@@ -23328,7 +23366,7 @@
       <c r="A39" s="39">
         <v>37</v>
       </c>
-      <c r="B39" s="255"/>
+      <c r="B39" s="254"/>
       <c r="C39" s="4" t="s">
         <v>1795</v>
       </c>
@@ -23350,7 +23388,7 @@
       <c r="A40" s="39">
         <v>38</v>
       </c>
-      <c r="B40" s="254" t="s">
+      <c r="B40" s="253" t="s">
         <v>559</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -23374,7 +23412,7 @@
       <c r="A41" s="39">
         <v>39</v>
       </c>
-      <c r="B41" s="255"/>
+      <c r="B41" s="254"/>
       <c r="C41" s="4" t="s">
         <v>1799</v>
       </c>
@@ -23420,7 +23458,7 @@
       <c r="A43" s="39">
         <v>41</v>
       </c>
-      <c r="B43" s="254" t="s">
+      <c r="B43" s="253" t="s">
         <v>565</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -23444,7 +23482,7 @@
       <c r="A44" s="39">
         <v>42</v>
       </c>
-      <c r="B44" s="256"/>
+      <c r="B44" s="255"/>
       <c r="C44" s="4" t="s">
         <v>1804</v>
       </c>
@@ -23466,7 +23504,7 @@
       <c r="A45" s="39">
         <v>43</v>
       </c>
-      <c r="B45" s="256"/>
+      <c r="B45" s="255"/>
       <c r="C45" s="4" t="s">
         <v>1806</v>
       </c>
@@ -23488,7 +23526,7 @@
       <c r="A46" s="39">
         <v>44</v>
       </c>
-      <c r="B46" s="256"/>
+      <c r="B46" s="255"/>
       <c r="C46" s="4" t="s">
         <v>1808</v>
       </c>
@@ -23512,7 +23550,7 @@
       <c r="A47" s="39">
         <v>45</v>
       </c>
-      <c r="B47" s="256"/>
+      <c r="B47" s="255"/>
       <c r="C47" s="4" t="s">
         <v>1811</v>
       </c>
@@ -23534,7 +23572,7 @@
       <c r="A48" s="39">
         <v>46</v>
       </c>
-      <c r="B48" s="256"/>
+      <c r="B48" s="255"/>
       <c r="C48" s="4" t="s">
         <v>1813</v>
       </c>
@@ -23556,7 +23594,7 @@
       <c r="A49" s="39">
         <v>47</v>
       </c>
-      <c r="B49" s="256"/>
+      <c r="B49" s="255"/>
       <c r="C49" s="4" t="s">
         <v>1815</v>
       </c>
@@ -23578,7 +23616,7 @@
       <c r="A50" s="39">
         <v>48</v>
       </c>
-      <c r="B50" s="256"/>
+      <c r="B50" s="255"/>
       <c r="C50" s="4" t="s">
         <v>1817</v>
       </c>
@@ -23602,7 +23640,7 @@
       <c r="A51" s="39">
         <v>49</v>
       </c>
-      <c r="B51" s="256"/>
+      <c r="B51" s="255"/>
       <c r="C51" s="4" t="s">
         <v>1819</v>
       </c>
@@ -23624,7 +23662,7 @@
       <c r="A52" s="39">
         <v>50</v>
       </c>
-      <c r="B52" s="256"/>
+      <c r="B52" s="255"/>
       <c r="C52" s="4" t="s">
         <v>1821</v>
       </c>
@@ -23646,7 +23684,7 @@
       <c r="A53" s="39">
         <v>51</v>
       </c>
-      <c r="B53" s="256"/>
+      <c r="B53" s="255"/>
       <c r="C53" s="4" t="s">
         <v>1823</v>
       </c>
@@ -23668,7 +23706,7 @@
       <c r="A54" s="39">
         <v>52</v>
       </c>
-      <c r="B54" s="255"/>
+      <c r="B54" s="254"/>
       <c r="C54" s="4" t="s">
         <v>1825</v>
       </c>
@@ -23701,16 +23739,16 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="10">
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B43:B54"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B35"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B16"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B43:B54"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -23722,11 +23760,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B2:U352"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -23751,26 +23789,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="235" t="s">
+      <c r="B2" s="234" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="236"/>
-      <c r="D2" s="236"/>
-      <c r="E2" s="236"/>
-      <c r="F2" s="236"/>
-      <c r="G2" s="236"/>
-      <c r="H2" s="236"/>
-      <c r="I2" s="237"/>
-      <c r="J2" s="236"/>
-      <c r="K2" s="236"/>
-      <c r="L2" s="236"/>
-      <c r="M2" s="236"/>
-      <c r="N2" s="236"/>
-      <c r="O2" s="236"/>
-      <c r="P2" s="236"/>
-      <c r="Q2" s="236"/>
-      <c r="R2" s="236"/>
-      <c r="S2" s="238"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="235"/>
+      <c r="G2" s="235"/>
+      <c r="H2" s="235"/>
+      <c r="I2" s="236"/>
+      <c r="J2" s="235"/>
+      <c r="K2" s="235"/>
+      <c r="L2" s="235"/>
+      <c r="M2" s="235"/>
+      <c r="N2" s="235"/>
+      <c r="O2" s="235"/>
+      <c r="P2" s="235"/>
+      <c r="Q2" s="235"/>
+      <c r="R2" s="235"/>
+      <c r="S2" s="237"/>
     </row>
     <row r="3" spans="2:19" ht="70" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
@@ -25772,7 +25810,7 @@
       <c r="R62" s="89"/>
       <c r="S62" s="47"/>
     </row>
-    <row r="63" spans="2:19" ht="168" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:19" ht="154" x14ac:dyDescent="0.35">
       <c r="B63" s="91">
         <v>60</v>
       </c>
@@ -25955,7 +25993,7 @@
       <c r="C68" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="D68" s="234" t="s">
+      <c r="D68" s="233" t="s">
         <v>222</v>
       </c>
       <c r="E68" s="118"/>
@@ -25989,7 +26027,7 @@
       <c r="C69" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="D69" s="234"/>
+      <c r="D69" s="233"/>
       <c r="E69" s="118"/>
       <c r="F69" s="47" t="s">
         <v>225</v>
@@ -27362,7 +27400,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="109" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:19" ht="28" x14ac:dyDescent="0.35">
       <c r="B109" s="91">
         <v>106</v>
       </c>
@@ -27398,7 +27436,7 @@
       <c r="R109" s="89"/>
       <c r="S109" s="47"/>
     </row>
-    <row r="110" spans="2:19" ht="70" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:19" ht="56" x14ac:dyDescent="0.35">
       <c r="B110" s="91">
         <v>107</v>
       </c>
@@ -28174,7 +28212,7 @@
       <c r="R131" s="89"/>
       <c r="S131" s="47"/>
     </row>
-    <row r="132" spans="2:19" ht="154" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:19" ht="140" x14ac:dyDescent="0.35">
       <c r="B132" s="91">
         <v>129</v>
       </c>
@@ -35734,12 +35772,12 @@
       <c r="F1" s="41"/>
     </row>
     <row r="2" spans="2:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="235" t="s">
+      <c r="B2" s="234" t="s">
         <v>885</v>
       </c>
-      <c r="C2" s="236"/>
-      <c r="D2" s="236"/>
-      <c r="E2" s="238"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="237"/>
       <c r="F2" s="41"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
@@ -37307,18 +37345,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="234" t="s">
         <v>907</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="238"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -37587,7 +37625,7 @@
       <c r="G9" s="207" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="209">
+      <c r="H9" s="208">
         <v>235.25</v>
       </c>
       <c r="I9" s="39" t="s">
@@ -37839,7 +37877,7 @@
       <c r="A17" s="36">
         <v>14</v>
       </c>
-      <c r="B17" s="239" t="s">
+      <c r="B17" s="238" t="s">
         <v>143</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -37872,7 +37910,7 @@
       <c r="A18" s="36">
         <v>15</v>
       </c>
-      <c r="B18" s="240"/>
+      <c r="B18" s="239"/>
       <c r="C18" s="4" t="s">
         <v>954</v>
       </c>
@@ -37903,7 +37941,7 @@
       <c r="A19" s="36">
         <v>16</v>
       </c>
-      <c r="B19" s="239" t="s">
+      <c r="B19" s="238" t="s">
         <v>146</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -37936,7 +37974,7 @@
       <c r="A20" s="36">
         <v>17</v>
       </c>
-      <c r="B20" s="240"/>
+      <c r="B20" s="239"/>
       <c r="C20" s="4" t="s">
         <v>960</v>
       </c>
@@ -38091,7 +38129,7 @@
       <c r="G24" s="41" t="s">
         <v>1973</v>
       </c>
-      <c r="H24" s="210"/>
+      <c r="H24" s="209"/>
       <c r="I24" s="41"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
@@ -38249,18 +38287,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="234" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="238"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -38310,7 +38348,7 @@
       <c r="A3" s="36">
         <v>1</v>
       </c>
-      <c r="B3" s="228" t="s">
+      <c r="B3" s="226" t="s">
         <v>155</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -38319,7 +38357,7 @@
       <c r="D3" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="E3" s="231" t="s">
+      <c r="E3" s="229" t="s">
         <v>157</v>
       </c>
       <c r="F3" s="39" t="s">
@@ -38352,7 +38390,7 @@
       <c r="A4" s="36">
         <v>2</v>
       </c>
-      <c r="B4" s="242" t="s">
+      <c r="B4" s="241" t="s">
         <v>158</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -38361,7 +38399,7 @@
       <c r="D4" s="39" t="s">
         <v>971</v>
       </c>
-      <c r="E4" s="231" t="s">
+      <c r="E4" s="229" t="s">
         <v>972</v>
       </c>
       <c r="F4" s="39" t="s">
@@ -38386,14 +38424,14 @@
       <c r="A5" s="36">
         <v>3</v>
       </c>
-      <c r="B5" s="243"/>
+      <c r="B5" s="242"/>
       <c r="C5" s="4" t="s">
         <v>974</v>
       </c>
       <c r="D5" s="39" t="s">
         <v>975</v>
       </c>
-      <c r="E5" s="231" t="s">
+      <c r="E5" s="229" t="s">
         <v>976</v>
       </c>
       <c r="F5" s="39" t="s">
@@ -38418,7 +38456,7 @@
       <c r="A6" s="36">
         <v>4</v>
       </c>
-      <c r="B6" s="231" t="s">
+      <c r="B6" s="229" t="s">
         <v>161</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -38427,7 +38465,7 @@
       <c r="D6" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="231" t="s">
+      <c r="E6" s="229" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="39" t="s">
@@ -38462,7 +38500,7 @@
       <c r="A7" s="36">
         <v>5</v>
       </c>
-      <c r="B7" s="231" t="s">
+      <c r="B7" s="229" t="s">
         <v>165</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -38471,7 +38509,7 @@
       <c r="D7" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="231" t="s">
+      <c r="E7" s="229" t="s">
         <v>979</v>
       </c>
       <c r="F7" s="39" t="s">
@@ -38506,7 +38544,7 @@
       <c r="A8" s="36">
         <v>6</v>
       </c>
-      <c r="B8" s="242" t="s">
+      <c r="B8" s="241" t="s">
         <v>169</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -38515,7 +38553,7 @@
       <c r="D8" s="39" t="s">
         <v>981</v>
       </c>
-      <c r="E8" s="231" t="s">
+      <c r="E8" s="229" t="s">
         <v>982</v>
       </c>
       <c r="F8" s="39" t="s">
@@ -38542,14 +38580,14 @@
       <c r="A9" s="36">
         <v>11</v>
       </c>
-      <c r="B9" s="243"/>
+      <c r="B9" s="242"/>
       <c r="C9" s="4" t="s">
         <v>984</v>
       </c>
       <c r="D9" s="39" t="s">
         <v>985</v>
       </c>
-      <c r="E9" s="231" t="s">
+      <c r="E9" s="229" t="s">
         <v>986</v>
       </c>
       <c r="F9" s="39" t="s">
@@ -38573,7 +38611,7 @@
       <c r="A10" s="36">
         <v>7</v>
       </c>
-      <c r="B10" s="228" t="s">
+      <c r="B10" s="226" t="s">
         <v>173</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -38582,7 +38620,7 @@
       <c r="D10" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="E10" s="231" t="s">
+      <c r="E10" s="229" t="s">
         <v>175</v>
       </c>
       <c r="F10" s="39" t="s">
@@ -38607,7 +38645,7 @@
       <c r="A11" s="36">
         <v>8</v>
       </c>
-      <c r="B11" s="231" t="s">
+      <c r="B11" s="229" t="s">
         <v>176</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -38616,7 +38654,7 @@
       <c r="D11" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="E11" s="231" t="s">
+      <c r="E11" s="229" t="s">
         <v>178</v>
       </c>
       <c r="F11" s="39" t="s">
@@ -38641,7 +38679,7 @@
       <c r="A12" s="36">
         <v>9</v>
       </c>
-      <c r="B12" s="231" t="s">
+      <c r="B12" s="229" t="s">
         <v>179</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -38650,7 +38688,7 @@
       <c r="D12" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="E12" s="231" t="s">
+      <c r="E12" s="229" t="s">
         <v>991</v>
       </c>
       <c r="F12" s="39" t="s">
@@ -38677,7 +38715,7 @@
       <c r="A13" s="36">
         <v>10</v>
       </c>
-      <c r="B13" s="231" t="s">
+      <c r="B13" s="229" t="s">
         <v>993</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -38686,7 +38724,7 @@
       <c r="D13" s="39" t="s">
         <v>995</v>
       </c>
-      <c r="E13" s="231" t="s">
+      <c r="E13" s="229" t="s">
         <v>996</v>
       </c>
       <c r="F13" s="39" t="s">
@@ -38713,7 +38751,7 @@
       <c r="A14" s="36">
         <v>12</v>
       </c>
-      <c r="B14" s="242" t="s">
+      <c r="B14" s="241" t="s">
         <v>182</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -38722,7 +38760,7 @@
       <c r="D14" s="39" t="s">
         <v>998</v>
       </c>
-      <c r="E14" s="231" t="s">
+      <c r="E14" s="229" t="s">
         <v>999</v>
       </c>
       <c r="F14" s="39" t="s">
@@ -38749,14 +38787,14 @@
       <c r="A15" s="36">
         <v>13</v>
       </c>
-      <c r="B15" s="243"/>
+      <c r="B15" s="242"/>
       <c r="C15" s="4" t="s">
         <v>1000</v>
       </c>
       <c r="D15" s="39" t="s">
         <v>1001</v>
       </c>
-      <c r="E15" s="231" t="s">
+      <c r="E15" s="229" t="s">
         <v>1002</v>
       </c>
       <c r="F15" s="39" t="s">
@@ -38783,7 +38821,7 @@
       <c r="A16" s="36">
         <v>14</v>
       </c>
-      <c r="B16" s="231" t="s">
+      <c r="B16" s="229" t="s">
         <v>185</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -38792,7 +38830,7 @@
       <c r="D16" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="E16" s="231" t="s">
+      <c r="E16" s="229" t="s">
         <v>187</v>
       </c>
       <c r="F16" s="39" t="s">
@@ -38827,7 +38865,7 @@
       <c r="A17" s="36">
         <v>15</v>
       </c>
-      <c r="B17" s="231" t="s">
+      <c r="B17" s="229" t="s">
         <v>189</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -38836,7 +38874,7 @@
       <c r="D17" s="39" t="s">
         <v>190</v>
       </c>
-      <c r="E17" s="231" t="s">
+      <c r="E17" s="229" t="s">
         <v>191</v>
       </c>
       <c r="F17" s="39" t="s">
@@ -38871,7 +38909,7 @@
       <c r="A18" s="36">
         <v>16</v>
       </c>
-      <c r="B18" s="231" t="s">
+      <c r="B18" s="229" t="s">
         <v>1914</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -38880,7 +38918,7 @@
       <c r="D18" s="39" t="s">
         <v>194</v>
       </c>
-      <c r="E18" s="231" t="s">
+      <c r="E18" s="229" t="s">
         <v>195</v>
       </c>
       <c r="F18" s="39" t="s">
@@ -38912,7 +38950,7 @@
       <c r="A19" s="36">
         <v>17</v>
       </c>
-      <c r="B19" s="231" t="s">
+      <c r="B19" s="229" t="s">
         <v>197</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -38921,7 +38959,7 @@
       <c r="D19" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="E19" s="231" t="s">
+      <c r="E19" s="229" t="s">
         <v>199</v>
       </c>
       <c r="F19" s="39" t="s">
@@ -38954,7 +38992,7 @@
       <c r="A20" s="36">
         <v>18</v>
       </c>
-      <c r="B20" s="231" t="s">
+      <c r="B20" s="229" t="s">
         <v>200</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -38963,7 +39001,7 @@
       <c r="D20" s="39" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="231" t="s">
+      <c r="E20" s="229" t="s">
         <v>202</v>
       </c>
       <c r="F20" s="39" t="s">
@@ -38996,7 +39034,7 @@
       <c r="A21" s="36">
         <v>19</v>
       </c>
-      <c r="B21" s="231" t="s">
+      <c r="B21" s="229" t="s">
         <v>203</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -39005,7 +39043,7 @@
       <c r="D21" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="E21" s="231" t="s">
+      <c r="E21" s="229" t="s">
         <v>205</v>
       </c>
       <c r="F21" s="39" t="s">
@@ -39038,7 +39076,7 @@
       <c r="A22" s="36">
         <v>20</v>
       </c>
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="241" t="s">
         <v>1009</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -39047,7 +39085,7 @@
       <c r="D22" s="39" t="s">
         <v>1011</v>
       </c>
-      <c r="E22" s="231" t="s">
+      <c r="E22" s="229" t="s">
         <v>1012</v>
       </c>
       <c r="F22" s="39" t="s">
@@ -39080,14 +39118,14 @@
       <c r="A23" s="36">
         <v>21</v>
       </c>
-      <c r="B23" s="245"/>
+      <c r="B23" s="244"/>
       <c r="C23" s="4" t="s">
         <v>1013</v>
       </c>
       <c r="D23" s="39" t="s">
         <v>1014</v>
       </c>
-      <c r="E23" s="231" t="s">
+      <c r="E23" s="229" t="s">
         <v>1015</v>
       </c>
       <c r="F23" s="39" t="s">
@@ -39119,14 +39157,14 @@
       <c r="A24" s="36">
         <v>22</v>
       </c>
-      <c r="B24" s="243"/>
+      <c r="B24" s="242"/>
       <c r="C24" s="4" t="s">
         <v>1016</v>
       </c>
       <c r="D24" s="39" t="s">
         <v>1017</v>
       </c>
-      <c r="E24" s="231" t="s">
+      <c r="E24" s="229" t="s">
         <v>1018</v>
       </c>
       <c r="F24" s="39" t="s">
@@ -39159,7 +39197,7 @@
       <c r="A25" s="36">
         <v>23</v>
       </c>
-      <c r="B25" s="231" t="s">
+      <c r="B25" s="229" t="s">
         <v>209</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -39168,7 +39206,7 @@
       <c r="D25" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="E25" s="231" t="s">
+      <c r="E25" s="229" t="s">
         <v>211</v>
       </c>
       <c r="F25" s="39" t="s">
@@ -39201,7 +39239,7 @@
       <c r="A26" s="36">
         <v>24</v>
       </c>
-      <c r="B26" s="231" t="s">
+      <c r="B26" s="229" t="s">
         <v>212</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -39210,7 +39248,7 @@
       <c r="D26" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="E26" s="231" t="s">
+      <c r="E26" s="229" t="s">
         <v>214</v>
       </c>
       <c r="F26" s="39" t="s">
@@ -39266,7 +39304,7 @@
       <c r="A28" s="36">
         <v>26</v>
       </c>
-      <c r="B28" s="228" t="s">
+      <c r="B28" s="226" t="s">
         <v>215</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -39275,7 +39313,7 @@
       <c r="D28" s="39" t="s">
         <v>216</v>
       </c>
-      <c r="E28" s="231" t="s">
+      <c r="E28" s="229" t="s">
         <v>217</v>
       </c>
       <c r="F28" s="39" t="s">
@@ -39308,7 +39346,7 @@
       <c r="A29" s="36">
         <v>27</v>
       </c>
-      <c r="B29" s="228" t="s">
+      <c r="B29" s="226" t="s">
         <v>218</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -39317,7 +39355,7 @@
       <c r="D29" s="39" t="s">
         <v>219</v>
       </c>
-      <c r="E29" s="231" t="s">
+      <c r="E29" s="229" t="s">
         <v>220</v>
       </c>
       <c r="F29" s="39" t="s">
@@ -39344,7 +39382,7 @@
       <c r="A30" s="36">
         <v>28</v>
       </c>
-      <c r="B30" s="242" t="s">
+      <c r="B30" s="241" t="s">
         <v>222</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -39353,7 +39391,7 @@
       <c r="D30" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="E30" s="231" t="s">
+      <c r="E30" s="229" t="s">
         <v>224</v>
       </c>
       <c r="F30" s="39" t="s">
@@ -39380,14 +39418,14 @@
       <c r="A31" s="36">
         <v>29</v>
       </c>
-      <c r="B31" s="243"/>
+      <c r="B31" s="242"/>
       <c r="C31" s="4" t="s">
         <v>1029</v>
       </c>
       <c r="D31" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="E31" s="231" t="s">
+      <c r="E31" s="229" t="s">
         <v>224</v>
       </c>
       <c r="F31" s="39" t="s">
@@ -39414,7 +39452,7 @@
       <c r="A32" s="36">
         <v>30</v>
       </c>
-      <c r="B32" s="242" t="s">
+      <c r="B32" s="241" t="s">
         <v>226</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -39423,7 +39461,7 @@
       <c r="D32" s="39" t="s">
         <v>1031</v>
       </c>
-      <c r="E32" s="231" t="s">
+      <c r="E32" s="229" t="s">
         <v>1032</v>
       </c>
       <c r="F32" s="39" t="s">
@@ -39450,14 +39488,14 @@
       <c r="A33" s="36">
         <v>31</v>
       </c>
-      <c r="B33" s="243"/>
+      <c r="B33" s="242"/>
       <c r="C33" s="4" t="s">
         <v>1033</v>
       </c>
       <c r="D33" s="39" t="s">
         <v>1034</v>
       </c>
-      <c r="E33" s="231" t="s">
+      <c r="E33" s="229" t="s">
         <v>228</v>
       </c>
       <c r="F33" s="39" t="s">
@@ -39484,7 +39522,7 @@
       <c r="A34" s="36">
         <v>32</v>
       </c>
-      <c r="B34" s="231" t="s">
+      <c r="B34" s="229" t="s">
         <v>230</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -39493,7 +39531,7 @@
       <c r="D34" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="E34" s="231" t="s">
+      <c r="E34" s="229" t="s">
         <v>232</v>
       </c>
       <c r="F34" s="39" t="s">
@@ -39506,7 +39544,7 @@
       <c r="I34" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J34" s="232" t="s">
+      <c r="J34" s="230" t="s">
         <v>71</v>
       </c>
       <c r="K34" s="5" t="s">
@@ -39520,7 +39558,7 @@
       <c r="A35" s="36">
         <v>33</v>
       </c>
-      <c r="B35" s="231" t="s">
+      <c r="B35" s="229" t="s">
         <v>233</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -39529,7 +39567,7 @@
       <c r="D35" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="E35" s="231" t="s">
+      <c r="E35" s="229" t="s">
         <v>235</v>
       </c>
       <c r="F35" s="39" t="s">
@@ -39561,7 +39599,7 @@
       <c r="A36" s="36">
         <v>34</v>
       </c>
-      <c r="B36" s="231" t="s">
+      <c r="B36" s="229" t="s">
         <v>237</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -39570,7 +39608,7 @@
       <c r="D36" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="E36" s="231" t="s">
+      <c r="E36" s="229" t="s">
         <v>239</v>
       </c>
       <c r="F36" s="39" t="s">
@@ -39579,11 +39617,11 @@
       <c r="G36" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="H36" s="233"/>
+      <c r="H36" s="231"/>
       <c r="I36" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J36" s="233" t="s">
+      <c r="J36" s="231" t="s">
         <v>71</v>
       </c>
       <c r="K36" s="5" t="s">
@@ -39597,7 +39635,7 @@
       <c r="A37" s="36">
         <v>35</v>
       </c>
-      <c r="B37" s="231" t="s">
+      <c r="B37" s="229" t="s">
         <v>240</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -39606,7 +39644,7 @@
       <c r="D37" s="39" t="s">
         <v>241</v>
       </c>
-      <c r="E37" s="231" t="s">
+      <c r="E37" s="229" t="s">
         <v>242</v>
       </c>
       <c r="F37" s="39" t="s">
@@ -39631,7 +39669,7 @@
       <c r="A38" s="36">
         <v>36</v>
       </c>
-      <c r="B38" s="231" t="s">
+      <c r="B38" s="229" t="s">
         <v>243</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -39640,7 +39678,7 @@
       <c r="D38" s="39" t="s">
         <v>244</v>
       </c>
-      <c r="E38" s="231" t="s">
+      <c r="E38" s="229" t="s">
         <v>245</v>
       </c>
       <c r="F38" s="39" t="s">
@@ -39667,7 +39705,7 @@
       <c r="A39" s="36">
         <v>37</v>
       </c>
-      <c r="B39" s="228" t="s">
+      <c r="B39" s="226" t="s">
         <v>247</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -39676,7 +39714,7 @@
       <c r="D39" s="39" t="s">
         <v>248</v>
       </c>
-      <c r="E39" s="231" t="s">
+      <c r="E39" s="229" t="s">
         <v>1915</v>
       </c>
       <c r="F39" s="39" t="s">
@@ -39709,7 +39747,7 @@
       <c r="A40" s="36">
         <v>38</v>
       </c>
-      <c r="B40" s="231" t="s">
+      <c r="B40" s="229" t="s">
         <v>250</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -39718,7 +39756,7 @@
       <c r="D40" s="39" t="s">
         <v>251</v>
       </c>
-      <c r="E40" s="231" t="s">
+      <c r="E40" s="229" t="s">
         <v>252</v>
       </c>
       <c r="F40" s="39" t="s">
@@ -39731,7 +39769,7 @@
       <c r="I40" s="39" t="s">
         <v>918</v>
       </c>
-      <c r="J40" s="233" t="s">
+      <c r="J40" s="231" t="s">
         <v>253</v>
       </c>
       <c r="K40" s="29" t="s">
@@ -39745,7 +39783,7 @@
       <c r="A41" s="36">
         <v>39</v>
       </c>
-      <c r="B41" s="242" t="s">
+      <c r="B41" s="241" t="s">
         <v>254</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -39754,7 +39792,7 @@
       <c r="D41" s="39" t="s">
         <v>1044</v>
       </c>
-      <c r="E41" s="231" t="s">
+      <c r="E41" s="229" t="s">
         <v>256</v>
       </c>
       <c r="F41" s="39" t="s">
@@ -39781,14 +39819,14 @@
       <c r="A42" s="36">
         <v>40</v>
       </c>
-      <c r="B42" s="243"/>
+      <c r="B42" s="242"/>
       <c r="C42" s="4" t="s">
         <v>1045</v>
       </c>
       <c r="D42" s="39" t="s">
         <v>1046</v>
       </c>
-      <c r="E42" s="231" t="s">
+      <c r="E42" s="229" t="s">
         <v>256</v>
       </c>
       <c r="F42" s="39" t="s">
@@ -39815,7 +39853,7 @@
       <c r="A43" s="36">
         <v>41</v>
       </c>
-      <c r="B43" s="231" t="s">
+      <c r="B43" s="229" t="s">
         <v>257</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -39824,7 +39862,7 @@
       <c r="D43" s="39" t="s">
         <v>258</v>
       </c>
-      <c r="E43" s="231" t="s">
+      <c r="E43" s="229" t="s">
         <v>259</v>
       </c>
       <c r="F43" s="39" t="s">
@@ -39851,7 +39889,7 @@
       <c r="A44" s="36">
         <v>42</v>
       </c>
-      <c r="B44" s="242" t="s">
+      <c r="B44" s="241" t="s">
         <v>260</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -39860,7 +39898,7 @@
       <c r="D44" s="39" t="s">
         <v>1050</v>
       </c>
-      <c r="E44" s="231" t="s">
+      <c r="E44" s="229" t="s">
         <v>1051</v>
       </c>
       <c r="F44" s="39" t="s">
@@ -39887,14 +39925,14 @@
       <c r="A45" s="36">
         <v>43</v>
       </c>
-      <c r="B45" s="243"/>
+      <c r="B45" s="242"/>
       <c r="C45" s="4" t="s">
         <v>1052</v>
       </c>
       <c r="D45" s="39" t="s">
         <v>1053</v>
       </c>
-      <c r="E45" s="231" t="s">
+      <c r="E45" s="229" t="s">
         <v>262</v>
       </c>
       <c r="F45" s="39" t="s">
@@ -39921,7 +39959,7 @@
       <c r="A46" s="36">
         <v>44</v>
       </c>
-      <c r="B46" s="231" t="s">
+      <c r="B46" s="229" t="s">
         <v>264</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -39930,7 +39968,7 @@
       <c r="D46" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="E46" s="231" t="s">
+      <c r="E46" s="229" t="s">
         <v>266</v>
       </c>
       <c r="F46" s="39" t="s">
@@ -39957,7 +39995,7 @@
       <c r="A47" s="36">
         <v>45</v>
       </c>
-      <c r="B47" s="231" t="s">
+      <c r="B47" s="229" t="s">
         <v>268</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -39966,7 +40004,7 @@
       <c r="D47" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="E47" s="231" t="s">
+      <c r="E47" s="229" t="s">
         <v>270</v>
       </c>
       <c r="F47" s="39" t="s">
@@ -39979,7 +40017,7 @@
       <c r="I47" s="39" t="s">
         <v>1007</v>
       </c>
-      <c r="J47" s="232"/>
+      <c r="J47" s="230"/>
       <c r="K47" s="5" t="s">
         <v>349</v>
       </c>
@@ -40000,7 +40038,7 @@
       <c r="D48" s="39" t="s">
         <v>1057</v>
       </c>
-      <c r="E48" s="231" t="s">
+      <c r="E48" s="229" t="s">
         <v>1058</v>
       </c>
       <c r="F48" s="39" t="s">
@@ -40015,7 +40053,7 @@
       <c r="I48" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J48" s="244" t="s">
+      <c r="J48" s="243" t="s">
         <v>274</v>
       </c>
       <c r="K48" s="85" t="s">
@@ -40035,7 +40073,7 @@
       <c r="D49" s="39" t="s">
         <v>1061</v>
       </c>
-      <c r="E49" s="231" t="s">
+      <c r="E49" s="229" t="s">
         <v>1062</v>
       </c>
       <c r="F49" s="39" t="s">
@@ -40050,7 +40088,7 @@
       <c r="I49" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J49" s="244"/>
+      <c r="J49" s="243"/>
       <c r="K49" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40068,7 +40106,7 @@
       <c r="D50" s="39" t="s">
         <v>1065</v>
       </c>
-      <c r="E50" s="231" t="s">
+      <c r="E50" s="229" t="s">
         <v>1066</v>
       </c>
       <c r="F50" s="39" t="s">
@@ -40083,7 +40121,7 @@
       <c r="I50" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J50" s="244"/>
+      <c r="J50" s="243"/>
       <c r="K50" s="129" t="s">
         <v>349</v>
       </c>
@@ -40101,7 +40139,7 @@
       <c r="D51" s="39" t="s">
         <v>1068</v>
       </c>
-      <c r="E51" s="231" t="s">
+      <c r="E51" s="229" t="s">
         <v>1069</v>
       </c>
       <c r="F51" s="39" t="s">
@@ -40116,7 +40154,7 @@
       <c r="I51" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J51" s="244"/>
+      <c r="J51" s="243"/>
       <c r="K51" s="129" t="s">
         <v>1070</v>
       </c>
@@ -40134,7 +40172,7 @@
       <c r="D52" s="39" t="s">
         <v>1072</v>
       </c>
-      <c r="E52" s="231" t="s">
+      <c r="E52" s="229" t="s">
         <v>1073</v>
       </c>
       <c r="F52" s="39" t="s">
@@ -40149,7 +40187,7 @@
       <c r="I52" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J52" s="244"/>
+      <c r="J52" s="243"/>
       <c r="K52" s="129" t="s">
         <v>1074</v>
       </c>
@@ -40167,7 +40205,7 @@
       <c r="D53" s="39" t="s">
         <v>1076</v>
       </c>
-      <c r="E53" s="231" t="s">
+      <c r="E53" s="229" t="s">
         <v>1077</v>
       </c>
       <c r="F53" s="39" t="s">
@@ -40182,7 +40220,7 @@
       <c r="I53" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J53" s="244"/>
+      <c r="J53" s="243"/>
       <c r="K53" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40200,7 +40238,7 @@
       <c r="D54" s="39" t="s">
         <v>1079</v>
       </c>
-      <c r="E54" s="231" t="s">
+      <c r="E54" s="229" t="s">
         <v>1080</v>
       </c>
       <c r="F54" s="39" t="s">
@@ -40215,7 +40253,7 @@
       <c r="I54" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J54" s="244"/>
+      <c r="J54" s="243"/>
       <c r="K54" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40233,7 +40271,7 @@
       <c r="D55" s="39" t="s">
         <v>1082</v>
       </c>
-      <c r="E55" s="231" t="s">
+      <c r="E55" s="229" t="s">
         <v>1083</v>
       </c>
       <c r="F55" s="39" t="s">
@@ -40248,7 +40286,7 @@
       <c r="I55" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J55" s="244"/>
+      <c r="J55" s="243"/>
       <c r="K55" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40263,21 +40301,21 @@
       <c r="C56" s="51" t="s">
         <v>1084</v>
       </c>
-      <c r="D56" s="232" t="s">
+      <c r="D56" s="230" t="s">
         <v>1085</v>
       </c>
-      <c r="E56" s="229" t="s">
+      <c r="E56" s="227" t="s">
         <v>1086</v>
       </c>
-      <c r="F56" s="232"/>
+      <c r="F56" s="230"/>
       <c r="G56" s="130" t="s">
         <v>73</v>
       </c>
-      <c r="H56" s="217">
+      <c r="H56" s="215">
         <v>0</v>
       </c>
       <c r="I56" s="84"/>
-      <c r="J56" s="244"/>
+      <c r="J56" s="243"/>
       <c r="K56" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40295,7 +40333,7 @@
       <c r="D57" s="39" t="s">
         <v>1088</v>
       </c>
-      <c r="E57" s="231" t="s">
+      <c r="E57" s="229" t="s">
         <v>1089</v>
       </c>
       <c r="F57" s="39" t="s">
@@ -40310,8 +40348,8 @@
       <c r="I57" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="J57" s="244"/>
-      <c r="K57" s="215" t="s">
+      <c r="J57" s="243"/>
+      <c r="K57" s="213" t="s">
         <v>1063</v>
       </c>
       <c r="L57" s="39" t="s">
@@ -40334,25 +40372,25 @@
       <c r="C58" s="50" t="s">
         <v>1090</v>
       </c>
-      <c r="D58" s="233" t="s">
+      <c r="D58" s="231" t="s">
         <v>1091</v>
       </c>
-      <c r="E58" s="230" t="s">
+      <c r="E58" s="228" t="s">
         <v>1092</v>
       </c>
-      <c r="F58" s="233" t="s">
+      <c r="F58" s="231" t="s">
         <v>917</v>
       </c>
-      <c r="G58" s="219" t="s">
+      <c r="G58" s="217" t="s">
         <v>94</v>
       </c>
-      <c r="H58" s="220">
+      <c r="H58" s="218">
         <v>0</v>
       </c>
       <c r="I58" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J58" s="241" t="s">
+      <c r="J58" s="240" t="s">
         <v>274</v>
       </c>
       <c r="K58" s="129" t="s">
@@ -40372,7 +40410,7 @@
       <c r="D59" s="39" t="s">
         <v>1094</v>
       </c>
-      <c r="E59" s="231" t="s">
+      <c r="E59" s="229" t="s">
         <v>1095</v>
       </c>
       <c r="F59" s="39" t="s">
@@ -40387,7 +40425,7 @@
       <c r="I59" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J59" s="241"/>
+      <c r="J59" s="240"/>
       <c r="K59" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40405,7 +40443,7 @@
       <c r="D60" s="39" t="s">
         <v>1097</v>
       </c>
-      <c r="E60" s="231" t="s">
+      <c r="E60" s="229" t="s">
         <v>1098</v>
       </c>
       <c r="F60" s="39" t="s">
@@ -40420,7 +40458,7 @@
       <c r="I60" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J60" s="241"/>
+      <c r="J60" s="240"/>
       <c r="K60" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40438,7 +40476,7 @@
       <c r="D61" s="39" t="s">
         <v>1100</v>
       </c>
-      <c r="E61" s="231" t="s">
+      <c r="E61" s="229" t="s">
         <v>1101</v>
       </c>
       <c r="F61" s="39" t="s">
@@ -40453,7 +40491,7 @@
       <c r="I61" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J61" s="241"/>
+      <c r="J61" s="240"/>
       <c r="K61" s="133" t="s">
         <v>66</v>
       </c>
@@ -40486,7 +40524,7 @@
       <c r="I62" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J62" s="241"/>
+      <c r="J62" s="240"/>
       <c r="K62" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40504,7 +40542,7 @@
       <c r="D63" s="39" t="s">
         <v>1105</v>
       </c>
-      <c r="E63" s="231" t="s">
+      <c r="E63" s="229" t="s">
         <v>1106</v>
       </c>
       <c r="F63" s="39" t="s">
@@ -40519,7 +40557,7 @@
       <c r="I63" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J63" s="241"/>
+      <c r="J63" s="240"/>
       <c r="K63" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40552,7 +40590,7 @@
       <c r="I64" s="39" t="s">
         <v>939</v>
       </c>
-      <c r="J64" s="241"/>
+      <c r="J64" s="240"/>
       <c r="K64" s="133" t="s">
         <v>1109</v>
       </c>
@@ -40570,7 +40608,7 @@
       <c r="D65" s="39" t="s">
         <v>1111</v>
       </c>
-      <c r="E65" s="231" t="s">
+      <c r="E65" s="229" t="s">
         <v>1112</v>
       </c>
       <c r="F65" s="39" t="s">
@@ -40585,7 +40623,7 @@
       <c r="I65" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J65" s="241"/>
+      <c r="J65" s="240"/>
       <c r="K65" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40598,23 +40636,23 @@
       <c r="C66" s="51" t="s">
         <v>1113</v>
       </c>
-      <c r="D66" s="232" t="s">
+      <c r="D66" s="230" t="s">
         <v>1114</v>
       </c>
-      <c r="E66" s="229" t="s">
+      <c r="E66" s="227" t="s">
         <v>1115</v>
       </c>
-      <c r="F66" s="232" t="s">
+      <c r="F66" s="230" t="s">
         <v>917</v>
       </c>
       <c r="G66" s="130" t="s">
         <v>73</v>
       </c>
-      <c r="H66" s="218">
+      <c r="H66" s="216">
         <v>60</v>
       </c>
       <c r="I66" s="39"/>
-      <c r="J66" s="241"/>
+      <c r="J66" s="240"/>
       <c r="K66" s="129" t="s">
         <v>1063</v>
       </c>
@@ -40643,8 +40681,8 @@
         <v>30</v>
       </c>
       <c r="I67" s="39"/>
-      <c r="J67" s="241"/>
-      <c r="K67" s="216" t="s">
+      <c r="J67" s="240"/>
+      <c r="K67" s="214" t="s">
         <v>1119</v>
       </c>
       <c r="L67" s="39" t="s">
@@ -40664,19 +40702,19 @@
       <c r="B68" s="57" t="s">
         <v>271</v>
       </c>
-      <c r="C68" s="230" t="s">
+      <c r="C68" s="228" t="s">
         <v>1120</v>
       </c>
-      <c r="D68" s="233" t="s">
+      <c r="D68" s="231" t="s">
         <v>1121</v>
       </c>
-      <c r="E68" s="230" t="s">
+      <c r="E68" s="228" t="s">
         <v>1122</v>
       </c>
-      <c r="F68" s="233" t="s">
+      <c r="F68" s="231" t="s">
         <v>917</v>
       </c>
-      <c r="G68" s="221" t="s">
+      <c r="G68" s="219" t="s">
         <v>5</v>
       </c>
       <c r="H68" s="134">
@@ -40685,7 +40723,7 @@
       <c r="I68" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J68" s="241"/>
+      <c r="J68" s="240"/>
       <c r="K68" s="133" t="s">
         <v>1123</v>
       </c>
@@ -40712,7 +40750,7 @@
       <c r="D69" s="39" t="s">
         <v>1125</v>
       </c>
-      <c r="E69" s="231" t="s">
+      <c r="E69" s="229" t="s">
         <v>1126</v>
       </c>
       <c r="F69" s="39" t="s">
@@ -40727,7 +40765,7 @@
       <c r="I69" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J69" s="241"/>
+      <c r="J69" s="240"/>
       <c r="K69" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40745,7 +40783,7 @@
       <c r="D70" s="39" t="s">
         <v>1128</v>
       </c>
-      <c r="E70" s="231" t="s">
+      <c r="E70" s="229" t="s">
         <v>1129</v>
       </c>
       <c r="F70" s="39" t="s">
@@ -40760,7 +40798,7 @@
       <c r="I70" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J70" s="241"/>
+      <c r="J70" s="240"/>
       <c r="K70" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40778,7 +40816,7 @@
       <c r="D71" s="39" t="s">
         <v>1131</v>
       </c>
-      <c r="E71" s="231" t="s">
+      <c r="E71" s="229" t="s">
         <v>1132</v>
       </c>
       <c r="F71" s="39" t="s">
@@ -40793,7 +40831,7 @@
       <c r="I71" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J71" s="241"/>
+      <c r="J71" s="240"/>
       <c r="K71" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40811,7 +40849,7 @@
       <c r="D72" s="39" t="s">
         <v>1134</v>
       </c>
-      <c r="E72" s="231" t="s">
+      <c r="E72" s="229" t="s">
         <v>1133</v>
       </c>
       <c r="F72" s="39" t="s">
@@ -40826,7 +40864,7 @@
       <c r="I72" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J72" s="241"/>
+      <c r="J72" s="240"/>
       <c r="K72" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40844,7 +40882,7 @@
       <c r="D73" s="39" t="s">
         <v>1136</v>
       </c>
-      <c r="E73" s="231" t="s">
+      <c r="E73" s="229" t="s">
         <v>1137</v>
       </c>
       <c r="F73" s="39" t="s">
@@ -40859,7 +40897,7 @@
       <c r="I73" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="J73" s="241"/>
+      <c r="J73" s="240"/>
       <c r="K73" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40871,13 +40909,13 @@
       <c r="B74" s="51" t="s">
         <v>271</v>
       </c>
-      <c r="C74" s="231" t="s">
+      <c r="C74" s="229" t="s">
         <v>1138</v>
       </c>
       <c r="D74" s="39" t="s">
         <v>1139</v>
       </c>
-      <c r="E74" s="231" t="s">
+      <c r="E74" s="229" t="s">
         <v>1140</v>
       </c>
       <c r="F74" s="39" t="s">
@@ -40890,7 +40928,7 @@
         <v>20</v>
       </c>
       <c r="I74" s="44"/>
-      <c r="J74" s="241"/>
+      <c r="J74" s="240"/>
       <c r="K74" s="133" t="s">
         <v>1063</v>
       </c>
@@ -40900,21 +40938,21 @@
         <v>70</v>
       </c>
       <c r="B75" s="202"/>
-      <c r="C75" s="231"/>
+      <c r="C75" s="229"/>
       <c r="D75" s="39"/>
-      <c r="E75" s="231"/>
+      <c r="E75" s="229"/>
       <c r="F75" s="39"/>
       <c r="G75" s="83"/>
       <c r="H75" s="36"/>
       <c r="I75" s="44"/>
-      <c r="J75" s="241"/>
+      <c r="J75" s="240"/>
       <c r="K75" s="69"/>
     </row>
     <row r="76" spans="1:14" s="2" customFormat="1" ht="39.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="36">
         <v>71</v>
       </c>
-      <c r="B76" s="228" t="s">
+      <c r="B76" s="226" t="s">
         <v>1141</v>
       </c>
       <c r="C76" s="4" t="s">
@@ -40948,7 +40986,7 @@
       <c r="A77" s="36">
         <v>72</v>
       </c>
-      <c r="B77" s="231" t="s">
+      <c r="B77" s="229" t="s">
         <v>278</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -40957,7 +40995,7 @@
       <c r="D77" s="39" t="s">
         <v>279</v>
       </c>
-      <c r="E77" s="231" t="s">
+      <c r="E77" s="229" t="s">
         <v>280</v>
       </c>
       <c r="F77" s="39" t="s">
@@ -40987,17 +41025,17 @@
       <c r="C78" s="51" t="s">
         <v>1146</v>
       </c>
-      <c r="D78" s="232" t="s">
+      <c r="D78" s="230" t="s">
         <v>282</v>
       </c>
-      <c r="E78" s="229" t="s">
+      <c r="E78" s="227" t="s">
         <v>283</v>
       </c>
       <c r="F78" s="198"/>
       <c r="G78" s="187" t="s">
         <v>94</v>
       </c>
-      <c r="H78" s="232"/>
+      <c r="H78" s="230"/>
       <c r="I78" s="44"/>
       <c r="J78" s="44"/>
       <c r="K78" s="44"/>
@@ -41050,7 +41088,7 @@
       <c r="D80" s="39" t="s">
         <v>1911</v>
       </c>
-      <c r="E80" s="231"/>
+      <c r="E80" s="229"/>
       <c r="F80" s="39"/>
       <c r="G80" s="39" t="s">
         <v>5</v>
@@ -41204,11 +41242,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -41230,19 +41267,23 @@
     <col min="15" max="16384" width="9.1796875" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="235" t="s">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="256" t="s">
         <v>1147</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="238"/>
+      <c r="B1" s="256"/>
+      <c r="C1" s="256"/>
+      <c r="D1" s="256"/>
+      <c r="E1" s="256"/>
+      <c r="F1" s="256"/>
+      <c r="G1" s="256"/>
+      <c r="H1" s="256"/>
+      <c r="I1" s="257"/>
+      <c r="J1" s="257"/>
+      <c r="K1" s="256"/>
+      <c r="L1" s="256"/>
+      <c r="M1" s="256"/>
+      <c r="N1" s="256"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -41275,16 +41316,16 @@
       <c r="J2" s="7" t="s">
         <v>886</v>
       </c>
-      <c r="K2" s="179" t="s">
+      <c r="K2" s="258" t="s">
         <v>1148</v>
       </c>
-      <c r="L2" s="63" t="s">
+      <c r="L2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="8" t="s">
         <v>1941</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="N2" s="10" t="s">
         <v>1358</v>
       </c>
     </row>
@@ -41319,7 +41360,7 @@
       <c r="J3" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K3" s="212" t="s">
+      <c r="K3" s="163" t="s">
         <v>1931</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -41363,7 +41404,7 @@
       <c r="J4" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K4" s="212" t="s">
+      <c r="K4" s="163" t="s">
         <v>1155</v>
       </c>
       <c r="L4" s="39" t="s">
@@ -41376,7 +41417,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="42" x14ac:dyDescent="0.35">
       <c r="A5" s="161">
         <v>3</v>
       </c>
@@ -41407,14 +41448,17 @@
       <c r="J5" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K5" s="212" t="s">
+      <c r="K5" s="163" t="s">
         <v>1159</v>
       </c>
       <c r="L5" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="M5" s="41" t="s">
+      <c r="M5" s="39" t="s">
         <v>1943</v>
+      </c>
+      <c r="N5" s="36" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="126" x14ac:dyDescent="0.35">
@@ -41448,7 +41492,7 @@
       <c r="J6" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K6" s="212" t="s">
+      <c r="K6" s="163" t="s">
         <v>1163</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -41492,14 +41536,14 @@
       <c r="J7" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K7" s="212" t="s">
+      <c r="K7" s="163" t="s">
         <v>1167</v>
       </c>
       <c r="L7" s="39" t="s">
         <v>1872</v>
       </c>
       <c r="M7" s="39" t="s">
-        <v>1943</v>
+        <v>1988</v>
       </c>
       <c r="N7" s="36" t="s">
         <v>1960</v>
@@ -41536,7 +41580,7 @@
       <c r="J8" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K8" s="212" t="s">
+      <c r="K8" s="163" t="s">
         <v>1932</v>
       </c>
       <c r="L8" s="39" t="s">
@@ -41580,20 +41624,20 @@
       <c r="J9" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K9" s="212" t="s">
+      <c r="K9" s="163" t="s">
         <v>1172</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>1872</v>
       </c>
       <c r="M9" s="39" t="s">
-        <v>1943</v>
+        <v>1988</v>
       </c>
       <c r="N9" s="36" t="s">
         <v>1960</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="140" x14ac:dyDescent="0.35">
       <c r="A10" s="161">
         <v>8</v>
       </c>
@@ -41624,12 +41668,18 @@
       <c r="J10" s="166" t="s">
         <v>1175</v>
       </c>
-      <c r="K10" s="212" t="s">
+      <c r="K10" s="163" t="s">
         <v>1176</v>
       </c>
       <c r="L10" s="39"/>
-    </row>
-    <row r="11" spans="1:14" s="2" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M10" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N10" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A11" s="161">
         <v>9</v>
       </c>
@@ -41658,10 +41708,16 @@
       <c r="J11" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K11" s="160"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="39"/>
-    </row>
-    <row r="12" spans="1:14" s="2" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M11" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N11" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A12" s="161">
         <v>10</v>
       </c>
@@ -41690,10 +41746,16 @@
       <c r="J12" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K12" s="160"/>
+      <c r="K12" s="45"/>
       <c r="L12" s="39"/>
-    </row>
-    <row r="13" spans="1:14" s="2" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M12" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N12" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="2" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A13" s="161">
         <v>11</v>
       </c>
@@ -41722,10 +41784,16 @@
       <c r="J13" s="163" t="s">
         <v>305</v>
       </c>
-      <c r="K13" s="160"/>
+      <c r="K13" s="45"/>
       <c r="L13" s="39"/>
-    </row>
-    <row r="14" spans="1:14" ht="378" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M13" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N13" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="378" x14ac:dyDescent="0.35">
       <c r="A14" s="161">
         <v>12</v>
       </c>
@@ -41756,17 +41824,20 @@
       <c r="J14" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K14" s="212" t="s">
+      <c r="K14" s="163" t="s">
         <v>1181</v>
       </c>
       <c r="L14" s="39" t="s">
         <v>1871</v>
       </c>
-      <c r="M14" s="41" t="s">
+      <c r="M14" s="39" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="N14" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="42" x14ac:dyDescent="0.35">
       <c r="A15" s="161">
         <v>13</v>
       </c>
@@ -41797,15 +41868,18 @@
       <c r="J15" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K15" s="213"/>
+      <c r="K15" s="45"/>
       <c r="L15" s="39" t="s">
         <v>802</v>
       </c>
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="39" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="56" hidden="1" x14ac:dyDescent="0.35">
+      <c r="N15" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="56" x14ac:dyDescent="0.35">
       <c r="A16" s="161">
         <v>14</v>
       </c>
@@ -41836,15 +41910,18 @@
       <c r="J16" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K16" s="213"/>
+      <c r="K16" s="45"/>
       <c r="L16" s="39" t="s">
         <v>1869</v>
       </c>
-      <c r="M16" s="41" t="s">
+      <c r="M16" s="39" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N16" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="150.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="161">
         <v>15</v>
       </c>
@@ -41875,17 +41952,20 @@
       <c r="J17" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K17" s="212" t="s">
+      <c r="K17" s="163" t="s">
         <v>1185</v>
       </c>
       <c r="L17" s="39" t="s">
         <v>1871</v>
       </c>
-      <c r="M17" s="41" t="s">
-        <v>1944</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M17" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N17" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="2" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A18" s="161">
         <v>16</v>
       </c>
@@ -41914,8 +41994,14 @@
       <c r="J18" s="163" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="160"/>
+      <c r="K18" s="45"/>
       <c r="L18" s="39"/>
+      <c r="M18" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N18" s="36" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="150" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="161">
@@ -41946,20 +42032,20 @@
       <c r="J19" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K19" s="212" t="s">
+      <c r="K19" s="163" t="s">
         <v>1188</v>
       </c>
       <c r="L19" s="39" t="s">
         <v>1872</v>
       </c>
       <c r="M19" s="39" t="s">
-        <v>1945</v>
+        <v>1988</v>
       </c>
       <c r="N19" s="36" t="s">
         <v>1960</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A20" s="161">
         <v>18</v>
       </c>
@@ -41988,10 +42074,16 @@
       <c r="J20" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K20" s="160"/>
+      <c r="K20" s="45"/>
       <c r="L20" s="39"/>
-    </row>
-    <row r="21" spans="1:14" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M20" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N20" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="161">
         <v>19</v>
       </c>
@@ -42010,10 +42102,16 @@
       <c r="J21" s="163" t="s">
         <v>902</v>
       </c>
-      <c r="K21" s="160"/>
+      <c r="K21" s="45"/>
       <c r="L21" s="39"/>
-    </row>
-    <row r="22" spans="1:14" s="2" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M21" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N21" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="2" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A22" s="161">
         <v>20</v>
       </c>
@@ -42042,10 +42140,16 @@
       <c r="J22" s="163" t="s">
         <v>66</v>
       </c>
-      <c r="K22" s="160"/>
+      <c r="K22" s="45"/>
       <c r="L22" s="39"/>
-    </row>
-    <row r="23" spans="1:14" s="2" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M22" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N22" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A23" s="161">
         <v>21</v>
       </c>
@@ -42074,10 +42178,16 @@
       <c r="J23" s="163" t="s">
         <v>349</v>
       </c>
-      <c r="K23" s="160"/>
+      <c r="K23" s="45"/>
       <c r="L23" s="39"/>
-    </row>
-    <row r="24" spans="1:14" s="2" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M23" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N23" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A24" s="170">
         <v>22</v>
       </c>
@@ -42106,10 +42216,14 @@
       <c r="J24" s="173" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="160"/>
+      <c r="K24" s="45"/>
       <c r="L24" s="39"/>
-    </row>
-    <row r="25" spans="1:14" s="2" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M24" s="39"/>
+      <c r="N24" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="2" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A25" s="161">
         <v>23</v>
       </c>
@@ -42138,10 +42252,16 @@
       <c r="J25" s="166" t="s">
         <v>1198</v>
       </c>
-      <c r="K25" s="160"/>
+      <c r="K25" s="45"/>
       <c r="L25" s="39"/>
-    </row>
-    <row r="26" spans="1:14" s="2" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M25" s="39" t="s">
+        <v>1944</v>
+      </c>
+      <c r="N25" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="2" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A26" s="161">
         <v>24</v>
       </c>
@@ -42170,10 +42290,16 @@
       <c r="J26" s="163" t="s">
         <v>349</v>
       </c>
-      <c r="K26" s="160"/>
+      <c r="K26" s="45"/>
       <c r="L26" s="39"/>
-    </row>
-    <row r="27" spans="1:14" ht="252" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M26" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N26" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="252" x14ac:dyDescent="0.35">
       <c r="A27" s="161">
         <v>25</v>
       </c>
@@ -42204,17 +42330,20 @@
       <c r="J27" s="163" t="s">
         <v>349</v>
       </c>
-      <c r="K27" s="212" t="s">
+      <c r="K27" s="163" t="s">
         <v>1201</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>1869</v>
       </c>
-      <c r="M27" s="41" t="s">
-        <v>1944</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="2" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M27" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N27" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A28" s="170">
         <v>26</v>
       </c>
@@ -42243,10 +42372,16 @@
       <c r="J28" s="169" t="s">
         <v>1206</v>
       </c>
-      <c r="K28" s="160"/>
+      <c r="K28" s="45"/>
       <c r="L28" s="39"/>
-    </row>
-    <row r="29" spans="1:14" s="2" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M28" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="N28" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A29" s="170">
         <v>27</v>
       </c>
@@ -42275,10 +42410,16 @@
       <c r="J29" s="169" t="s">
         <v>1206</v>
       </c>
-      <c r="K29" s="160"/>
+      <c r="K29" s="45"/>
       <c r="L29" s="39"/>
-    </row>
-    <row r="30" spans="1:14" s="2" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M29" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="N29" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A30" s="170">
         <v>28</v>
       </c>
@@ -42305,10 +42446,16 @@
       <c r="J30" s="169" t="s">
         <v>1206</v>
       </c>
-      <c r="K30" s="160"/>
+      <c r="K30" s="45"/>
       <c r="L30" s="39"/>
-    </row>
-    <row r="31" spans="1:14" s="2" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M30" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="N30" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="2" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A31" s="161">
         <v>29</v>
       </c>
@@ -42337,10 +42484,16 @@
       <c r="J31" s="163" t="s">
         <v>349</v>
       </c>
-      <c r="K31" s="160"/>
+      <c r="K31" s="45"/>
       <c r="L31" s="39"/>
-    </row>
-    <row r="32" spans="1:14" s="2" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M31" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N31" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="2" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A32" s="161">
         <v>30</v>
       </c>
@@ -42365,10 +42518,16 @@
       <c r="J32" s="163" t="s">
         <v>353</v>
       </c>
-      <c r="K32" s="160"/>
+      <c r="K32" s="45"/>
       <c r="L32" s="39"/>
-    </row>
-    <row r="33" spans="1:14" s="2" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M32" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N32" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="2" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A33" s="161">
         <v>31</v>
       </c>
@@ -42393,8 +42552,14 @@
       <c r="J33" s="163" t="s">
         <v>357</v>
       </c>
-      <c r="K33" s="160"/>
+      <c r="K33" s="45"/>
       <c r="L33" s="39"/>
+      <c r="M33" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N33" s="36" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="34" spans="1:14" ht="154" x14ac:dyDescent="0.35">
       <c r="A34" s="161">
@@ -42423,7 +42588,7 @@
       </c>
       <c r="I34" s="160"/>
       <c r="J34" s="163"/>
-      <c r="K34" s="212" t="s">
+      <c r="K34" s="210" t="s">
         <v>1219</v>
       </c>
       <c r="L34" s="39" t="s">
@@ -42436,7 +42601,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" ht="28" x14ac:dyDescent="0.35">
       <c r="A35" s="161">
         <v>33</v>
       </c>
@@ -42463,26 +42628,29 @@
       </c>
       <c r="I35" s="163"/>
       <c r="J35" s="163"/>
-      <c r="K35" s="213"/>
+      <c r="K35" s="211"/>
       <c r="L35" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="M35" s="41" t="s">
+      <c r="M35" s="39" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="N35" s="36" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="42" x14ac:dyDescent="0.35">
       <c r="A36" s="184">
         <v>34</v>
       </c>
       <c r="B36" s="185" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="186" t="s">
-        <v>73</v>
+      <c r="C36" s="185" t="s">
+        <v>113</v>
       </c>
       <c r="D36" s="186" t="s">
-        <v>73</v>
+        <v>1990</v>
       </c>
       <c r="E36" s="186" t="s">
         <v>114</v>
@@ -42498,14 +42666,17 @@
       </c>
       <c r="I36" s="163"/>
       <c r="J36" s="187"/>
-      <c r="K36" s="214" t="s">
+      <c r="K36" s="212" t="s">
         <v>1222</v>
       </c>
       <c r="L36" s="39" t="s">
         <v>1871</v>
       </c>
-      <c r="M36" s="41" t="s">
-        <v>1944</v>
+      <c r="M36" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N36" s="36" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="28" x14ac:dyDescent="0.35">
@@ -42535,12 +42706,12 @@
       </c>
       <c r="I37" s="160"/>
       <c r="J37" s="163"/>
-      <c r="K37" s="213"/>
+      <c r="K37" s="211"/>
       <c r="L37" s="39" t="s">
         <v>1872</v>
       </c>
       <c r="M37" s="39" t="s">
-        <v>1945</v>
+        <v>1988</v>
       </c>
       <c r="N37" s="36" t="s">
         <v>1960</v>
@@ -42573,7 +42744,7 @@
       </c>
       <c r="I38" s="160"/>
       <c r="J38" s="163"/>
-      <c r="K38" s="213" t="s">
+      <c r="K38" s="211" t="s">
         <v>1858</v>
       </c>
       <c r="L38" s="39" t="s">
@@ -42590,7 +42761,7 @@
       <c r="A39" s="36">
         <v>37</v>
       </c>
-      <c r="B39" s="208" t="s">
+      <c r="B39" s="232" t="s">
         <v>1917</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -42629,7 +42800,7 @@
       <c r="A40" s="36">
         <v>38</v>
       </c>
-      <c r="B40" s="208" t="s">
+      <c r="B40" s="232" t="s">
         <v>1923</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -42656,7 +42827,7 @@
         <v>1872</v>
       </c>
       <c r="M40" s="39" t="s">
-        <v>1945</v>
+        <v>1988</v>
       </c>
       <c r="N40" s="36" t="s">
         <v>1960</v>
@@ -42666,7 +42837,7 @@
       <c r="A41" s="36">
         <v>39</v>
       </c>
-      <c r="B41" s="208" t="s">
+      <c r="B41" s="232" t="s">
         <v>1927</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -42703,7 +42874,7 @@
       <c r="A42" s="36">
         <v>40</v>
       </c>
-      <c r="B42" s="211" t="s">
+      <c r="B42" s="232" t="s">
         <v>1936</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -42730,35 +42901,90 @@
         <v>1872</v>
       </c>
       <c r="M42" s="39" t="s">
-        <v>1945</v>
+        <v>1988</v>
       </c>
       <c r="N42" s="36" t="s">
         <v>1960</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="I43" s="41"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="I44" s="41"/>
+    <row r="43" spans="1:14" ht="42" x14ac:dyDescent="0.35">
+      <c r="A43" s="36">
+        <v>41</v>
+      </c>
+      <c r="B43" s="232" t="s">
+        <v>1991</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>1992</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>917</v>
+      </c>
+      <c r="G43" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="36" t="s">
+        <v>474</v>
+      </c>
+      <c r="I43" s="39"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="39" t="s">
+        <v>1872</v>
+      </c>
+      <c r="M43" s="39" t="s">
+        <v>1944</v>
+      </c>
+      <c r="N43" s="36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="28" x14ac:dyDescent="0.35">
+      <c r="A44" s="36">
+        <v>42</v>
+      </c>
+      <c r="B44" s="232" t="s">
+        <v>1994</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>1995</v>
+      </c>
+      <c r="D44" s="39" t="s">
+        <v>1996</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>1995</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>917</v>
+      </c>
+      <c r="G44" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="36" t="s">
+        <v>474</v>
+      </c>
+      <c r="I44" s="39"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39" t="s">
+        <v>1869</v>
+      </c>
+      <c r="M44" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N44" s="36" t="s">
+        <v>474</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:L42" xr:uid="{9E26C98F-F63D-4634-AED6-5AE6EA2A8036}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Vital"/>
-        <filter val="Vital?"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="11">
-      <filters>
-        <filter val="P1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
-  </mergeCells>
+  <autoFilter ref="A2:L42" xr:uid="{9E26C98F-F63D-4634-AED6-5AE6EA2A8036}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -42795,18 +43021,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="247" t="s">
+      <c r="A1" s="246" t="s">
         <v>1223</v>
       </c>
-      <c r="B1" s="248"/>
-      <c r="C1" s="248"/>
-      <c r="D1" s="248"/>
-      <c r="E1" s="249"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="247"/>
-      <c r="H1" s="249"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="250"/>
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="247"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="248"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="249"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -43013,7 +43239,7 @@
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="36"/>
-      <c r="B7" s="242" t="s">
+      <c r="B7" s="241" t="s">
         <v>373</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -43049,7 +43275,7 @@
     </row>
     <row r="8" spans="1:14" ht="28" x14ac:dyDescent="0.35">
       <c r="A8" s="36"/>
-      <c r="B8" s="245"/>
+      <c r="B8" s="244"/>
       <c r="C8" s="4" t="s">
         <v>1969</v>
       </c>
@@ -43085,7 +43311,7 @@
       <c r="A9" s="36">
         <v>5</v>
       </c>
-      <c r="B9" s="245"/>
+      <c r="B9" s="244"/>
       <c r="C9" s="4" t="s">
         <v>1948</v>
       </c>
@@ -43122,7 +43348,7 @@
       <c r="A10" s="36">
         <v>6</v>
       </c>
-      <c r="B10" s="245"/>
+      <c r="B10" s="244"/>
       <c r="C10" s="4" t="s">
         <v>1230</v>
       </c>
@@ -43156,7 +43382,7 @@
       <c r="A11" s="36">
         <v>7</v>
       </c>
-      <c r="B11" s="245"/>
+      <c r="B11" s="244"/>
       <c r="C11" s="4" t="s">
         <v>1233</v>
       </c>
@@ -43190,7 +43416,7 @@
       <c r="A12" s="36">
         <v>8</v>
       </c>
-      <c r="B12" s="245"/>
+      <c r="B12" s="244"/>
       <c r="C12" s="4" t="s">
         <v>1949</v>
       </c>
@@ -43227,7 +43453,7 @@
       <c r="A13" s="36">
         <v>9</v>
       </c>
-      <c r="B13" s="245"/>
+      <c r="B13" s="244"/>
       <c r="C13" s="4" t="s">
         <v>1950</v>
       </c>
@@ -43256,7 +43482,7 @@
       <c r="L13" s="4" t="s">
         <v>1873</v>
       </c>
-      <c r="M13" s="223" t="s">
+      <c r="M13" s="221" t="s">
         <v>1956</v>
       </c>
     </row>
@@ -43264,7 +43490,7 @@
       <c r="A14" s="36">
         <v>10</v>
       </c>
-      <c r="B14" s="245"/>
+      <c r="B14" s="244"/>
       <c r="C14" s="4" t="s">
         <v>1951</v>
       </c>
@@ -43293,7 +43519,7 @@
       <c r="L14" s="4" t="s">
         <v>1873</v>
       </c>
-      <c r="M14" s="223" t="s">
+      <c r="M14" s="221" t="s">
         <v>1956</v>
       </c>
     </row>
@@ -43301,7 +43527,7 @@
       <c r="A15" s="36">
         <v>11</v>
       </c>
-      <c r="B15" s="245"/>
+      <c r="B15" s="244"/>
       <c r="C15" s="4" t="s">
         <v>1952</v>
       </c>
@@ -43330,7 +43556,7 @@
       <c r="L15" s="4" t="s">
         <v>1873</v>
       </c>
-      <c r="M15" s="223" t="s">
+      <c r="M15" s="221" t="s">
         <v>1956</v>
       </c>
     </row>
@@ -43338,7 +43564,7 @@
       <c r="A16" s="36">
         <v>12</v>
       </c>
-      <c r="B16" s="243"/>
+      <c r="B16" s="242"/>
       <c r="C16" s="4" t="s">
         <v>1953</v>
       </c>
@@ -43367,7 +43593,7 @@
       <c r="L16" s="4" t="s">
         <v>1873</v>
       </c>
-      <c r="M16" s="223" t="s">
+      <c r="M16" s="221" t="s">
         <v>1956</v>
       </c>
     </row>
@@ -43618,7 +43844,7 @@
       <c r="L23" s="4" t="s">
         <v>1873</v>
       </c>
-      <c r="M23" s="222" t="s">
+      <c r="M23" s="220" t="s">
         <v>1955</v>
       </c>
     </row>
@@ -43626,7 +43852,7 @@
       <c r="A24" s="36">
         <v>20</v>
       </c>
-      <c r="B24" s="244" t="s">
+      <c r="B24" s="243" t="s">
         <v>399</v>
       </c>
       <c r="C24" s="22" t="s">
@@ -43662,7 +43888,7 @@
       <c r="A25" s="56">
         <v>21</v>
       </c>
-      <c r="B25" s="251"/>
+      <c r="B25" s="250"/>
       <c r="C25" s="59" t="s">
         <v>1256</v>
       </c>
@@ -43694,7 +43920,7 @@
       <c r="A26" s="36">
         <v>22</v>
       </c>
-      <c r="B26" s="252"/>
+      <c r="B26" s="251"/>
       <c r="C26" s="22" t="s">
         <v>1259</v>
       </c>
@@ -43726,7 +43952,7 @@
       <c r="A27" s="36">
         <v>23</v>
       </c>
-      <c r="B27" s="252"/>
+      <c r="B27" s="251"/>
       <c r="C27" s="22" t="s">
         <v>1262</v>
       </c>
@@ -43758,7 +43984,7 @@
       <c r="A28" s="56">
         <v>24</v>
       </c>
-      <c r="B28" s="251"/>
+      <c r="B28" s="250"/>
       <c r="C28" s="59" t="s">
         <v>1265</v>
       </c>
@@ -43790,7 +44016,7 @@
       <c r="A29" s="36">
         <v>25</v>
       </c>
-      <c r="B29" s="252"/>
+      <c r="B29" s="251"/>
       <c r="C29" s="22" t="s">
         <v>1268</v>
       </c>
@@ -43894,7 +44120,7 @@
       <c r="A32" s="36">
         <v>28</v>
       </c>
-      <c r="B32" s="244" t="s">
+      <c r="B32" s="243" t="s">
         <v>409</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -43930,7 +44156,7 @@
       <c r="A33" s="36">
         <v>29</v>
       </c>
-      <c r="B33" s="252"/>
+      <c r="B33" s="251"/>
       <c r="C33" s="4" t="s">
         <v>1276</v>
       </c>
@@ -43964,7 +44190,7 @@
       <c r="A34" s="36">
         <v>30</v>
       </c>
-      <c r="B34" s="252"/>
+      <c r="B34" s="251"/>
       <c r="C34" s="4" t="s">
         <v>1279</v>
       </c>
@@ -43998,7 +44224,7 @@
       <c r="A35" s="36">
         <v>31</v>
       </c>
-      <c r="B35" s="252"/>
+      <c r="B35" s="251"/>
       <c r="C35" s="4" t="s">
         <v>1282</v>
       </c>
@@ -44270,7 +44496,7 @@
       <c r="A42" s="58">
         <v>37</v>
       </c>
-      <c r="B42" s="245" t="s">
+      <c r="B42" s="244" t="s">
         <v>428</v>
       </c>
       <c r="C42" s="50" t="s">
@@ -44302,7 +44528,7 @@
       <c r="A43" s="36">
         <v>38</v>
       </c>
-      <c r="B43" s="251"/>
+      <c r="B43" s="250"/>
       <c r="C43" s="4" t="s">
         <v>1294</v>
       </c>
@@ -44332,7 +44558,7 @@
       <c r="A44" s="52">
         <v>39</v>
       </c>
-      <c r="B44" s="251"/>
+      <c r="B44" s="250"/>
       <c r="C44" s="51" t="s">
         <v>1297</v>
       </c>
@@ -44360,7 +44586,7 @@
     </row>
     <row r="45" spans="1:14" ht="116.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="36"/>
-      <c r="B45" s="246" t="s">
+      <c r="B45" s="245" t="s">
         <v>1300</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -44402,7 +44628,7 @@
     </row>
     <row r="46" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="36"/>
-      <c r="B46" s="246"/>
+      <c r="B46" s="245"/>
       <c r="C46" s="4" t="s">
         <v>1304</v>
       </c>
@@ -44436,7 +44662,7 @@
     </row>
     <row r="47" spans="1:14" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="36"/>
-      <c r="B47" s="246"/>
+      <c r="B47" s="245"/>
       <c r="C47" s="4" t="s">
         <v>1307</v>
       </c>
@@ -44470,7 +44696,7 @@
     </row>
     <row r="48" spans="1:14" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="36"/>
-      <c r="B48" s="246" t="s">
+      <c r="B48" s="245" t="s">
         <v>435</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -44506,7 +44732,7 @@
     </row>
     <row r="49" spans="1:14" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="36"/>
-      <c r="B49" s="246"/>
+      <c r="B49" s="245"/>
       <c r="C49" s="4" t="s">
         <v>1313</v>
       </c>
@@ -44540,7 +44766,7 @@
     </row>
     <row r="50" spans="1:14" ht="42" x14ac:dyDescent="0.35">
       <c r="A50" s="52"/>
-      <c r="B50" s="227" t="s">
+      <c r="B50" s="225" t="s">
         <v>1863</v>
       </c>
       <c r="C50" s="51" t="s">
@@ -44549,10 +44775,10 @@
       <c r="D50" s="198" t="s">
         <v>1862</v>
       </c>
-      <c r="E50" s="226" t="s">
+      <c r="E50" s="224" t="s">
         <v>1865</v>
       </c>
-      <c r="G50" s="226" t="s">
+      <c r="G50" s="224" t="s">
         <v>1861</v>
       </c>
       <c r="H50" s="52"/>
@@ -45290,18 +45516,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="234" t="s">
         <v>1866</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="238"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="237"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -45392,7 +45618,7 @@
       <c r="A4" s="36">
         <v>40</v>
       </c>
-      <c r="B4" s="242" t="s">
+      <c r="B4" s="241" t="s">
         <v>431</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -45432,7 +45658,7 @@
       <c r="A5" s="52">
         <v>41</v>
       </c>
-      <c r="B5" s="245"/>
+      <c r="B5" s="244"/>
       <c r="C5" s="51" t="s">
         <v>1319</v>
       </c>
@@ -45620,18 +45846,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="234" t="s">
         <v>1323</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="253"/>
-      <c r="H1" s="238"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="250"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="237"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="237"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="249"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -45704,7 +45930,7 @@
         <v>1145</v>
       </c>
       <c r="J3" s="41"/>
-      <c r="K3" s="224" t="s">
+      <c r="K3" s="222" t="s">
         <v>94</v>
       </c>
       <c r="L3" s="39"/>
@@ -45784,7 +46010,7 @@
       <c r="J5" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="K5" s="225" t="s">
+      <c r="K5" s="223" t="s">
         <v>5</v>
       </c>
       <c r="L5" s="39" t="s">
@@ -45828,7 +46054,7 @@
       <c r="J6" s="39" t="s">
         <v>1328</v>
       </c>
-      <c r="K6" s="225" t="s">
+      <c r="K6" s="223" t="s">
         <v>474</v>
       </c>
       <c r="L6" s="39" t="s">
@@ -46328,15 +46554,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -46360,6 +46577,15 @@
     </RatedBy>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46570,14 +46796,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -46590,6 +46808,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>